<commit_message>
[FEATURE] set first tab as active sheet
abas-specificationsconfigurator-web#34
</commit_message>
<xml_diff>
--- a/resources/excel/specification_configurator_template.xlsx
+++ b/resources/excel/specification_configurator_template.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
-  <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2-Vertrieb\Marketing\Homepage\Lastenheftkonfigurator\Excel-Ausgabe\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\abas-specificationsconfigurator-api-web\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC99D77-FDE9-4021-B0DE-0D278973BFFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18876" windowHeight="7632" firstSheet="3" activeTab="5"/>
+    <workbookView xWindow="41550" yWindow="3315" windowWidth="32100" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Firmenprofil" sheetId="1" r:id="rId1"/>
@@ -28,10 +29,16 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'6. Anforderungen'!$A$1:$L$15</definedName>
     <definedName name="Bewertung">[1]Listen!$B$4:$B$9</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1667,7 +1674,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
   </numFmts>
@@ -2292,49 +2299,6 @@
     <xf numFmtId="9" fontId="18" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2350,11 +2314,54 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Standard 2" xfId="1"/>
-    <cellStyle name="Währung 2" xfId="2"/>
+    <cellStyle name="Standard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Währung 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2400,7 +2407,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="6" name="Grafik 5"/>
+        <xdr:cNvPr id="6" name="Grafik 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -2778,102 +2791,102 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="48.44140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="81.109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="68.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="47.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="11.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="111" t="s">
         <v>355</v>
       </c>
-      <c r="B1" s="106"/>
+      <c r="B1" s="111"/>
       <c r="C1" s="30"/>
     </row>
-    <row r="2" spans="1:5" ht="28.8" customHeight="1">
+    <row r="2" spans="1:5" ht="28.9" customHeight="1">
       <c r="A2" s="41" t="s">
         <v>356</v>
       </c>
       <c r="B2" s="41"/>
-      <c r="C2" s="105"/>
+      <c r="C2" s="110"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="42" t="s">
         <v>357</v>
       </c>
       <c r="B3" s="43"/>
-      <c r="C3" s="105"/>
+      <c r="C3" s="110"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="42" t="s">
         <v>358</v>
       </c>
       <c r="B4" s="43"/>
-      <c r="C4" s="105"/>
+      <c r="C4" s="110"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="42" t="s">
         <v>370</v>
       </c>
       <c r="B5" s="43"/>
-      <c r="C5" s="105"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1">
+      <c r="C5" s="110"/>
+    </row>
+    <row r="6" spans="1:5" ht="14.45" customHeight="1">
       <c r="A6" s="42" t="s">
         <v>359</v>
       </c>
       <c r="B6" s="43"/>
-      <c r="C6" s="105"/>
+      <c r="C6" s="110"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="42" t="s">
         <v>360</v>
       </c>
       <c r="B7" s="43"/>
-      <c r="C7" s="105"/>
+      <c r="C7" s="110"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="42" t="s">
         <v>371</v>
       </c>
       <c r="B8" s="43"/>
-      <c r="C8" s="105"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="C8" s="110"/>
+    </row>
+    <row r="9" spans="1:5" ht="22.5">
       <c r="A9" s="40" t="s">
         <v>372</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="105"/>
+      <c r="C9" s="110"/>
     </row>
     <row r="10" spans="1:5" ht="24" customHeight="1">
       <c r="A10" s="40" t="s">
         <v>373</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="105"/>
-    </row>
-    <row r="11" spans="1:5" ht="95.4" customHeight="1">
+      <c r="C10" s="110"/>
+    </row>
+    <row r="11" spans="1:5" ht="95.45" customHeight="1">
       <c r="A11" s="40"/>
       <c r="B11" s="8"/>
-      <c r="C11" s="105"/>
+      <c r="C11" s="110"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="13">
@@ -2888,10 +2901,10 @@
     </row>
     <row r="13" spans="1:5" ht="30.6" customHeight="1">
       <c r="A13" s="10"/>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="109" t="s">
         <v>374</v>
       </c>
-      <c r="C13" s="104"/>
+      <c r="C13" s="109"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="10"/>
@@ -2983,7 +2996,7 @@
       <c r="C24" s="7"/>
       <c r="E24" s="3"/>
     </row>
-    <row r="25" spans="1:5" ht="49.8" customHeight="1">
+    <row r="25" spans="1:5" ht="49.9" customHeight="1">
       <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>511</v>
@@ -3098,7 +3111,7 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C21">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"ja, nein"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3116,7 +3129,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:E75"/>
   <sheetViews>
@@ -3124,18 +3137,18 @@
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="68.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="47.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3151,10 +3164,10 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="10"/>
-      <c r="B2" s="104" t="s">
+      <c r="B2" s="109" t="s">
         <v>347</v>
       </c>
-      <c r="C2" s="104"/>
+      <c r="C2" s="109"/>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="18" t="s">
@@ -3420,12 +3433,12 @@
       </c>
       <c r="C33" s="20"/>
     </row>
-    <row r="34" spans="1:3" ht="41.4">
+    <row r="34" spans="1:3" ht="38.25">
       <c r="B34" s="6" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="41.4">
+    <row r="35" spans="1:3" ht="38.25">
       <c r="B35" s="6" t="s">
         <v>389</v>
       </c>
@@ -3438,7 +3451,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="27.6">
+    <row r="37" spans="1:3" ht="25.5">
       <c r="B37" s="6" t="s">
         <v>390</v>
       </c>
@@ -3727,7 +3740,7 @@
     <mergeCell ref="B2:C2"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C4:C8 C70">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C4:C8 C70" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>nicht relevant, außer Haus," außer Haus, Schnittstelle"," im Haus, manuell"," im Haus, systemgestützt"</x12ac:list>
@@ -3737,10 +3750,10 @@
         </mc:Fallback>
       </mc:AlternateContent>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C9:C13 C15:C25 C48:C50 C52:C57 C59:C65 C67:C68 C71 C73:C75">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C9:C13 C15:C25 C48:C50 C52:C57 C59:C65 C67:C68 C71 C73:C75" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"ja, nein"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C36">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C36" xr:uid="{00000000-0002-0000-0100-000002000000}">
       <formula1>"manuell, elektronisch"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3761,7 +3774,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:E88"/>
   <sheetViews>
@@ -3769,18 +3782,18 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="80.5546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="68.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="47.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3852,7 +3865,7 @@
       <c r="C8" s="7"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:5" ht="27.6">
+    <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="8"/>
       <c r="B9" s="5" t="s">
         <v>158</v>
@@ -4293,7 +4306,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C17 C19 C21 C23">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C17 C19 C21 C23" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"ja, nein"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4310,7 +4323,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:E238"/>
   <sheetViews>
@@ -4318,18 +4331,18 @@
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="85.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1"/>
-    <col min="5" max="5" width="68.88671875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" style="1"/>
-    <col min="8" max="8" width="47.5546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.44140625" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5546875" style="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="85.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1"/>
+    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="1"/>
+    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -6051,10 +6064,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C5 C11 C17 C23 C29 C35 C41 C47 C53 C59 C65 C71 C77 C83 C89 C95 C101 C107 C113 C119 C125 C131 C137 C143 C149 C155 C161 C167 C173 C179 C185 C191 C197 C203 C209 C215 C221 C227 C233">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C5 C11 C17 C23 C29 C35 C41 C47 C53 C59 C65 C71 C77 C83 C89 C95 C101 C107 C113 C119 C125 C131 C137 C143 C149 C155 C161 C167 C173 C179 C185 C191 C197 C203 C209 C215 C221 C227 C233" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"keine IT Lösung im Einsatz, nicht integrierte IT Lösung, Anbindung über Schnittstelle, Voll integriert, ERP Modul"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C8 C14 C20 C26 C32 C38 C44 C50 C56 C62 C68 C74 C80 C86 C92 C98 C104 C110 C116 C122 C128 C134 C140 C146 C152 C158 C164 C170 C176 C182 C188 C194 C200 C206 C212 C218 C224 C230 C236">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C8 C14 C20 C26 C32 C38 C44 C50 C56 C62 C68 C74 C80 C86 C92 C98 C104 C110 C116 C122 C128 C134 C140 C146 C152 C158 C164 C170 C176 C182 C188 C194 C200 C206 C212 C218 C224 C230 C236" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"ja, nein, offen"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6080,7 +6093,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:C240"/>
   <sheetViews>
@@ -6088,12 +6101,12 @@
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="56.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6107,7 +6120,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="27.6">
+    <row r="2" spans="1:3" ht="25.5">
       <c r="A2" s="10"/>
       <c r="B2" s="22" t="s">
         <v>367</v>
@@ -6123,7 +6136,7 @@
       </c>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:3" ht="41.4">
+    <row r="4" spans="1:3" ht="38.25">
       <c r="A4" s="39"/>
       <c r="B4" s="5" t="s">
         <v>254</v>
@@ -6132,7 +6145,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="27.6">
+    <row r="5" spans="1:3" ht="25.5">
       <c r="A5" s="39"/>
       <c r="B5" s="5" t="s">
         <v>255</v>
@@ -6141,7 +6154,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="27.6">
+    <row r="6" spans="1:3" ht="25.5">
       <c r="A6" s="39"/>
       <c r="B6" s="5" t="s">
         <v>256</v>
@@ -6150,7 +6163,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="27.6">
+    <row r="7" spans="1:3" ht="25.5">
       <c r="A7" s="15"/>
       <c r="B7" s="5" t="s">
         <v>257</v>
@@ -6159,7 +6172,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27.6">
+    <row r="8" spans="1:3" ht="25.5">
       <c r="A8" s="39"/>
       <c r="B8" s="5" t="s">
         <v>258</v>
@@ -6168,7 +6181,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="27.6">
+    <row r="9" spans="1:3" ht="25.5">
       <c r="A9" s="15"/>
       <c r="B9" s="5" t="s">
         <v>259</v>
@@ -6186,7 +6199,7 @@
       </c>
       <c r="C10" s="20"/>
     </row>
-    <row r="11" spans="1:3" ht="41.4">
+    <row r="11" spans="1:3" ht="25.5">
       <c r="A11" s="39"/>
       <c r="B11" s="5" t="s">
         <v>308</v>
@@ -6195,7 +6208,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="27.6">
+    <row r="12" spans="1:3" ht="25.5">
       <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>309</v>
@@ -6204,7 +6217,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="27.6">
+    <row r="13" spans="1:3" ht="25.5">
       <c r="A13" s="39"/>
       <c r="B13" s="5" t="s">
         <v>310</v>
@@ -6222,7 +6235,7 @@
       </c>
       <c r="C14" s="20"/>
     </row>
-    <row r="15" spans="1:3" ht="41.4">
+    <row r="15" spans="1:3" ht="38.25">
       <c r="A15" s="15"/>
       <c r="B15" s="5" t="s">
         <v>250</v>
@@ -6240,7 +6253,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="55.2">
+    <row r="17" spans="1:3" ht="51">
       <c r="A17" s="23"/>
       <c r="B17" s="5" t="s">
         <v>252</v>
@@ -6249,7 +6262,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="41.4">
+    <row r="18" spans="1:3" ht="38.25">
       <c r="A18" s="23"/>
       <c r="B18" s="5" t="s">
         <v>253</v>
@@ -6267,7 +6280,7 @@
       </c>
       <c r="C19" s="20"/>
     </row>
-    <row r="20" spans="1:3" ht="27.6">
+    <row r="20" spans="1:3" ht="25.5">
       <c r="A20" s="23"/>
       <c r="B20" s="5" t="s">
         <v>311</v>
@@ -6276,7 +6289,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="27.6">
+    <row r="21" spans="1:3" ht="25.5">
       <c r="A21" s="15"/>
       <c r="B21" s="5" t="s">
         <v>312</v>
@@ -6285,7 +6298,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="27.6">
+    <row r="22" spans="1:3" ht="25.5">
       <c r="A22" s="23"/>
       <c r="B22" s="5" t="s">
         <v>313</v>
@@ -6303,7 +6316,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="27.6">
+    <row r="24" spans="1:3" ht="25.5">
       <c r="A24" s="23"/>
       <c r="B24" s="5" t="s">
         <v>315</v>
@@ -6312,7 +6325,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="41.4">
+    <row r="25" spans="1:3" ht="38.25">
       <c r="A25" s="23"/>
       <c r="B25" s="5" t="s">
         <v>316</v>
@@ -6330,7 +6343,7 @@
       </c>
       <c r="C26" s="20"/>
     </row>
-    <row r="27" spans="1:3" ht="27.6">
+    <row r="27" spans="1:3" ht="25.5">
       <c r="A27" s="15"/>
       <c r="B27" s="5" t="s">
         <v>368</v>
@@ -7404,7 +7417,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C4:C9 C11:C13 C15:C18 C20:C25">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C4:C9 C11:C13 C15:C18 C20:C25" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <mc:AlternateContent xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
         <mc:Choice Requires="x12ac">
           <x12ac:list>1 = Findet keine Beachtung," 2 = Thema ist uns bewusst, wir haben uns darüber informiert", 3 = Konzepte sind entwickelt, 4 = Realisierungsphase, 5 = Ist bereits umgesetzt und dem KVP zugeführt</x12ac:list>
@@ -7428,26 +7441,26 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" style="59" customWidth="1"/>
-    <col min="2" max="2" width="32.44140625" style="59" customWidth="1"/>
-    <col min="3" max="5" width="8.6640625" style="59" customWidth="1"/>
-    <col min="6" max="11" width="5.33203125" style="59" customWidth="1"/>
-    <col min="12" max="12" width="45.109375" style="59" customWidth="1"/>
-    <col min="13" max="13" width="28.33203125" style="59" customWidth="1"/>
-    <col min="14" max="14" width="11.5546875" style="59"/>
-    <col min="15" max="15" width="47.5546875" style="59" customWidth="1"/>
-    <col min="16" max="16" width="34.44140625" style="59" customWidth="1"/>
-    <col min="17" max="16384" width="11.5546875" style="59"/>
+    <col min="1" max="1" width="4.7109375" style="59" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="59" customWidth="1"/>
+    <col min="3" max="5" width="8.7109375" style="59" customWidth="1"/>
+    <col min="6" max="11" width="5.28515625" style="59" customWidth="1"/>
+    <col min="12" max="12" width="45.140625" style="59" customWidth="1"/>
+    <col min="13" max="13" width="28.28515625" style="59" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" style="59"/>
+    <col min="15" max="15" width="47.5703125" style="59" customWidth="1"/>
+    <col min="16" max="16" width="34.42578125" style="59" customWidth="1"/>
+    <col min="17" max="16384" width="11.5703125" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -7457,38 +7470,38 @@
       <c r="B1" s="75" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="115" t="s">
+      <c r="C1" s="113" t="s">
         <v>345</v>
       </c>
-      <c r="D1" s="115"/>
-      <c r="E1" s="115"/>
-      <c r="F1" s="111" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="112" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="111"/>
-      <c r="H1" s="111"/>
-      <c r="I1" s="111"/>
-      <c r="J1" s="111"/>
-      <c r="K1" s="111"/>
-      <c r="L1" s="111"/>
-    </row>
-    <row r="2" spans="1:12" ht="37.799999999999997" customHeight="1">
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
+    </row>
+    <row r="2" spans="1:12" ht="37.9" customHeight="1">
       <c r="A2" s="76"/>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>512</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
-      <c r="E2" s="116"/>
-      <c r="F2" s="111" t="s">
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="112" t="s">
         <v>503</v>
       </c>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
     </row>
     <row r="3" spans="1:12" ht="24">
       <c r="A3" s="77" t="s">
@@ -7709,9 +7722,9 @@
       <c r="B15" s="99" t="s">
         <v>474</v>
       </c>
-      <c r="C15" s="118"/>
-      <c r="D15" s="118"/>
-      <c r="E15" s="118"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
       <c r="F15" s="93"/>
       <c r="G15" s="93"/>
       <c r="H15" s="93"/>
@@ -7722,10 +7735,10 @@
     </row>
     <row r="16" spans="1:12">
       <c r="A16" s="60"/>
-      <c r="B16" s="119"/>
-      <c r="C16" s="120"/>
-      <c r="D16" s="120"/>
-      <c r="E16" s="120"/>
+      <c r="B16" s="105"/>
+      <c r="C16" s="106"/>
+      <c r="D16" s="106"/>
+      <c r="E16" s="106"/>
       <c r="F16" s="93"/>
       <c r="G16" s="93"/>
       <c r="H16" s="93"/>
@@ -7931,9 +7944,9 @@
       <c r="B29" s="99" t="s">
         <v>475</v>
       </c>
-      <c r="C29" s="121"/>
-      <c r="D29" s="121"/>
-      <c r="E29" s="121"/>
+      <c r="C29" s="107"/>
+      <c r="D29" s="107"/>
+      <c r="E29" s="107"/>
       <c r="F29" s="93"/>
       <c r="G29" s="93"/>
       <c r="H29" s="93"/>
@@ -7944,10 +7957,10 @@
     </row>
     <row r="30" spans="1:12">
       <c r="A30" s="60"/>
-      <c r="B30" s="119"/>
-      <c r="C30" s="120"/>
-      <c r="D30" s="120"/>
-      <c r="E30" s="120"/>
+      <c r="B30" s="105"/>
+      <c r="C30" s="106"/>
+      <c r="D30" s="106"/>
+      <c r="E30" s="106"/>
       <c r="F30" s="93"/>
       <c r="G30" s="93"/>
       <c r="H30" s="93"/>
@@ -8052,14 +8065,14 @@
       <c r="K36" s="71"/>
       <c r="L36" s="86"/>
     </row>
-    <row r="37" spans="1:12" ht="22.2" customHeight="1">
+    <row r="37" spans="1:12" ht="22.15" customHeight="1">
       <c r="A37" s="61"/>
       <c r="B37" s="99" t="s">
         <v>476</v>
       </c>
-      <c r="C37" s="118"/>
-      <c r="D37" s="118"/>
-      <c r="E37" s="118"/>
+      <c r="C37" s="104"/>
+      <c r="D37" s="104"/>
+      <c r="E37" s="104"/>
       <c r="F37" s="93"/>
       <c r="G37" s="93"/>
       <c r="H37" s="93"/>
@@ -8070,10 +8083,10 @@
     </row>
     <row r="38" spans="1:12">
       <c r="A38" s="61"/>
-      <c r="B38" s="119"/>
-      <c r="C38" s="120"/>
-      <c r="D38" s="120"/>
-      <c r="E38" s="120"/>
+      <c r="B38" s="105"/>
+      <c r="C38" s="106"/>
+      <c r="D38" s="106"/>
+      <c r="E38" s="106"/>
       <c r="F38" s="93"/>
       <c r="G38" s="93"/>
       <c r="H38" s="93"/>
@@ -8226,7 +8239,7 @@
       <c r="K47" s="71"/>
       <c r="L47" s="86"/>
     </row>
-    <row r="48" spans="1:12" ht="27.6">
+    <row r="48" spans="1:12" ht="25.5">
       <c r="A48" s="60"/>
       <c r="B48" s="64" t="s">
         <v>47</v>
@@ -8242,14 +8255,14 @@
       <c r="K48" s="71"/>
       <c r="L48" s="86"/>
     </row>
-    <row r="49" spans="1:12" ht="23.4" customHeight="1">
+    <row r="49" spans="1:12" ht="23.45" customHeight="1">
       <c r="A49" s="61"/>
       <c r="B49" s="99" t="s">
         <v>477</v>
       </c>
-      <c r="C49" s="118"/>
-      <c r="D49" s="118"/>
-      <c r="E49" s="118"/>
+      <c r="C49" s="104"/>
+      <c r="D49" s="104"/>
+      <c r="E49" s="104"/>
       <c r="F49" s="93"/>
       <c r="G49" s="93"/>
       <c r="H49" s="93"/>
@@ -8260,10 +8273,10 @@
     </row>
     <row r="50" spans="1:12">
       <c r="A50" s="61"/>
-      <c r="B50" s="119"/>
-      <c r="C50" s="120"/>
-      <c r="D50" s="120"/>
-      <c r="E50" s="120"/>
+      <c r="B50" s="105"/>
+      <c r="C50" s="106"/>
+      <c r="D50" s="106"/>
+      <c r="E50" s="106"/>
       <c r="F50" s="93"/>
       <c r="G50" s="93"/>
       <c r="H50" s="93"/>
@@ -8400,7 +8413,7 @@
       <c r="K58" s="71"/>
       <c r="L58" s="86"/>
     </row>
-    <row r="59" spans="1:12" ht="22.8" customHeight="1">
+    <row r="59" spans="1:12" ht="22.9" customHeight="1">
       <c r="A59" s="61"/>
       <c r="B59" s="96" t="s">
         <v>478</v>
@@ -8417,10 +8430,10 @@
     </row>
     <row r="60" spans="1:12">
       <c r="A60" s="61"/>
-      <c r="B60" s="119"/>
-      <c r="C60" s="120"/>
-      <c r="D60" s="120"/>
-      <c r="E60" s="120"/>
+      <c r="B60" s="105"/>
+      <c r="C60" s="106"/>
+      <c r="D60" s="106"/>
+      <c r="E60" s="106"/>
       <c r="F60" s="93"/>
       <c r="G60" s="93"/>
       <c r="H60" s="93"/>
@@ -8717,14 +8730,14 @@
       <c r="K78" s="71"/>
       <c r="L78" s="86"/>
     </row>
-    <row r="79" spans="1:12" ht="23.4" customHeight="1">
+    <row r="79" spans="1:12" ht="23.45" customHeight="1">
       <c r="A79" s="61"/>
       <c r="B79" s="99" t="s">
         <v>479</v>
       </c>
-      <c r="C79" s="118"/>
-      <c r="D79" s="118"/>
-      <c r="E79" s="118"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="104"/>
+      <c r="E79" s="104"/>
       <c r="F79" s="94"/>
       <c r="G79" s="94"/>
       <c r="H79" s="94"/>
@@ -8735,10 +8748,10 @@
     </row>
     <row r="80" spans="1:12">
       <c r="A80" s="61"/>
-      <c r="B80" s="119"/>
-      <c r="C80" s="120"/>
-      <c r="D80" s="120"/>
-      <c r="E80" s="120"/>
+      <c r="B80" s="105"/>
+      <c r="C80" s="106"/>
+      <c r="D80" s="106"/>
+      <c r="E80" s="106"/>
       <c r="F80" s="94"/>
       <c r="G80" s="94"/>
       <c r="H80" s="94"/>
@@ -8795,7 +8808,7 @@
       <c r="K83" s="71"/>
       <c r="L83" s="86"/>
     </row>
-    <row r="84" spans="1:12" ht="27.6">
+    <row r="84" spans="1:12" ht="25.5">
       <c r="A84" s="61"/>
       <c r="B84" s="64" t="s">
         <v>75</v>
@@ -8827,14 +8840,14 @@
       <c r="K85" s="71"/>
       <c r="L85" s="86"/>
     </row>
-    <row r="86" spans="1:12" ht="13.8" customHeight="1">
+    <row r="86" spans="1:12" ht="13.9" customHeight="1">
       <c r="A86" s="61"/>
       <c r="B86" s="99" t="s">
         <v>480</v>
       </c>
-      <c r="C86" s="118"/>
-      <c r="D86" s="118"/>
-      <c r="E86" s="118"/>
+      <c r="C86" s="104"/>
+      <c r="D86" s="104"/>
+      <c r="E86" s="104"/>
       <c r="F86" s="93"/>
       <c r="G86" s="93"/>
       <c r="H86" s="93"/>
@@ -8845,10 +8858,10 @@
     </row>
     <row r="87" spans="1:12">
       <c r="A87" s="61"/>
-      <c r="B87" s="119"/>
-      <c r="C87" s="120"/>
-      <c r="D87" s="120"/>
-      <c r="E87" s="120"/>
+      <c r="B87" s="105"/>
+      <c r="C87" s="106"/>
+      <c r="D87" s="106"/>
+      <c r="E87" s="106"/>
       <c r="F87" s="93"/>
       <c r="G87" s="93"/>
       <c r="H87" s="93"/>
@@ -8926,9 +8939,9 @@
       <c r="B92" s="99" t="s">
         <v>481</v>
       </c>
-      <c r="C92" s="118"/>
-      <c r="D92" s="118"/>
-      <c r="E92" s="118"/>
+      <c r="C92" s="104"/>
+      <c r="D92" s="104"/>
+      <c r="E92" s="104"/>
       <c r="F92" s="93"/>
       <c r="G92" s="93"/>
       <c r="H92" s="93"/>
@@ -8939,10 +8952,10 @@
     </row>
     <row r="93" spans="1:12">
       <c r="A93" s="61"/>
-      <c r="B93" s="119"/>
-      <c r="C93" s="120"/>
-      <c r="D93" s="120"/>
-      <c r="E93" s="120"/>
+      <c r="B93" s="105"/>
+      <c r="C93" s="106"/>
+      <c r="D93" s="106"/>
+      <c r="E93" s="106"/>
       <c r="F93" s="93"/>
       <c r="G93" s="93"/>
       <c r="H93" s="93"/>
@@ -9116,9 +9129,9 @@
       <c r="B104" s="99" t="s">
         <v>483</v>
       </c>
-      <c r="C104" s="118"/>
-      <c r="D104" s="118"/>
-      <c r="E104" s="118"/>
+      <c r="C104" s="104"/>
+      <c r="D104" s="104"/>
+      <c r="E104" s="104"/>
       <c r="F104" s="93"/>
       <c r="G104" s="93"/>
       <c r="H104" s="93"/>
@@ -9129,10 +9142,10 @@
     </row>
     <row r="105" spans="1:12">
       <c r="A105" s="61"/>
-      <c r="B105" s="119"/>
-      <c r="C105" s="120"/>
-      <c r="D105" s="120"/>
-      <c r="E105" s="120"/>
+      <c r="B105" s="105"/>
+      <c r="C105" s="106"/>
+      <c r="D105" s="106"/>
+      <c r="E105" s="106"/>
       <c r="F105" s="93"/>
       <c r="G105" s="93"/>
       <c r="H105" s="93"/>
@@ -9205,14 +9218,14 @@
       <c r="K109" s="71"/>
       <c r="L109" s="86"/>
     </row>
-    <row r="110" spans="1:12" ht="23.4" customHeight="1">
+    <row r="110" spans="1:12" ht="23.45" customHeight="1">
       <c r="A110" s="61"/>
       <c r="B110" s="99" t="s">
         <v>484</v>
       </c>
-      <c r="C110" s="118"/>
-      <c r="D110" s="118"/>
-      <c r="E110" s="118"/>
+      <c r="C110" s="104"/>
+      <c r="D110" s="104"/>
+      <c r="E110" s="104"/>
       <c r="F110" s="93"/>
       <c r="G110" s="93"/>
       <c r="H110" s="93"/>
@@ -9363,14 +9376,14 @@
       <c r="K119" s="71"/>
       <c r="L119" s="86"/>
     </row>
-    <row r="120" spans="1:12" ht="22.2" customHeight="1">
+    <row r="120" spans="1:12" ht="22.15" customHeight="1">
       <c r="A120" s="61"/>
       <c r="B120" s="99" t="s">
         <v>485</v>
       </c>
-      <c r="C120" s="118"/>
-      <c r="D120" s="118"/>
-      <c r="E120" s="118"/>
+      <c r="C120" s="104"/>
+      <c r="D120" s="104"/>
+      <c r="E120" s="104"/>
       <c r="F120" s="93"/>
       <c r="G120" s="93"/>
       <c r="H120" s="93"/>
@@ -9381,10 +9394,10 @@
     </row>
     <row r="121" spans="1:12">
       <c r="A121" s="61"/>
-      <c r="B121" s="119"/>
-      <c r="C121" s="120"/>
-      <c r="D121" s="120"/>
-      <c r="E121" s="120"/>
+      <c r="B121" s="105"/>
+      <c r="C121" s="106"/>
+      <c r="D121" s="106"/>
+      <c r="E121" s="106"/>
       <c r="F121" s="93"/>
       <c r="G121" s="93"/>
       <c r="H121" s="93"/>
@@ -9414,9 +9427,9 @@
       <c r="B123" s="99" t="s">
         <v>486</v>
       </c>
-      <c r="C123" s="118"/>
-      <c r="D123" s="118"/>
-      <c r="E123" s="118"/>
+      <c r="C123" s="104"/>
+      <c r="D123" s="104"/>
+      <c r="E123" s="104"/>
       <c r="F123" s="93"/>
       <c r="G123" s="93"/>
       <c r="H123" s="93"/>
@@ -9427,10 +9440,10 @@
     </row>
     <row r="124" spans="1:12">
       <c r="A124" s="61"/>
-      <c r="B124" s="119"/>
-      <c r="C124" s="120"/>
-      <c r="D124" s="120"/>
-      <c r="E124" s="120"/>
+      <c r="B124" s="105"/>
+      <c r="C124" s="106"/>
+      <c r="D124" s="106"/>
+      <c r="E124" s="106"/>
       <c r="F124" s="93"/>
       <c r="G124" s="93"/>
       <c r="H124" s="93"/>
@@ -9455,14 +9468,14 @@
       <c r="K125" s="71"/>
       <c r="L125" s="86"/>
     </row>
-    <row r="126" spans="1:12" ht="23.4" customHeight="1">
+    <row r="126" spans="1:12" ht="23.45" customHeight="1">
       <c r="A126" s="61"/>
       <c r="B126" s="99" t="s">
         <v>487</v>
       </c>
-      <c r="C126" s="118"/>
-      <c r="D126" s="118"/>
-      <c r="E126" s="118"/>
+      <c r="C126" s="104"/>
+      <c r="D126" s="104"/>
+      <c r="E126" s="104"/>
       <c r="F126" s="93"/>
       <c r="G126" s="93"/>
       <c r="H126" s="93"/>
@@ -9473,10 +9486,10 @@
     </row>
     <row r="127" spans="1:12">
       <c r="A127" s="61"/>
-      <c r="B127" s="119"/>
-      <c r="C127" s="120"/>
-      <c r="D127" s="120"/>
-      <c r="E127" s="120"/>
+      <c r="B127" s="105"/>
+      <c r="C127" s="106"/>
+      <c r="D127" s="106"/>
+      <c r="E127" s="106"/>
       <c r="F127" s="93"/>
       <c r="G127" s="93"/>
       <c r="H127" s="93"/>
@@ -9501,7 +9514,7 @@
       <c r="K128" s="71"/>
       <c r="L128" s="86"/>
     </row>
-    <row r="129" spans="1:12" ht="27.6">
+    <row r="129" spans="1:12" ht="25.5">
       <c r="A129" s="61"/>
       <c r="B129" s="64" t="s">
         <v>105</v>
@@ -9549,14 +9562,14 @@
       <c r="K131" s="71"/>
       <c r="L131" s="86"/>
     </row>
-    <row r="132" spans="1:12" ht="22.8" customHeight="1">
+    <row r="132" spans="1:12" ht="22.9" customHeight="1">
       <c r="A132" s="61"/>
       <c r="B132" s="99" t="s">
         <v>488</v>
       </c>
-      <c r="C132" s="121"/>
-      <c r="D132" s="121"/>
-      <c r="E132" s="121"/>
+      <c r="C132" s="107"/>
+      <c r="D132" s="107"/>
+      <c r="E132" s="107"/>
       <c r="F132" s="93"/>
       <c r="G132" s="93"/>
       <c r="H132" s="93"/>
@@ -9567,10 +9580,10 @@
     </row>
     <row r="133" spans="1:12">
       <c r="A133" s="61"/>
-      <c r="B133" s="119"/>
-      <c r="C133" s="120"/>
-      <c r="D133" s="120"/>
-      <c r="E133" s="120"/>
+      <c r="B133" s="105"/>
+      <c r="C133" s="106"/>
+      <c r="D133" s="106"/>
+      <c r="E133" s="106"/>
       <c r="F133" s="93"/>
       <c r="G133" s="93"/>
       <c r="H133" s="93"/>
@@ -9659,14 +9672,14 @@
       <c r="K138" s="71"/>
       <c r="L138" s="86"/>
     </row>
-    <row r="139" spans="1:12" ht="25.8" customHeight="1">
+    <row r="139" spans="1:12" ht="25.9" customHeight="1">
       <c r="A139" s="61"/>
       <c r="B139" s="99" t="s">
         <v>489</v>
       </c>
-      <c r="C139" s="121"/>
-      <c r="D139" s="121"/>
-      <c r="E139" s="121"/>
+      <c r="C139" s="107"/>
+      <c r="D139" s="107"/>
+      <c r="E139" s="107"/>
       <c r="F139" s="93"/>
       <c r="G139" s="93"/>
       <c r="H139" s="93"/>
@@ -9677,10 +9690,10 @@
     </row>
     <row r="140" spans="1:12">
       <c r="A140" s="61"/>
-      <c r="B140" s="119"/>
-      <c r="C140" s="120"/>
-      <c r="D140" s="120"/>
-      <c r="E140" s="120"/>
+      <c r="B140" s="105"/>
+      <c r="C140" s="106"/>
+      <c r="D140" s="106"/>
+      <c r="E140" s="106"/>
       <c r="F140" s="93"/>
       <c r="G140" s="93"/>
       <c r="H140" s="93"/>
@@ -9705,7 +9718,7 @@
       <c r="K141" s="71"/>
       <c r="L141" s="86"/>
     </row>
-    <row r="142" spans="1:12" ht="22.8" customHeight="1">
+    <row r="142" spans="1:12" ht="22.9" customHeight="1">
       <c r="A142" s="61"/>
       <c r="B142" s="96" t="s">
         <v>490</v>
@@ -9723,10 +9736,10 @@
     </row>
     <row r="143" spans="1:12">
       <c r="A143" s="61"/>
-      <c r="B143" s="119"/>
-      <c r="C143" s="120"/>
-      <c r="D143" s="120"/>
-      <c r="E143" s="120"/>
+      <c r="B143" s="105"/>
+      <c r="C143" s="106"/>
+      <c r="D143" s="106"/>
+      <c r="E143" s="106"/>
       <c r="F143" s="95"/>
       <c r="G143" s="95"/>
       <c r="H143" s="95"/>
@@ -9815,7 +9828,7 @@
       <c r="K148" s="71"/>
       <c r="L148" s="86"/>
     </row>
-    <row r="149" spans="1:12" ht="14.4" customHeight="1">
+    <row r="149" spans="1:12" ht="14.45" customHeight="1">
       <c r="A149" s="61"/>
       <c r="B149" s="96" t="s">
         <v>491</v>
@@ -9832,10 +9845,10 @@
     </row>
     <row r="150" spans="1:12">
       <c r="A150" s="61"/>
-      <c r="B150" s="119"/>
-      <c r="C150" s="120"/>
-      <c r="D150" s="120"/>
-      <c r="E150" s="120"/>
+      <c r="B150" s="105"/>
+      <c r="C150" s="106"/>
+      <c r="D150" s="106"/>
+      <c r="E150" s="106"/>
       <c r="F150" s="95"/>
       <c r="G150" s="95"/>
       <c r="H150" s="95"/>
@@ -9844,7 +9857,7 @@
       <c r="K150" s="95"/>
       <c r="L150" s="87"/>
     </row>
-    <row r="151" spans="1:12" ht="27.6">
+    <row r="151" spans="1:12" ht="25.5">
       <c r="A151" s="61"/>
       <c r="B151" s="63" t="s">
         <v>114</v>
@@ -9860,7 +9873,7 @@
       <c r="K151" s="71"/>
       <c r="L151" s="86"/>
     </row>
-    <row r="152" spans="1:12" ht="22.2" customHeight="1">
+    <row r="152" spans="1:12" ht="22.15" customHeight="1">
       <c r="A152" s="60"/>
       <c r="B152" s="96" t="s">
         <v>492</v>
@@ -9877,10 +9890,10 @@
     </row>
     <row r="153" spans="1:12">
       <c r="A153" s="60"/>
-      <c r="B153" s="119"/>
-      <c r="C153" s="120"/>
-      <c r="D153" s="120"/>
-      <c r="E153" s="120"/>
+      <c r="B153" s="105"/>
+      <c r="C153" s="106"/>
+      <c r="D153" s="106"/>
+      <c r="E153" s="106"/>
       <c r="F153" s="93"/>
       <c r="G153" s="93"/>
       <c r="H153" s="93"/>
@@ -9889,7 +9902,7 @@
       <c r="K153" s="93"/>
       <c r="L153" s="87"/>
     </row>
-    <row r="154" spans="1:12" ht="27.6">
+    <row r="154" spans="1:12" ht="25.5">
       <c r="A154" s="61"/>
       <c r="B154" s="63" t="s">
         <v>115</v>
@@ -9922,7 +9935,7 @@
     </row>
     <row r="156" spans="1:12">
       <c r="A156" s="61"/>
-      <c r="B156" s="122"/>
+      <c r="B156" s="108"/>
       <c r="C156" s="84"/>
       <c r="D156" s="84"/>
       <c r="E156" s="84"/>
@@ -9935,18 +9948,18 @@
       <c r="L156" s="87"/>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" s="114"/>
-      <c r="B157" s="114"/>
-      <c r="C157" s="114"/>
-      <c r="D157" s="114"/>
-      <c r="E157" s="114"/>
-      <c r="F157" s="114"/>
-      <c r="G157" s="114"/>
-      <c r="H157" s="114"/>
-      <c r="I157" s="114"/>
-      <c r="J157" s="114"/>
-      <c r="K157" s="114"/>
-      <c r="L157" s="114"/>
+      <c r="A157" s="119"/>
+      <c r="B157" s="119"/>
+      <c r="C157" s="119"/>
+      <c r="D157" s="119"/>
+      <c r="E157" s="119"/>
+      <c r="F157" s="119"/>
+      <c r="G157" s="119"/>
+      <c r="H157" s="119"/>
+      <c r="I157" s="119"/>
+      <c r="J157" s="119"/>
+      <c r="K157" s="119"/>
+      <c r="L157" s="119"/>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="61"/>
@@ -9982,7 +9995,7 @@
       </c>
       <c r="L158" s="61"/>
     </row>
-    <row r="159" spans="1:12" ht="16.2" customHeight="1">
+    <row r="159" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A159" s="61"/>
       <c r="B159" s="32" t="s">
         <v>502</v>
@@ -10050,648 +10063,648 @@
       </c>
     </row>
     <row r="161" spans="1:12">
-      <c r="A161" s="113"/>
-      <c r="B161" s="113"/>
-      <c r="C161" s="113"/>
-      <c r="D161" s="113"/>
-      <c r="E161" s="113"/>
-      <c r="F161" s="113"/>
-      <c r="G161" s="113"/>
-      <c r="H161" s="113"/>
-      <c r="I161" s="113"/>
-      <c r="J161" s="113"/>
-      <c r="K161" s="113"/>
-      <c r="L161" s="113"/>
-    </row>
-    <row r="162" spans="1:12" ht="16.2" customHeight="1">
+      <c r="A161" s="118"/>
+      <c r="B161" s="118"/>
+      <c r="C161" s="118"/>
+      <c r="D161" s="118"/>
+      <c r="E161" s="118"/>
+      <c r="F161" s="118"/>
+      <c r="G161" s="118"/>
+      <c r="H161" s="118"/>
+      <c r="I161" s="118"/>
+      <c r="J161" s="118"/>
+      <c r="K161" s="118"/>
+      <c r="L161" s="118"/>
+    </row>
+    <row r="162" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A162" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="B162" s="117" t="s">
+      <c r="B162" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="C162" s="117"/>
-      <c r="D162" s="117"/>
-      <c r="E162" s="117"/>
-      <c r="F162" s="117"/>
-      <c r="G162" s="117"/>
-      <c r="H162" s="117"/>
-      <c r="I162" s="117"/>
-      <c r="J162" s="117"/>
-      <c r="K162" s="117"/>
-      <c r="L162" s="117"/>
+      <c r="C162" s="116"/>
+      <c r="D162" s="116"/>
+      <c r="E162" s="116"/>
+      <c r="F162" s="116"/>
+      <c r="G162" s="116"/>
+      <c r="H162" s="116"/>
+      <c r="I162" s="116"/>
+      <c r="J162" s="116"/>
+      <c r="K162" s="116"/>
+      <c r="L162" s="116"/>
     </row>
     <row r="163" spans="1:12" ht="33" customHeight="1">
-      <c r="A163" s="112"/>
-      <c r="B163" s="112"/>
-      <c r="C163" s="112"/>
-      <c r="D163" s="112"/>
-      <c r="E163" s="112"/>
-      <c r="F163" s="111" t="s">
+      <c r="A163" s="117"/>
+      <c r="B163" s="117"/>
+      <c r="C163" s="117"/>
+      <c r="D163" s="117"/>
+      <c r="E163" s="117"/>
+      <c r="F163" s="112" t="s">
         <v>501</v>
       </c>
-      <c r="G163" s="111"/>
-      <c r="H163" s="111"/>
-      <c r="I163" s="111"/>
-      <c r="J163" s="111"/>
-      <c r="K163" s="111"/>
-      <c r="L163" s="111"/>
+      <c r="G163" s="112"/>
+      <c r="H163" s="112"/>
+      <c r="I163" s="112"/>
+      <c r="J163" s="112"/>
+      <c r="K163" s="112"/>
+      <c r="L163" s="112"/>
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="61"/>
       <c r="B164" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="C164" s="107"/>
-      <c r="D164" s="107"/>
-      <c r="E164" s="107"/>
-      <c r="F164" s="109"/>
-      <c r="G164" s="109"/>
-      <c r="H164" s="109"/>
-      <c r="I164" s="109"/>
-      <c r="J164" s="109"/>
-      <c r="K164" s="109"/>
-      <c r="L164" s="109"/>
-    </row>
-    <row r="165" spans="1:12" ht="27.6">
+      <c r="C164" s="114"/>
+      <c r="D164" s="114"/>
+      <c r="E164" s="114"/>
+      <c r="F164" s="121"/>
+      <c r="G164" s="121"/>
+      <c r="H164" s="121"/>
+      <c r="I164" s="121"/>
+      <c r="J164" s="121"/>
+      <c r="K164" s="121"/>
+      <c r="L164" s="121"/>
+    </row>
+    <row r="165" spans="1:12" ht="25.5">
       <c r="A165" s="61"/>
       <c r="B165" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C165" s="107"/>
-      <c r="D165" s="107"/>
-      <c r="E165" s="107"/>
-      <c r="F165" s="109"/>
-      <c r="G165" s="109"/>
-      <c r="H165" s="109"/>
-      <c r="I165" s="109"/>
-      <c r="J165" s="109"/>
-      <c r="K165" s="109"/>
-      <c r="L165" s="109"/>
-    </row>
-    <row r="166" spans="1:12" ht="27.6">
+      <c r="C165" s="114"/>
+      <c r="D165" s="114"/>
+      <c r="E165" s="114"/>
+      <c r="F165" s="121"/>
+      <c r="G165" s="121"/>
+      <c r="H165" s="121"/>
+      <c r="I165" s="121"/>
+      <c r="J165" s="121"/>
+      <c r="K165" s="121"/>
+      <c r="L165" s="121"/>
+    </row>
+    <row r="166" spans="1:12" ht="25.5">
       <c r="A166" s="60"/>
       <c r="B166" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C166" s="107"/>
-      <c r="D166" s="107"/>
-      <c r="E166" s="107"/>
-      <c r="F166" s="109"/>
-      <c r="G166" s="109"/>
-      <c r="H166" s="109"/>
-      <c r="I166" s="109"/>
-      <c r="J166" s="109"/>
-      <c r="K166" s="109"/>
-      <c r="L166" s="109"/>
-    </row>
-    <row r="167" spans="1:12" ht="14.4" customHeight="1">
+      <c r="C166" s="114"/>
+      <c r="D166" s="114"/>
+      <c r="E166" s="114"/>
+      <c r="F166" s="121"/>
+      <c r="G166" s="121"/>
+      <c r="H166" s="121"/>
+      <c r="I166" s="121"/>
+      <c r="J166" s="121"/>
+      <c r="K166" s="121"/>
+      <c r="L166" s="121"/>
+    </row>
+    <row r="167" spans="1:12" ht="14.45" customHeight="1">
       <c r="A167" s="61"/>
       <c r="B167" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="C167" s="110" t="s">
-        <v>510</v>
-      </c>
-      <c r="D167" s="110"/>
-      <c r="E167" s="110"/>
-      <c r="F167" s="109"/>
-      <c r="G167" s="109"/>
-      <c r="H167" s="109"/>
-      <c r="I167" s="109"/>
-      <c r="J167" s="109"/>
-      <c r="K167" s="109"/>
-      <c r="L167" s="109"/>
+      <c r="C167" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D167" s="120"/>
+      <c r="E167" s="120"/>
+      <c r="F167" s="121"/>
+      <c r="G167" s="121"/>
+      <c r="H167" s="121"/>
+      <c r="I167" s="121"/>
+      <c r="J167" s="121"/>
+      <c r="K167" s="121"/>
+      <c r="L167" s="121"/>
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="61"/>
       <c r="B168" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="C168" s="107"/>
-      <c r="D168" s="107"/>
-      <c r="E168" s="107"/>
-      <c r="F168" s="109"/>
-      <c r="G168" s="109"/>
-      <c r="H168" s="109"/>
-      <c r="I168" s="109"/>
-      <c r="J168" s="109"/>
-      <c r="K168" s="109"/>
-      <c r="L168" s="109"/>
-    </row>
-    <row r="169" spans="1:12" ht="27.6">
+      <c r="C168" s="114"/>
+      <c r="D168" s="114"/>
+      <c r="E168" s="114"/>
+      <c r="F168" s="121"/>
+      <c r="G168" s="121"/>
+      <c r="H168" s="121"/>
+      <c r="I168" s="121"/>
+      <c r="J168" s="121"/>
+      <c r="K168" s="121"/>
+      <c r="L168" s="121"/>
+    </row>
+    <row r="169" spans="1:12" ht="25.5">
       <c r="A169" s="61"/>
       <c r="B169" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C169" s="110" t="s">
-        <v>510</v>
-      </c>
-      <c r="D169" s="110"/>
-      <c r="E169" s="110"/>
-      <c r="F169" s="109"/>
-      <c r="G169" s="109"/>
-      <c r="H169" s="109"/>
-      <c r="I169" s="109"/>
-      <c r="J169" s="109"/>
-      <c r="K169" s="109"/>
-      <c r="L169" s="109"/>
-    </row>
-    <row r="170" spans="1:12" ht="27.6">
+      <c r="C169" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D169" s="120"/>
+      <c r="E169" s="120"/>
+      <c r="F169" s="121"/>
+      <c r="G169" s="121"/>
+      <c r="H169" s="121"/>
+      <c r="I169" s="121"/>
+      <c r="J169" s="121"/>
+      <c r="K169" s="121"/>
+      <c r="L169" s="121"/>
+    </row>
+    <row r="170" spans="1:12" ht="25.5">
       <c r="A170" s="61"/>
       <c r="B170" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C170" s="110" t="s">
-        <v>510</v>
-      </c>
-      <c r="D170" s="110"/>
-      <c r="E170" s="110"/>
-      <c r="F170" s="109"/>
-      <c r="G170" s="109"/>
-      <c r="H170" s="109"/>
-      <c r="I170" s="109"/>
-      <c r="J170" s="109"/>
-      <c r="K170" s="109"/>
-      <c r="L170" s="109"/>
-    </row>
-    <row r="171" spans="1:12" ht="27.6">
+      <c r="C170" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D170" s="120"/>
+      <c r="E170" s="120"/>
+      <c r="F170" s="121"/>
+      <c r="G170" s="121"/>
+      <c r="H170" s="121"/>
+      <c r="I170" s="121"/>
+      <c r="J170" s="121"/>
+      <c r="K170" s="121"/>
+      <c r="L170" s="121"/>
+    </row>
+    <row r="171" spans="1:12" ht="25.5">
       <c r="A171" s="61"/>
       <c r="B171" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C171" s="107"/>
-      <c r="D171" s="107"/>
-      <c r="E171" s="107"/>
-      <c r="F171" s="109"/>
-      <c r="G171" s="109"/>
-      <c r="H171" s="109"/>
-      <c r="I171" s="109"/>
-      <c r="J171" s="109"/>
-      <c r="K171" s="109"/>
-      <c r="L171" s="109"/>
+      <c r="C171" s="114"/>
+      <c r="D171" s="114"/>
+      <c r="E171" s="114"/>
+      <c r="F171" s="121"/>
+      <c r="G171" s="121"/>
+      <c r="H171" s="121"/>
+      <c r="I171" s="121"/>
+      <c r="J171" s="121"/>
+      <c r="K171" s="121"/>
+      <c r="L171" s="121"/>
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="60"/>
       <c r="B172" s="16"/>
-      <c r="C172" s="107"/>
-      <c r="D172" s="107"/>
-      <c r="E172" s="107"/>
-      <c r="F172" s="108"/>
-      <c r="G172" s="108"/>
-      <c r="H172" s="108"/>
-      <c r="I172" s="108"/>
-      <c r="J172" s="108"/>
-      <c r="K172" s="108"/>
-      <c r="L172" s="108"/>
+      <c r="C172" s="114"/>
+      <c r="D172" s="114"/>
+      <c r="E172" s="114"/>
+      <c r="F172" s="122"/>
+      <c r="G172" s="122"/>
+      <c r="H172" s="122"/>
+      <c r="I172" s="122"/>
+      <c r="J172" s="122"/>
+      <c r="K172" s="122"/>
+      <c r="L172" s="122"/>
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="61"/>
       <c r="B173" s="5"/>
-      <c r="C173" s="107"/>
-      <c r="D173" s="107"/>
-      <c r="E173" s="107"/>
-      <c r="F173" s="108"/>
-      <c r="G173" s="108"/>
-      <c r="H173" s="108"/>
-      <c r="I173" s="108"/>
-      <c r="J173" s="108"/>
-      <c r="K173" s="108"/>
-      <c r="L173" s="108"/>
+      <c r="C173" s="114"/>
+      <c r="D173" s="114"/>
+      <c r="E173" s="114"/>
+      <c r="F173" s="122"/>
+      <c r="G173" s="122"/>
+      <c r="H173" s="122"/>
+      <c r="I173" s="122"/>
+      <c r="J173" s="122"/>
+      <c r="K173" s="122"/>
+      <c r="L173" s="122"/>
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="61"/>
       <c r="B174" s="5"/>
-      <c r="C174" s="107"/>
-      <c r="D174" s="107"/>
-      <c r="E174" s="107"/>
-      <c r="F174" s="108"/>
-      <c r="G174" s="108"/>
-      <c r="H174" s="108"/>
-      <c r="I174" s="108"/>
-      <c r="J174" s="108"/>
-      <c r="K174" s="108"/>
-      <c r="L174" s="108"/>
+      <c r="C174" s="114"/>
+      <c r="D174" s="114"/>
+      <c r="E174" s="114"/>
+      <c r="F174" s="122"/>
+      <c r="G174" s="122"/>
+      <c r="H174" s="122"/>
+      <c r="I174" s="122"/>
+      <c r="J174" s="122"/>
+      <c r="K174" s="122"/>
+      <c r="L174" s="122"/>
     </row>
     <row r="175" spans="1:12">
       <c r="A175" s="61"/>
       <c r="B175" s="5"/>
-      <c r="C175" s="107"/>
-      <c r="D175" s="107"/>
-      <c r="E175" s="107"/>
-      <c r="F175" s="108"/>
-      <c r="G175" s="108"/>
-      <c r="H175" s="108"/>
-      <c r="I175" s="108"/>
-      <c r="J175" s="108"/>
-      <c r="K175" s="108"/>
-      <c r="L175" s="108"/>
+      <c r="C175" s="114"/>
+      <c r="D175" s="114"/>
+      <c r="E175" s="114"/>
+      <c r="F175" s="122"/>
+      <c r="G175" s="122"/>
+      <c r="H175" s="122"/>
+      <c r="I175" s="122"/>
+      <c r="J175" s="122"/>
+      <c r="K175" s="122"/>
+      <c r="L175" s="122"/>
     </row>
     <row r="176" spans="1:12">
       <c r="A176" s="61"/>
       <c r="B176" s="5"/>
-      <c r="C176" s="107"/>
-      <c r="D176" s="107"/>
-      <c r="E176" s="107"/>
-      <c r="F176" s="108"/>
-      <c r="G176" s="108"/>
-      <c r="H176" s="108"/>
-      <c r="I176" s="108"/>
-      <c r="J176" s="108"/>
-      <c r="K176" s="108"/>
-      <c r="L176" s="108"/>
+      <c r="C176" s="114"/>
+      <c r="D176" s="114"/>
+      <c r="E176" s="114"/>
+      <c r="F176" s="122"/>
+      <c r="G176" s="122"/>
+      <c r="H176" s="122"/>
+      <c r="I176" s="122"/>
+      <c r="J176" s="122"/>
+      <c r="K176" s="122"/>
+      <c r="L176" s="122"/>
     </row>
     <row r="177" spans="1:12">
       <c r="A177" s="61"/>
       <c r="B177" s="5"/>
-      <c r="C177" s="107"/>
-      <c r="D177" s="107"/>
-      <c r="E177" s="107"/>
-      <c r="F177" s="108"/>
-      <c r="G177" s="108"/>
-      <c r="H177" s="108"/>
-      <c r="I177" s="108"/>
-      <c r="J177" s="108"/>
-      <c r="K177" s="108"/>
-      <c r="L177" s="108"/>
+      <c r="C177" s="114"/>
+      <c r="D177" s="114"/>
+      <c r="E177" s="114"/>
+      <c r="F177" s="122"/>
+      <c r="G177" s="122"/>
+      <c r="H177" s="122"/>
+      <c r="I177" s="122"/>
+      <c r="J177" s="122"/>
+      <c r="K177" s="122"/>
+      <c r="L177" s="122"/>
     </row>
     <row r="178" spans="1:12">
       <c r="A178" s="60"/>
       <c r="B178" s="16"/>
-      <c r="C178" s="107"/>
-      <c r="D178" s="107"/>
-      <c r="E178" s="107"/>
-      <c r="F178" s="108"/>
-      <c r="G178" s="108"/>
-      <c r="H178" s="108"/>
-      <c r="I178" s="108"/>
-      <c r="J178" s="108"/>
-      <c r="K178" s="108"/>
-      <c r="L178" s="108"/>
+      <c r="C178" s="114"/>
+      <c r="D178" s="114"/>
+      <c r="E178" s="114"/>
+      <c r="F178" s="122"/>
+      <c r="G178" s="122"/>
+      <c r="H178" s="122"/>
+      <c r="I178" s="122"/>
+      <c r="J178" s="122"/>
+      <c r="K178" s="122"/>
+      <c r="L178" s="122"/>
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="61"/>
       <c r="B179" s="5"/>
-      <c r="C179" s="107"/>
-      <c r="D179" s="107"/>
-      <c r="E179" s="107"/>
-      <c r="F179" s="108"/>
-      <c r="G179" s="108"/>
-      <c r="H179" s="108"/>
-      <c r="I179" s="108"/>
-      <c r="J179" s="108"/>
-      <c r="K179" s="108"/>
-      <c r="L179" s="108"/>
+      <c r="C179" s="114"/>
+      <c r="D179" s="114"/>
+      <c r="E179" s="114"/>
+      <c r="F179" s="122"/>
+      <c r="G179" s="122"/>
+      <c r="H179" s="122"/>
+      <c r="I179" s="122"/>
+      <c r="J179" s="122"/>
+      <c r="K179" s="122"/>
+      <c r="L179" s="122"/>
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="61"/>
       <c r="B180" s="5"/>
-      <c r="C180" s="107"/>
-      <c r="D180" s="107"/>
-      <c r="E180" s="107"/>
-      <c r="F180" s="108"/>
-      <c r="G180" s="108"/>
-      <c r="H180" s="108"/>
-      <c r="I180" s="108"/>
-      <c r="J180" s="108"/>
-      <c r="K180" s="108"/>
-      <c r="L180" s="108"/>
+      <c r="C180" s="114"/>
+      <c r="D180" s="114"/>
+      <c r="E180" s="114"/>
+      <c r="F180" s="122"/>
+      <c r="G180" s="122"/>
+      <c r="H180" s="122"/>
+      <c r="I180" s="122"/>
+      <c r="J180" s="122"/>
+      <c r="K180" s="122"/>
+      <c r="L180" s="122"/>
     </row>
     <row r="181" spans="1:12">
       <c r="A181" s="61"/>
       <c r="B181" s="5"/>
-      <c r="C181" s="107"/>
-      <c r="D181" s="107"/>
-      <c r="E181" s="107"/>
-      <c r="F181" s="108"/>
-      <c r="G181" s="108"/>
-      <c r="H181" s="108"/>
-      <c r="I181" s="108"/>
-      <c r="J181" s="108"/>
-      <c r="K181" s="108"/>
-      <c r="L181" s="108"/>
+      <c r="C181" s="114"/>
+      <c r="D181" s="114"/>
+      <c r="E181" s="114"/>
+      <c r="F181" s="122"/>
+      <c r="G181" s="122"/>
+      <c r="H181" s="122"/>
+      <c r="I181" s="122"/>
+      <c r="J181" s="122"/>
+      <c r="K181" s="122"/>
+      <c r="L181" s="122"/>
     </row>
     <row r="182" spans="1:12">
       <c r="A182" s="61"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="107"/>
-      <c r="D182" s="107"/>
-      <c r="E182" s="107"/>
-      <c r="F182" s="108"/>
-      <c r="G182" s="108"/>
-      <c r="H182" s="108"/>
-      <c r="I182" s="108"/>
-      <c r="J182" s="108"/>
-      <c r="K182" s="108"/>
-      <c r="L182" s="108"/>
+      <c r="C182" s="114"/>
+      <c r="D182" s="114"/>
+      <c r="E182" s="114"/>
+      <c r="F182" s="122"/>
+      <c r="G182" s="122"/>
+      <c r="H182" s="122"/>
+      <c r="I182" s="122"/>
+      <c r="J182" s="122"/>
+      <c r="K182" s="122"/>
+      <c r="L182" s="122"/>
     </row>
     <row r="183" spans="1:12">
       <c r="A183" s="61"/>
       <c r="B183" s="5"/>
-      <c r="C183" s="107"/>
-      <c r="D183" s="107"/>
-      <c r="E183" s="107"/>
-      <c r="F183" s="108"/>
-      <c r="G183" s="108"/>
-      <c r="H183" s="108"/>
-      <c r="I183" s="108"/>
-      <c r="J183" s="108"/>
-      <c r="K183" s="108"/>
-      <c r="L183" s="108"/>
+      <c r="C183" s="114"/>
+      <c r="D183" s="114"/>
+      <c r="E183" s="114"/>
+      <c r="F183" s="122"/>
+      <c r="G183" s="122"/>
+      <c r="H183" s="122"/>
+      <c r="I183" s="122"/>
+      <c r="J183" s="122"/>
+      <c r="K183" s="122"/>
+      <c r="L183" s="122"/>
     </row>
     <row r="184" spans="1:12">
       <c r="A184" s="60"/>
       <c r="B184" s="16"/>
-      <c r="C184" s="107"/>
-      <c r="D184" s="107"/>
-      <c r="E184" s="107"/>
-      <c r="F184" s="108"/>
-      <c r="G184" s="108"/>
-      <c r="H184" s="108"/>
-      <c r="I184" s="108"/>
-      <c r="J184" s="108"/>
-      <c r="K184" s="108"/>
-      <c r="L184" s="108"/>
+      <c r="C184" s="114"/>
+      <c r="D184" s="114"/>
+      <c r="E184" s="114"/>
+      <c r="F184" s="122"/>
+      <c r="G184" s="122"/>
+      <c r="H184" s="122"/>
+      <c r="I184" s="122"/>
+      <c r="J184" s="122"/>
+      <c r="K184" s="122"/>
+      <c r="L184" s="122"/>
     </row>
     <row r="185" spans="1:12">
       <c r="A185" s="61"/>
       <c r="B185" s="5"/>
-      <c r="C185" s="107"/>
-      <c r="D185" s="107"/>
-      <c r="E185" s="107"/>
-      <c r="F185" s="108"/>
-      <c r="G185" s="108"/>
-      <c r="H185" s="108"/>
-      <c r="I185" s="108"/>
-      <c r="J185" s="108"/>
-      <c r="K185" s="108"/>
-      <c r="L185" s="108"/>
+      <c r="C185" s="114"/>
+      <c r="D185" s="114"/>
+      <c r="E185" s="114"/>
+      <c r="F185" s="122"/>
+      <c r="G185" s="122"/>
+      <c r="H185" s="122"/>
+      <c r="I185" s="122"/>
+      <c r="J185" s="122"/>
+      <c r="K185" s="122"/>
+      <c r="L185" s="122"/>
     </row>
     <row r="186" spans="1:12">
       <c r="A186" s="61"/>
       <c r="B186" s="5"/>
-      <c r="C186" s="107"/>
-      <c r="D186" s="107"/>
-      <c r="E186" s="107"/>
-      <c r="F186" s="108"/>
-      <c r="G186" s="108"/>
-      <c r="H186" s="108"/>
-      <c r="I186" s="108"/>
-      <c r="J186" s="108"/>
-      <c r="K186" s="108"/>
-      <c r="L186" s="108"/>
+      <c r="C186" s="114"/>
+      <c r="D186" s="114"/>
+      <c r="E186" s="114"/>
+      <c r="F186" s="122"/>
+      <c r="G186" s="122"/>
+      <c r="H186" s="122"/>
+      <c r="I186" s="122"/>
+      <c r="J186" s="122"/>
+      <c r="K186" s="122"/>
+      <c r="L186" s="122"/>
     </row>
     <row r="187" spans="1:12">
       <c r="A187" s="61"/>
       <c r="B187" s="5"/>
-      <c r="C187" s="107"/>
-      <c r="D187" s="107"/>
-      <c r="E187" s="107"/>
-      <c r="F187" s="108"/>
-      <c r="G187" s="108"/>
-      <c r="H187" s="108"/>
-      <c r="I187" s="108"/>
-      <c r="J187" s="108"/>
-      <c r="K187" s="108"/>
-      <c r="L187" s="108"/>
+      <c r="C187" s="114"/>
+      <c r="D187" s="114"/>
+      <c r="E187" s="114"/>
+      <c r="F187" s="122"/>
+      <c r="G187" s="122"/>
+      <c r="H187" s="122"/>
+      <c r="I187" s="122"/>
+      <c r="J187" s="122"/>
+      <c r="K187" s="122"/>
+      <c r="L187" s="122"/>
     </row>
     <row r="188" spans="1:12">
       <c r="A188" s="61"/>
       <c r="B188" s="5"/>
-      <c r="C188" s="107"/>
-      <c r="D188" s="107"/>
-      <c r="E188" s="107"/>
-      <c r="F188" s="108"/>
-      <c r="G188" s="108"/>
-      <c r="H188" s="108"/>
-      <c r="I188" s="108"/>
-      <c r="J188" s="108"/>
-      <c r="K188" s="108"/>
-      <c r="L188" s="108"/>
+      <c r="C188" s="114"/>
+      <c r="D188" s="114"/>
+      <c r="E188" s="114"/>
+      <c r="F188" s="122"/>
+      <c r="G188" s="122"/>
+      <c r="H188" s="122"/>
+      <c r="I188" s="122"/>
+      <c r="J188" s="122"/>
+      <c r="K188" s="122"/>
+      <c r="L188" s="122"/>
     </row>
     <row r="189" spans="1:12">
       <c r="A189" s="61"/>
       <c r="B189" s="5"/>
-      <c r="C189" s="107"/>
-      <c r="D189" s="107"/>
-      <c r="E189" s="107"/>
-      <c r="F189" s="108"/>
-      <c r="G189" s="108"/>
-      <c r="H189" s="108"/>
-      <c r="I189" s="108"/>
-      <c r="J189" s="108"/>
-      <c r="K189" s="108"/>
-      <c r="L189" s="108"/>
+      <c r="C189" s="114"/>
+      <c r="D189" s="114"/>
+      <c r="E189" s="114"/>
+      <c r="F189" s="122"/>
+      <c r="G189" s="122"/>
+      <c r="H189" s="122"/>
+      <c r="I189" s="122"/>
+      <c r="J189" s="122"/>
+      <c r="K189" s="122"/>
+      <c r="L189" s="122"/>
     </row>
     <row r="190" spans="1:12">
       <c r="A190" s="60"/>
       <c r="B190" s="16"/>
-      <c r="C190" s="107"/>
-      <c r="D190" s="107"/>
-      <c r="E190" s="107"/>
-      <c r="F190" s="108"/>
-      <c r="G190" s="108"/>
-      <c r="H190" s="108"/>
-      <c r="I190" s="108"/>
-      <c r="J190" s="108"/>
-      <c r="K190" s="108"/>
-      <c r="L190" s="108"/>
+      <c r="C190" s="114"/>
+      <c r="D190" s="114"/>
+      <c r="E190" s="114"/>
+      <c r="F190" s="122"/>
+      <c r="G190" s="122"/>
+      <c r="H190" s="122"/>
+      <c r="I190" s="122"/>
+      <c r="J190" s="122"/>
+      <c r="K190" s="122"/>
+      <c r="L190" s="122"/>
     </row>
     <row r="191" spans="1:12">
       <c r="A191" s="61"/>
       <c r="B191" s="5"/>
-      <c r="C191" s="107"/>
-      <c r="D191" s="107"/>
-      <c r="E191" s="107"/>
-      <c r="F191" s="108"/>
-      <c r="G191" s="108"/>
-      <c r="H191" s="108"/>
-      <c r="I191" s="108"/>
-      <c r="J191" s="108"/>
-      <c r="K191" s="108"/>
-      <c r="L191" s="108"/>
+      <c r="C191" s="114"/>
+      <c r="D191" s="114"/>
+      <c r="E191" s="114"/>
+      <c r="F191" s="122"/>
+      <c r="G191" s="122"/>
+      <c r="H191" s="122"/>
+      <c r="I191" s="122"/>
+      <c r="J191" s="122"/>
+      <c r="K191" s="122"/>
+      <c r="L191" s="122"/>
     </row>
     <row r="192" spans="1:12">
       <c r="A192" s="61"/>
       <c r="B192" s="5"/>
-      <c r="C192" s="107"/>
-      <c r="D192" s="107"/>
-      <c r="E192" s="107"/>
-      <c r="F192" s="108"/>
-      <c r="G192" s="108"/>
-      <c r="H192" s="108"/>
-      <c r="I192" s="108"/>
-      <c r="J192" s="108"/>
-      <c r="K192" s="108"/>
-      <c r="L192" s="108"/>
+      <c r="C192" s="114"/>
+      <c r="D192" s="114"/>
+      <c r="E192" s="114"/>
+      <c r="F192" s="122"/>
+      <c r="G192" s="122"/>
+      <c r="H192" s="122"/>
+      <c r="I192" s="122"/>
+      <c r="J192" s="122"/>
+      <c r="K192" s="122"/>
+      <c r="L192" s="122"/>
     </row>
     <row r="193" spans="1:12">
       <c r="A193" s="61"/>
       <c r="B193" s="5"/>
-      <c r="C193" s="107"/>
-      <c r="D193" s="107"/>
-      <c r="E193" s="107"/>
-      <c r="F193" s="108"/>
-      <c r="G193" s="108"/>
-      <c r="H193" s="108"/>
-      <c r="I193" s="108"/>
-      <c r="J193" s="108"/>
-      <c r="K193" s="108"/>
-      <c r="L193" s="108"/>
+      <c r="C193" s="114"/>
+      <c r="D193" s="114"/>
+      <c r="E193" s="114"/>
+      <c r="F193" s="122"/>
+      <c r="G193" s="122"/>
+      <c r="H193" s="122"/>
+      <c r="I193" s="122"/>
+      <c r="J193" s="122"/>
+      <c r="K193" s="122"/>
+      <c r="L193" s="122"/>
     </row>
     <row r="194" spans="1:12">
       <c r="A194" s="61"/>
       <c r="B194" s="5"/>
-      <c r="C194" s="107"/>
-      <c r="D194" s="107"/>
-      <c r="E194" s="107"/>
-      <c r="F194" s="108"/>
-      <c r="G194" s="108"/>
-      <c r="H194" s="108"/>
-      <c r="I194" s="108"/>
-      <c r="J194" s="108"/>
-      <c r="K194" s="108"/>
-      <c r="L194" s="108"/>
+      <c r="C194" s="114"/>
+      <c r="D194" s="114"/>
+      <c r="E194" s="114"/>
+      <c r="F194" s="122"/>
+      <c r="G194" s="122"/>
+      <c r="H194" s="122"/>
+      <c r="I194" s="122"/>
+      <c r="J194" s="122"/>
+      <c r="K194" s="122"/>
+      <c r="L194" s="122"/>
     </row>
     <row r="195" spans="1:12">
       <c r="A195" s="61"/>
       <c r="B195" s="5"/>
-      <c r="C195" s="107"/>
-      <c r="D195" s="107"/>
-      <c r="E195" s="107"/>
-      <c r="F195" s="108"/>
-      <c r="G195" s="108"/>
-      <c r="H195" s="108"/>
-      <c r="I195" s="108"/>
-      <c r="J195" s="108"/>
-      <c r="K195" s="108"/>
-      <c r="L195" s="108"/>
+      <c r="C195" s="114"/>
+      <c r="D195" s="114"/>
+      <c r="E195" s="114"/>
+      <c r="F195" s="122"/>
+      <c r="G195" s="122"/>
+      <c r="H195" s="122"/>
+      <c r="I195" s="122"/>
+      <c r="J195" s="122"/>
+      <c r="K195" s="122"/>
+      <c r="L195" s="122"/>
     </row>
     <row r="196" spans="1:12">
       <c r="A196" s="60"/>
       <c r="B196" s="16"/>
-      <c r="C196" s="107"/>
-      <c r="D196" s="107"/>
-      <c r="E196" s="107"/>
-      <c r="F196" s="108"/>
-      <c r="G196" s="108"/>
-      <c r="H196" s="108"/>
-      <c r="I196" s="108"/>
-      <c r="J196" s="108"/>
-      <c r="K196" s="108"/>
-      <c r="L196" s="108"/>
+      <c r="C196" s="114"/>
+      <c r="D196" s="114"/>
+      <c r="E196" s="114"/>
+      <c r="F196" s="122"/>
+      <c r="G196" s="122"/>
+      <c r="H196" s="122"/>
+      <c r="I196" s="122"/>
+      <c r="J196" s="122"/>
+      <c r="K196" s="122"/>
+      <c r="L196" s="122"/>
     </row>
     <row r="197" spans="1:12">
       <c r="A197" s="61"/>
       <c r="B197" s="5"/>
-      <c r="C197" s="107"/>
-      <c r="D197" s="107"/>
-      <c r="E197" s="107"/>
-      <c r="F197" s="108"/>
-      <c r="G197" s="108"/>
-      <c r="H197" s="108"/>
-      <c r="I197" s="108"/>
-      <c r="J197" s="108"/>
-      <c r="K197" s="108"/>
-      <c r="L197" s="108"/>
+      <c r="C197" s="114"/>
+      <c r="D197" s="114"/>
+      <c r="E197" s="114"/>
+      <c r="F197" s="122"/>
+      <c r="G197" s="122"/>
+      <c r="H197" s="122"/>
+      <c r="I197" s="122"/>
+      <c r="J197" s="122"/>
+      <c r="K197" s="122"/>
+      <c r="L197" s="122"/>
     </row>
     <row r="198" spans="1:12">
       <c r="A198" s="61"/>
       <c r="B198" s="5"/>
-      <c r="C198" s="107"/>
-      <c r="D198" s="107"/>
-      <c r="E198" s="107"/>
-      <c r="F198" s="108"/>
-      <c r="G198" s="108"/>
-      <c r="H198" s="108"/>
-      <c r="I198" s="108"/>
-      <c r="J198" s="108"/>
-      <c r="K198" s="108"/>
-      <c r="L198" s="108"/>
+      <c r="C198" s="114"/>
+      <c r="D198" s="114"/>
+      <c r="E198" s="114"/>
+      <c r="F198" s="122"/>
+      <c r="G198" s="122"/>
+      <c r="H198" s="122"/>
+      <c r="I198" s="122"/>
+      <c r="J198" s="122"/>
+      <c r="K198" s="122"/>
+      <c r="L198" s="122"/>
     </row>
     <row r="199" spans="1:12">
       <c r="A199" s="61"/>
       <c r="B199" s="5"/>
-      <c r="C199" s="107"/>
-      <c r="D199" s="107"/>
-      <c r="E199" s="107"/>
-      <c r="F199" s="108"/>
-      <c r="G199" s="108"/>
-      <c r="H199" s="108"/>
-      <c r="I199" s="108"/>
-      <c r="J199" s="108"/>
-      <c r="K199" s="108"/>
-      <c r="L199" s="108"/>
+      <c r="C199" s="114"/>
+      <c r="D199" s="114"/>
+      <c r="E199" s="114"/>
+      <c r="F199" s="122"/>
+      <c r="G199" s="122"/>
+      <c r="H199" s="122"/>
+      <c r="I199" s="122"/>
+      <c r="J199" s="122"/>
+      <c r="K199" s="122"/>
+      <c r="L199" s="122"/>
     </row>
     <row r="200" spans="1:12">
       <c r="A200" s="61"/>
       <c r="B200" s="5"/>
-      <c r="C200" s="107"/>
-      <c r="D200" s="107"/>
-      <c r="E200" s="107"/>
-      <c r="F200" s="108"/>
-      <c r="G200" s="108"/>
-      <c r="H200" s="108"/>
-      <c r="I200" s="108"/>
-      <c r="J200" s="108"/>
-      <c r="K200" s="108"/>
-      <c r="L200" s="108"/>
+      <c r="C200" s="114"/>
+      <c r="D200" s="114"/>
+      <c r="E200" s="114"/>
+      <c r="F200" s="122"/>
+      <c r="G200" s="122"/>
+      <c r="H200" s="122"/>
+      <c r="I200" s="122"/>
+      <c r="J200" s="122"/>
+      <c r="K200" s="122"/>
+      <c r="L200" s="122"/>
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="61"/>
       <c r="B201" s="5"/>
-      <c r="C201" s="107"/>
-      <c r="D201" s="107"/>
-      <c r="E201" s="107"/>
-      <c r="F201" s="108"/>
-      <c r="G201" s="108"/>
-      <c r="H201" s="108"/>
-      <c r="I201" s="108"/>
-      <c r="J201" s="108"/>
-      <c r="K201" s="108"/>
-      <c r="L201" s="108"/>
+      <c r="C201" s="114"/>
+      <c r="D201" s="114"/>
+      <c r="E201" s="114"/>
+      <c r="F201" s="122"/>
+      <c r="G201" s="122"/>
+      <c r="H201" s="122"/>
+      <c r="I201" s="122"/>
+      <c r="J201" s="122"/>
+      <c r="K201" s="122"/>
+      <c r="L201" s="122"/>
     </row>
     <row r="202" spans="1:12">
       <c r="A202" s="60"/>
       <c r="B202" s="16"/>
-      <c r="C202" s="107"/>
-      <c r="D202" s="107"/>
-      <c r="E202" s="107"/>
-      <c r="F202" s="108"/>
-      <c r="G202" s="108"/>
-      <c r="H202" s="108"/>
-      <c r="I202" s="108"/>
-      <c r="J202" s="108"/>
-      <c r="K202" s="108"/>
-      <c r="L202" s="108"/>
+      <c r="C202" s="114"/>
+      <c r="D202" s="114"/>
+      <c r="E202" s="114"/>
+      <c r="F202" s="122"/>
+      <c r="G202" s="122"/>
+      <c r="H202" s="122"/>
+      <c r="I202" s="122"/>
+      <c r="J202" s="122"/>
+      <c r="K202" s="122"/>
+      <c r="L202" s="122"/>
     </row>
     <row r="203" spans="1:12">
       <c r="A203" s="61"/>
       <c r="B203" s="5"/>
-      <c r="C203" s="107"/>
-      <c r="D203" s="107"/>
-      <c r="E203" s="107"/>
-      <c r="F203" s="108"/>
-      <c r="G203" s="108"/>
-      <c r="H203" s="108"/>
-      <c r="I203" s="108"/>
-      <c r="J203" s="108"/>
-      <c r="K203" s="108"/>
-      <c r="L203" s="108"/>
+      <c r="C203" s="114"/>
+      <c r="D203" s="114"/>
+      <c r="E203" s="114"/>
+      <c r="F203" s="122"/>
+      <c r="G203" s="122"/>
+      <c r="H203" s="122"/>
+      <c r="I203" s="122"/>
+      <c r="J203" s="122"/>
+      <c r="K203" s="122"/>
+      <c r="L203" s="122"/>
     </row>
     <row r="204" spans="1:12">
       <c r="A204" s="61"/>
       <c r="B204" s="5"/>
-      <c r="C204" s="107"/>
-      <c r="D204" s="107"/>
-      <c r="E204" s="107"/>
-      <c r="F204" s="108"/>
-      <c r="G204" s="108"/>
-      <c r="H204" s="108"/>
-      <c r="I204" s="108"/>
-      <c r="J204" s="108"/>
-      <c r="K204" s="108"/>
-      <c r="L204" s="108"/>
+      <c r="C204" s="114"/>
+      <c r="D204" s="114"/>
+      <c r="E204" s="114"/>
+      <c r="F204" s="122"/>
+      <c r="G204" s="122"/>
+      <c r="H204" s="122"/>
+      <c r="I204" s="122"/>
+      <c r="J204" s="122"/>
+      <c r="K204" s="122"/>
+      <c r="L204" s="122"/>
     </row>
     <row r="205" spans="1:12">
       <c r="A205" s="61"/>
@@ -11150,84 +11163,6 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C165:E165"/>
-    <mergeCell ref="C166:E166"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B162:L162"/>
-    <mergeCell ref="F163:L163"/>
-    <mergeCell ref="A163:E163"/>
-    <mergeCell ref="A161:L161"/>
-    <mergeCell ref="A157:L157"/>
-    <mergeCell ref="C177:E177"/>
-    <mergeCell ref="C178:E178"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="C180:E180"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="C172:E172"/>
-    <mergeCell ref="C173:E173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C175:E175"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C164:E164"/>
-    <mergeCell ref="C169:E169"/>
-    <mergeCell ref="C170:E170"/>
-    <mergeCell ref="F164:L164"/>
-    <mergeCell ref="F165:L165"/>
-    <mergeCell ref="F166:L166"/>
-    <mergeCell ref="F167:L167"/>
-    <mergeCell ref="F168:L168"/>
-    <mergeCell ref="F169:L169"/>
-    <mergeCell ref="F170:L170"/>
-    <mergeCell ref="F171:L171"/>
-    <mergeCell ref="C167:E167"/>
-    <mergeCell ref="C168:E168"/>
-    <mergeCell ref="F181:L181"/>
-    <mergeCell ref="F182:L182"/>
-    <mergeCell ref="F183:L183"/>
-    <mergeCell ref="F184:L184"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="C194:E194"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="F172:L172"/>
-    <mergeCell ref="F173:L173"/>
-    <mergeCell ref="F174:L174"/>
-    <mergeCell ref="F175:L175"/>
-    <mergeCell ref="F176:L176"/>
-    <mergeCell ref="F177:L177"/>
-    <mergeCell ref="F178:L178"/>
-    <mergeCell ref="F179:L179"/>
-    <mergeCell ref="F180:L180"/>
-    <mergeCell ref="F195:L195"/>
-    <mergeCell ref="F196:L196"/>
-    <mergeCell ref="F197:L197"/>
-    <mergeCell ref="F190:L190"/>
-    <mergeCell ref="F191:L191"/>
-    <mergeCell ref="F192:L192"/>
-    <mergeCell ref="F193:L193"/>
-    <mergeCell ref="F194:L194"/>
-    <mergeCell ref="F185:L185"/>
-    <mergeCell ref="F186:L186"/>
-    <mergeCell ref="F187:L187"/>
-    <mergeCell ref="F188:L188"/>
-    <mergeCell ref="F189:L189"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C195:E195"/>
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C171:E171"/>
     <mergeCell ref="C204:E204"/>
     <mergeCell ref="F198:L198"/>
     <mergeCell ref="F199:L199"/>
@@ -11241,15 +11176,93 @@
     <mergeCell ref="C201:E201"/>
     <mergeCell ref="C202:E202"/>
     <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C171:E171"/>
+    <mergeCell ref="F195:L195"/>
+    <mergeCell ref="F196:L196"/>
+    <mergeCell ref="F197:L197"/>
+    <mergeCell ref="F190:L190"/>
+    <mergeCell ref="F191:L191"/>
+    <mergeCell ref="F192:L192"/>
+    <mergeCell ref="F193:L193"/>
+    <mergeCell ref="F194:L194"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="C194:E194"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="F183:L183"/>
+    <mergeCell ref="F184:L184"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="F185:L185"/>
+    <mergeCell ref="F186:L186"/>
+    <mergeCell ref="F187:L187"/>
+    <mergeCell ref="F188:L188"/>
+    <mergeCell ref="F189:L189"/>
+    <mergeCell ref="F171:L171"/>
+    <mergeCell ref="C167:E167"/>
+    <mergeCell ref="C168:E168"/>
+    <mergeCell ref="F181:L181"/>
+    <mergeCell ref="F182:L182"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="F172:L172"/>
+    <mergeCell ref="F173:L173"/>
+    <mergeCell ref="F174:L174"/>
+    <mergeCell ref="F175:L175"/>
+    <mergeCell ref="F176:L176"/>
+    <mergeCell ref="F177:L177"/>
+    <mergeCell ref="F178:L178"/>
+    <mergeCell ref="F179:L179"/>
+    <mergeCell ref="F180:L180"/>
+    <mergeCell ref="C169:E169"/>
+    <mergeCell ref="C170:E170"/>
+    <mergeCell ref="F164:L164"/>
+    <mergeCell ref="F165:L165"/>
+    <mergeCell ref="F166:L166"/>
+    <mergeCell ref="F167:L167"/>
+    <mergeCell ref="F168:L168"/>
+    <mergeCell ref="F169:L169"/>
+    <mergeCell ref="F170:L170"/>
+    <mergeCell ref="C172:E172"/>
+    <mergeCell ref="C173:E173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C175:E175"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C177:E177"/>
+    <mergeCell ref="C178:E178"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="C180:E180"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C166:E166"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B162:L162"/>
+    <mergeCell ref="F163:L163"/>
+    <mergeCell ref="A163:E163"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A157:L157"/>
+    <mergeCell ref="C164:E164"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C261:E261 C237:E237 C243:E243 C249:E249 C255:E255 C225:E225 C231:E231 C213:E213 C219:E219 C207:E207">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C261:E261 C237:E237 C243:E243 C249:E249 C255:E255 C225:E225 C231:E231 C213:E213 C219:E219 C207:E207" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"ja, nein, offen"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C252:E252 C258:E258 C222:E222 C228:E228 C234:E234 C240:E240 C246:E246 C216:E216 C210:E210">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C252:E252 C258:E258 C222:E222 C228:E228 C234:E234 C240:E240 C246:E246 C216:E216 C210:E210" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"keine IT Lösung im Einsatz, nicht integrierte IT Lösung, Anbindung über Schnittstelle, Voll integriert, ERP Modul"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C169:C170 C167">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" promptTitle="Bitte auswählen" prompt="dfdf" sqref="C169:C170 C167" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>"ja, nein"</formula1>
     </dataValidation>
   </dataValidations>
@@ -11266,7 +11279,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:D61"/>
   <sheetViews>
@@ -11274,17 +11287,17 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.88671875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="45.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5546875" style="1"/>
-    <col min="7" max="7" width="47.5546875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.44140625" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="45.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="1"/>
+    <col min="7" max="7" width="47.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="34.42578125" style="1" customWidth="1"/>
+    <col min="9" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11303,11 +11316,11 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10"/>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>403</v>
       </c>
-      <c r="C2" s="116"/>
-      <c r="D2" s="116"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="18" t="s">
@@ -11321,7 +11334,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="27.6">
+    <row r="4" spans="1:4" ht="25.5">
       <c r="A4" s="39"/>
       <c r="B4" s="2" t="s">
         <v>405</v>
@@ -11329,7 +11342,7 @@
       <c r="C4" s="17"/>
       <c r="D4" s="45"/>
     </row>
-    <row r="5" spans="1:4" ht="27.6">
+    <row r="5" spans="1:4" ht="25.5">
       <c r="A5" s="39"/>
       <c r="B5" s="2" t="s">
         <v>406</v>
@@ -11349,7 +11362,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="27.6">
+    <row r="7" spans="1:4" ht="25.5">
       <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>408</v>
@@ -11477,7 +11490,7 @@
       <c r="C22" s="17"/>
       <c r="D22" s="45"/>
     </row>
-    <row r="23" spans="1:4" ht="27.6">
+    <row r="23" spans="1:4" ht="25.5">
       <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>424</v>
@@ -11808,7 +11821,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1:C83"/>
   <sheetViews>
@@ -11816,16 +11829,16 @@
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.5546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="87.44140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" style="1"/>
-    <col min="6" max="6" width="47.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.44140625" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="87.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" style="1"/>
+    <col min="6" max="6" width="47.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -11837,14 +11850,14 @@
       </c>
       <c r="C1" s="55"/>
     </row>
-    <row r="2" spans="1:3" ht="44.4" customHeight="1">
+    <row r="2" spans="1:3" ht="44.45" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="116"/>
-    </row>
-    <row r="3" spans="1:3" ht="17.399999999999999" customHeight="1">
+      <c r="C2" s="115"/>
+    </row>
+    <row r="3" spans="1:3" ht="17.45" customHeight="1">
       <c r="A3" s="47"/>
       <c r="B3" s="47"/>
       <c r="C3" s="47" t="s">
@@ -11902,7 +11915,7 @@
       </c>
       <c r="C10" s="45"/>
     </row>
-    <row r="11" spans="1:3" ht="27.6">
+    <row r="11" spans="1:3" ht="25.5">
       <c r="A11" s="18" t="s">
         <v>331</v>
       </c>
@@ -12048,7 +12061,7 @@
       </c>
       <c r="C30" s="45"/>
     </row>
-    <row r="31" spans="1:3" ht="27.6">
+    <row r="31" spans="1:3" ht="25.5">
       <c r="A31" s="18" t="s">
         <v>337</v>
       </c>
@@ -12126,7 +12139,7 @@
       </c>
       <c r="C40" s="19"/>
     </row>
-    <row r="41" spans="1:3" ht="27.6">
+    <row r="41" spans="1:3" ht="25.5">
       <c r="A41" s="23"/>
       <c r="B41" s="2" t="s">
         <v>471</v>

</xml_diff>

<commit_message>
[BUGFIX] columns not fit into one page
</commit_message>
<xml_diff>
--- a/resources/excel/specification_configurator_template.xlsx
+++ b/resources/excel/specification_configurator_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\abas-specificationsconfigurator-api-web\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC99D77-FDE9-4021-B0DE-0D278973BFFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E35AE8-D625-4171-8122-76BF453FE78F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41550" yWindow="3315" windowWidth="32100" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Firmenprofil" sheetId="1" r:id="rId1"/>
@@ -2323,14 +2323,24 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2346,16 +2356,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2796,13 +2796,13 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="9" customWidth="1"/>
-    <col min="2" max="2" width="48.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" style="9" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -3133,14 +3133,14 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -3778,14 +3778,14 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -4327,14 +4327,14 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B172" sqref="B172"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="9" customWidth="1"/>
-    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="85.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -6097,14 +6097,14 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:C240"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="56.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5703125" style="1"/>
   </cols>
@@ -7445,14 +7445,14 @@
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F159" sqref="F159"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="59" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" style="59" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" style="59" customWidth="1"/>
     <col min="3" max="5" width="8.7109375" style="59" customWidth="1"/>
     <col min="6" max="11" width="5.28515625" style="59" customWidth="1"/>
     <col min="12" max="12" width="45.140625" style="59" customWidth="1"/>
@@ -7470,38 +7470,38 @@
       <c r="B1" s="75" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="113" t="s">
+      <c r="C1" s="117" t="s">
         <v>345</v>
       </c>
-      <c r="D1" s="113"/>
-      <c r="E1" s="113"/>
-      <c r="F1" s="112" t="s">
+      <c r="D1" s="117"/>
+      <c r="E1" s="117"/>
+      <c r="F1" s="116" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="112"/>
-      <c r="H1" s="112"/>
-      <c r="I1" s="112"/>
-      <c r="J1" s="112"/>
-      <c r="K1" s="112"/>
-      <c r="L1" s="112"/>
+      <c r="G1" s="116"/>
+      <c r="H1" s="116"/>
+      <c r="I1" s="116"/>
+      <c r="J1" s="116"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
     </row>
     <row r="2" spans="1:12" ht="37.9" customHeight="1">
       <c r="A2" s="76"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="118" t="s">
         <v>512</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="112" t="s">
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
+      <c r="E2" s="118"/>
+      <c r="F2" s="116" t="s">
         <v>503</v>
       </c>
-      <c r="G2" s="112"/>
-      <c r="H2" s="112"/>
-      <c r="I2" s="112"/>
-      <c r="J2" s="112"/>
-      <c r="K2" s="112"/>
-      <c r="L2" s="112"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
     </row>
     <row r="3" spans="1:12" ht="24">
       <c r="A3" s="77" t="s">
@@ -9948,18 +9948,18 @@
       <c r="L156" s="87"/>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" s="119"/>
-      <c r="B157" s="119"/>
-      <c r="C157" s="119"/>
-      <c r="D157" s="119"/>
-      <c r="E157" s="119"/>
-      <c r="F157" s="119"/>
-      <c r="G157" s="119"/>
-      <c r="H157" s="119"/>
-      <c r="I157" s="119"/>
-      <c r="J157" s="119"/>
-      <c r="K157" s="119"/>
-      <c r="L157" s="119"/>
+      <c r="A157" s="122"/>
+      <c r="B157" s="122"/>
+      <c r="C157" s="122"/>
+      <c r="D157" s="122"/>
+      <c r="E157" s="122"/>
+      <c r="F157" s="122"/>
+      <c r="G157" s="122"/>
+      <c r="H157" s="122"/>
+      <c r="I157" s="122"/>
+      <c r="J157" s="122"/>
+      <c r="K157" s="122"/>
+      <c r="L157" s="122"/>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="61"/>
@@ -10063,648 +10063,648 @@
       </c>
     </row>
     <row r="161" spans="1:12">
-      <c r="A161" s="118"/>
-      <c r="B161" s="118"/>
-      <c r="C161" s="118"/>
-      <c r="D161" s="118"/>
-      <c r="E161" s="118"/>
-      <c r="F161" s="118"/>
-      <c r="G161" s="118"/>
-      <c r="H161" s="118"/>
-      <c r="I161" s="118"/>
-      <c r="J161" s="118"/>
-      <c r="K161" s="118"/>
-      <c r="L161" s="118"/>
+      <c r="A161" s="121"/>
+      <c r="B161" s="121"/>
+      <c r="C161" s="121"/>
+      <c r="D161" s="121"/>
+      <c r="E161" s="121"/>
+      <c r="F161" s="121"/>
+      <c r="G161" s="121"/>
+      <c r="H161" s="121"/>
+      <c r="I161" s="121"/>
+      <c r="J161" s="121"/>
+      <c r="K161" s="121"/>
+      <c r="L161" s="121"/>
     </row>
     <row r="162" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A162" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="B162" s="116" t="s">
+      <c r="B162" s="119" t="s">
         <v>168</v>
       </c>
-      <c r="C162" s="116"/>
-      <c r="D162" s="116"/>
-      <c r="E162" s="116"/>
-      <c r="F162" s="116"/>
-      <c r="G162" s="116"/>
-      <c r="H162" s="116"/>
-      <c r="I162" s="116"/>
-      <c r="J162" s="116"/>
-      <c r="K162" s="116"/>
-      <c r="L162" s="116"/>
+      <c r="C162" s="119"/>
+      <c r="D162" s="119"/>
+      <c r="E162" s="119"/>
+      <c r="F162" s="119"/>
+      <c r="G162" s="119"/>
+      <c r="H162" s="119"/>
+      <c r="I162" s="119"/>
+      <c r="J162" s="119"/>
+      <c r="K162" s="119"/>
+      <c r="L162" s="119"/>
     </row>
     <row r="163" spans="1:12" ht="33" customHeight="1">
-      <c r="A163" s="117"/>
-      <c r="B163" s="117"/>
-      <c r="C163" s="117"/>
-      <c r="D163" s="117"/>
-      <c r="E163" s="117"/>
-      <c r="F163" s="112" t="s">
+      <c r="A163" s="120"/>
+      <c r="B163" s="120"/>
+      <c r="C163" s="120"/>
+      <c r="D163" s="120"/>
+      <c r="E163" s="120"/>
+      <c r="F163" s="116" t="s">
         <v>501</v>
       </c>
-      <c r="G163" s="112"/>
-      <c r="H163" s="112"/>
-      <c r="I163" s="112"/>
-      <c r="J163" s="112"/>
-      <c r="K163" s="112"/>
-      <c r="L163" s="112"/>
+      <c r="G163" s="116"/>
+      <c r="H163" s="116"/>
+      <c r="I163" s="116"/>
+      <c r="J163" s="116"/>
+      <c r="K163" s="116"/>
+      <c r="L163" s="116"/>
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="61"/>
       <c r="B164" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="C164" s="114"/>
-      <c r="D164" s="114"/>
-      <c r="E164" s="114"/>
-      <c r="F164" s="121"/>
-      <c r="G164" s="121"/>
-      <c r="H164" s="121"/>
-      <c r="I164" s="121"/>
-      <c r="J164" s="121"/>
-      <c r="K164" s="121"/>
-      <c r="L164" s="121"/>
+      <c r="C164" s="112"/>
+      <c r="D164" s="112"/>
+      <c r="E164" s="112"/>
+      <c r="F164" s="114"/>
+      <c r="G164" s="114"/>
+      <c r="H164" s="114"/>
+      <c r="I164" s="114"/>
+      <c r="J164" s="114"/>
+      <c r="K164" s="114"/>
+      <c r="L164" s="114"/>
     </row>
     <row r="165" spans="1:12" ht="25.5">
       <c r="A165" s="61"/>
       <c r="B165" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C165" s="114"/>
-      <c r="D165" s="114"/>
-      <c r="E165" s="114"/>
-      <c r="F165" s="121"/>
-      <c r="G165" s="121"/>
-      <c r="H165" s="121"/>
-      <c r="I165" s="121"/>
-      <c r="J165" s="121"/>
-      <c r="K165" s="121"/>
-      <c r="L165" s="121"/>
+      <c r="C165" s="112"/>
+      <c r="D165" s="112"/>
+      <c r="E165" s="112"/>
+      <c r="F165" s="114"/>
+      <c r="G165" s="114"/>
+      <c r="H165" s="114"/>
+      <c r="I165" s="114"/>
+      <c r="J165" s="114"/>
+      <c r="K165" s="114"/>
+      <c r="L165" s="114"/>
     </row>
     <row r="166" spans="1:12" ht="25.5">
       <c r="A166" s="60"/>
       <c r="B166" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C166" s="114"/>
-      <c r="D166" s="114"/>
-      <c r="E166" s="114"/>
-      <c r="F166" s="121"/>
-      <c r="G166" s="121"/>
-      <c r="H166" s="121"/>
-      <c r="I166" s="121"/>
-      <c r="J166" s="121"/>
-      <c r="K166" s="121"/>
-      <c r="L166" s="121"/>
+      <c r="C166" s="112"/>
+      <c r="D166" s="112"/>
+      <c r="E166" s="112"/>
+      <c r="F166" s="114"/>
+      <c r="G166" s="114"/>
+      <c r="H166" s="114"/>
+      <c r="I166" s="114"/>
+      <c r="J166" s="114"/>
+      <c r="K166" s="114"/>
+      <c r="L166" s="114"/>
     </row>
     <row r="167" spans="1:12" ht="14.45" customHeight="1">
       <c r="A167" s="61"/>
       <c r="B167" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="C167" s="120" t="s">
-        <v>510</v>
-      </c>
-      <c r="D167" s="120"/>
-      <c r="E167" s="120"/>
-      <c r="F167" s="121"/>
-      <c r="G167" s="121"/>
-      <c r="H167" s="121"/>
-      <c r="I167" s="121"/>
-      <c r="J167" s="121"/>
-      <c r="K167" s="121"/>
-      <c r="L167" s="121"/>
+      <c r="C167" s="115" t="s">
+        <v>510</v>
+      </c>
+      <c r="D167" s="115"/>
+      <c r="E167" s="115"/>
+      <c r="F167" s="114"/>
+      <c r="G167" s="114"/>
+      <c r="H167" s="114"/>
+      <c r="I167" s="114"/>
+      <c r="J167" s="114"/>
+      <c r="K167" s="114"/>
+      <c r="L167" s="114"/>
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="61"/>
       <c r="B168" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="C168" s="114"/>
-      <c r="D168" s="114"/>
-      <c r="E168" s="114"/>
-      <c r="F168" s="121"/>
-      <c r="G168" s="121"/>
-      <c r="H168" s="121"/>
-      <c r="I168" s="121"/>
-      <c r="J168" s="121"/>
-      <c r="K168" s="121"/>
-      <c r="L168" s="121"/>
+      <c r="C168" s="112"/>
+      <c r="D168" s="112"/>
+      <c r="E168" s="112"/>
+      <c r="F168" s="114"/>
+      <c r="G168" s="114"/>
+      <c r="H168" s="114"/>
+      <c r="I168" s="114"/>
+      <c r="J168" s="114"/>
+      <c r="K168" s="114"/>
+      <c r="L168" s="114"/>
     </row>
     <row r="169" spans="1:12" ht="25.5">
       <c r="A169" s="61"/>
       <c r="B169" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C169" s="120" t="s">
-        <v>510</v>
-      </c>
-      <c r="D169" s="120"/>
-      <c r="E169" s="120"/>
-      <c r="F169" s="121"/>
-      <c r="G169" s="121"/>
-      <c r="H169" s="121"/>
-      <c r="I169" s="121"/>
-      <c r="J169" s="121"/>
-      <c r="K169" s="121"/>
-      <c r="L169" s="121"/>
+      <c r="C169" s="115" t="s">
+        <v>510</v>
+      </c>
+      <c r="D169" s="115"/>
+      <c r="E169" s="115"/>
+      <c r="F169" s="114"/>
+      <c r="G169" s="114"/>
+      <c r="H169" s="114"/>
+      <c r="I169" s="114"/>
+      <c r="J169" s="114"/>
+      <c r="K169" s="114"/>
+      <c r="L169" s="114"/>
     </row>
     <row r="170" spans="1:12" ht="25.5">
       <c r="A170" s="61"/>
       <c r="B170" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C170" s="120" t="s">
-        <v>510</v>
-      </c>
-      <c r="D170" s="120"/>
-      <c r="E170" s="120"/>
-      <c r="F170" s="121"/>
-      <c r="G170" s="121"/>
-      <c r="H170" s="121"/>
-      <c r="I170" s="121"/>
-      <c r="J170" s="121"/>
-      <c r="K170" s="121"/>
-      <c r="L170" s="121"/>
+      <c r="C170" s="115" t="s">
+        <v>510</v>
+      </c>
+      <c r="D170" s="115"/>
+      <c r="E170" s="115"/>
+      <c r="F170" s="114"/>
+      <c r="G170" s="114"/>
+      <c r="H170" s="114"/>
+      <c r="I170" s="114"/>
+      <c r="J170" s="114"/>
+      <c r="K170" s="114"/>
+      <c r="L170" s="114"/>
     </row>
     <row r="171" spans="1:12" ht="25.5">
       <c r="A171" s="61"/>
       <c r="B171" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C171" s="114"/>
-      <c r="D171" s="114"/>
-      <c r="E171" s="114"/>
-      <c r="F171" s="121"/>
-      <c r="G171" s="121"/>
-      <c r="H171" s="121"/>
-      <c r="I171" s="121"/>
-      <c r="J171" s="121"/>
-      <c r="K171" s="121"/>
-      <c r="L171" s="121"/>
+      <c r="C171" s="112"/>
+      <c r="D171" s="112"/>
+      <c r="E171" s="112"/>
+      <c r="F171" s="114"/>
+      <c r="G171" s="114"/>
+      <c r="H171" s="114"/>
+      <c r="I171" s="114"/>
+      <c r="J171" s="114"/>
+      <c r="K171" s="114"/>
+      <c r="L171" s="114"/>
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="60"/>
       <c r="B172" s="16"/>
-      <c r="C172" s="114"/>
-      <c r="D172" s="114"/>
-      <c r="E172" s="114"/>
-      <c r="F172" s="122"/>
-      <c r="G172" s="122"/>
-      <c r="H172" s="122"/>
-      <c r="I172" s="122"/>
-      <c r="J172" s="122"/>
-      <c r="K172" s="122"/>
-      <c r="L172" s="122"/>
+      <c r="C172" s="112"/>
+      <c r="D172" s="112"/>
+      <c r="E172" s="112"/>
+      <c r="F172" s="113"/>
+      <c r="G172" s="113"/>
+      <c r="H172" s="113"/>
+      <c r="I172" s="113"/>
+      <c r="J172" s="113"/>
+      <c r="K172" s="113"/>
+      <c r="L172" s="113"/>
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="61"/>
       <c r="B173" s="5"/>
-      <c r="C173" s="114"/>
-      <c r="D173" s="114"/>
-      <c r="E173" s="114"/>
-      <c r="F173" s="122"/>
-      <c r="G173" s="122"/>
-      <c r="H173" s="122"/>
-      <c r="I173" s="122"/>
-      <c r="J173" s="122"/>
-      <c r="K173" s="122"/>
-      <c r="L173" s="122"/>
+      <c r="C173" s="112"/>
+      <c r="D173" s="112"/>
+      <c r="E173" s="112"/>
+      <c r="F173" s="113"/>
+      <c r="G173" s="113"/>
+      <c r="H173" s="113"/>
+      <c r="I173" s="113"/>
+      <c r="J173" s="113"/>
+      <c r="K173" s="113"/>
+      <c r="L173" s="113"/>
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="61"/>
       <c r="B174" s="5"/>
-      <c r="C174" s="114"/>
-      <c r="D174" s="114"/>
-      <c r="E174" s="114"/>
-      <c r="F174" s="122"/>
-      <c r="G174" s="122"/>
-      <c r="H174" s="122"/>
-      <c r="I174" s="122"/>
-      <c r="J174" s="122"/>
-      <c r="K174" s="122"/>
-      <c r="L174" s="122"/>
+      <c r="C174" s="112"/>
+      <c r="D174" s="112"/>
+      <c r="E174" s="112"/>
+      <c r="F174" s="113"/>
+      <c r="G174" s="113"/>
+      <c r="H174" s="113"/>
+      <c r="I174" s="113"/>
+      <c r="J174" s="113"/>
+      <c r="K174" s="113"/>
+      <c r="L174" s="113"/>
     </row>
     <row r="175" spans="1:12">
       <c r="A175" s="61"/>
       <c r="B175" s="5"/>
-      <c r="C175" s="114"/>
-      <c r="D175" s="114"/>
-      <c r="E175" s="114"/>
-      <c r="F175" s="122"/>
-      <c r="G175" s="122"/>
-      <c r="H175" s="122"/>
-      <c r="I175" s="122"/>
-      <c r="J175" s="122"/>
-      <c r="K175" s="122"/>
-      <c r="L175" s="122"/>
+      <c r="C175" s="112"/>
+      <c r="D175" s="112"/>
+      <c r="E175" s="112"/>
+      <c r="F175" s="113"/>
+      <c r="G175" s="113"/>
+      <c r="H175" s="113"/>
+      <c r="I175" s="113"/>
+      <c r="J175" s="113"/>
+      <c r="K175" s="113"/>
+      <c r="L175" s="113"/>
     </row>
     <row r="176" spans="1:12">
       <c r="A176" s="61"/>
       <c r="B176" s="5"/>
-      <c r="C176" s="114"/>
-      <c r="D176" s="114"/>
-      <c r="E176" s="114"/>
-      <c r="F176" s="122"/>
-      <c r="G176" s="122"/>
-      <c r="H176" s="122"/>
-      <c r="I176" s="122"/>
-      <c r="J176" s="122"/>
-      <c r="K176" s="122"/>
-      <c r="L176" s="122"/>
+      <c r="C176" s="112"/>
+      <c r="D176" s="112"/>
+      <c r="E176" s="112"/>
+      <c r="F176" s="113"/>
+      <c r="G176" s="113"/>
+      <c r="H176" s="113"/>
+      <c r="I176" s="113"/>
+      <c r="J176" s="113"/>
+      <c r="K176" s="113"/>
+      <c r="L176" s="113"/>
     </row>
     <row r="177" spans="1:12">
       <c r="A177" s="61"/>
       <c r="B177" s="5"/>
-      <c r="C177" s="114"/>
-      <c r="D177" s="114"/>
-      <c r="E177" s="114"/>
-      <c r="F177" s="122"/>
-      <c r="G177" s="122"/>
-      <c r="H177" s="122"/>
-      <c r="I177" s="122"/>
-      <c r="J177" s="122"/>
-      <c r="K177" s="122"/>
-      <c r="L177" s="122"/>
+      <c r="C177" s="112"/>
+      <c r="D177" s="112"/>
+      <c r="E177" s="112"/>
+      <c r="F177" s="113"/>
+      <c r="G177" s="113"/>
+      <c r="H177" s="113"/>
+      <c r="I177" s="113"/>
+      <c r="J177" s="113"/>
+      <c r="K177" s="113"/>
+      <c r="L177" s="113"/>
     </row>
     <row r="178" spans="1:12">
       <c r="A178" s="60"/>
       <c r="B178" s="16"/>
-      <c r="C178" s="114"/>
-      <c r="D178" s="114"/>
-      <c r="E178" s="114"/>
-      <c r="F178" s="122"/>
-      <c r="G178" s="122"/>
-      <c r="H178" s="122"/>
-      <c r="I178" s="122"/>
-      <c r="J178" s="122"/>
-      <c r="K178" s="122"/>
-      <c r="L178" s="122"/>
+      <c r="C178" s="112"/>
+      <c r="D178" s="112"/>
+      <c r="E178" s="112"/>
+      <c r="F178" s="113"/>
+      <c r="G178" s="113"/>
+      <c r="H178" s="113"/>
+      <c r="I178" s="113"/>
+      <c r="J178" s="113"/>
+      <c r="K178" s="113"/>
+      <c r="L178" s="113"/>
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="61"/>
       <c r="B179" s="5"/>
-      <c r="C179" s="114"/>
-      <c r="D179" s="114"/>
-      <c r="E179" s="114"/>
-      <c r="F179" s="122"/>
-      <c r="G179" s="122"/>
-      <c r="H179" s="122"/>
-      <c r="I179" s="122"/>
-      <c r="J179" s="122"/>
-      <c r="K179" s="122"/>
-      <c r="L179" s="122"/>
+      <c r="C179" s="112"/>
+      <c r="D179" s="112"/>
+      <c r="E179" s="112"/>
+      <c r="F179" s="113"/>
+      <c r="G179" s="113"/>
+      <c r="H179" s="113"/>
+      <c r="I179" s="113"/>
+      <c r="J179" s="113"/>
+      <c r="K179" s="113"/>
+      <c r="L179" s="113"/>
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="61"/>
       <c r="B180" s="5"/>
-      <c r="C180" s="114"/>
-      <c r="D180" s="114"/>
-      <c r="E180" s="114"/>
-      <c r="F180" s="122"/>
-      <c r="G180" s="122"/>
-      <c r="H180" s="122"/>
-      <c r="I180" s="122"/>
-      <c r="J180" s="122"/>
-      <c r="K180" s="122"/>
-      <c r="L180" s="122"/>
+      <c r="C180" s="112"/>
+      <c r="D180" s="112"/>
+      <c r="E180" s="112"/>
+      <c r="F180" s="113"/>
+      <c r="G180" s="113"/>
+      <c r="H180" s="113"/>
+      <c r="I180" s="113"/>
+      <c r="J180" s="113"/>
+      <c r="K180" s="113"/>
+      <c r="L180" s="113"/>
     </row>
     <row r="181" spans="1:12">
       <c r="A181" s="61"/>
       <c r="B181" s="5"/>
-      <c r="C181" s="114"/>
-      <c r="D181" s="114"/>
-      <c r="E181" s="114"/>
-      <c r="F181" s="122"/>
-      <c r="G181" s="122"/>
-      <c r="H181" s="122"/>
-      <c r="I181" s="122"/>
-      <c r="J181" s="122"/>
-      <c r="K181" s="122"/>
-      <c r="L181" s="122"/>
+      <c r="C181" s="112"/>
+      <c r="D181" s="112"/>
+      <c r="E181" s="112"/>
+      <c r="F181" s="113"/>
+      <c r="G181" s="113"/>
+      <c r="H181" s="113"/>
+      <c r="I181" s="113"/>
+      <c r="J181" s="113"/>
+      <c r="K181" s="113"/>
+      <c r="L181" s="113"/>
     </row>
     <row r="182" spans="1:12">
       <c r="A182" s="61"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="114"/>
-      <c r="D182" s="114"/>
-      <c r="E182" s="114"/>
-      <c r="F182" s="122"/>
-      <c r="G182" s="122"/>
-      <c r="H182" s="122"/>
-      <c r="I182" s="122"/>
-      <c r="J182" s="122"/>
-      <c r="K182" s="122"/>
-      <c r="L182" s="122"/>
+      <c r="C182" s="112"/>
+      <c r="D182" s="112"/>
+      <c r="E182" s="112"/>
+      <c r="F182" s="113"/>
+      <c r="G182" s="113"/>
+      <c r="H182" s="113"/>
+      <c r="I182" s="113"/>
+      <c r="J182" s="113"/>
+      <c r="K182" s="113"/>
+      <c r="L182" s="113"/>
     </row>
     <row r="183" spans="1:12">
       <c r="A183" s="61"/>
       <c r="B183" s="5"/>
-      <c r="C183" s="114"/>
-      <c r="D183" s="114"/>
-      <c r="E183" s="114"/>
-      <c r="F183" s="122"/>
-      <c r="G183" s="122"/>
-      <c r="H183" s="122"/>
-      <c r="I183" s="122"/>
-      <c r="J183" s="122"/>
-      <c r="K183" s="122"/>
-      <c r="L183" s="122"/>
+      <c r="C183" s="112"/>
+      <c r="D183" s="112"/>
+      <c r="E183" s="112"/>
+      <c r="F183" s="113"/>
+      <c r="G183" s="113"/>
+      <c r="H183" s="113"/>
+      <c r="I183" s="113"/>
+      <c r="J183" s="113"/>
+      <c r="K183" s="113"/>
+      <c r="L183" s="113"/>
     </row>
     <row r="184" spans="1:12">
       <c r="A184" s="60"/>
       <c r="B184" s="16"/>
-      <c r="C184" s="114"/>
-      <c r="D184" s="114"/>
-      <c r="E184" s="114"/>
-      <c r="F184" s="122"/>
-      <c r="G184" s="122"/>
-      <c r="H184" s="122"/>
-      <c r="I184" s="122"/>
-      <c r="J184" s="122"/>
-      <c r="K184" s="122"/>
-      <c r="L184" s="122"/>
+      <c r="C184" s="112"/>
+      <c r="D184" s="112"/>
+      <c r="E184" s="112"/>
+      <c r="F184" s="113"/>
+      <c r="G184" s="113"/>
+      <c r="H184" s="113"/>
+      <c r="I184" s="113"/>
+      <c r="J184" s="113"/>
+      <c r="K184" s="113"/>
+      <c r="L184" s="113"/>
     </row>
     <row r="185" spans="1:12">
       <c r="A185" s="61"/>
       <c r="B185" s="5"/>
-      <c r="C185" s="114"/>
-      <c r="D185" s="114"/>
-      <c r="E185" s="114"/>
-      <c r="F185" s="122"/>
-      <c r="G185" s="122"/>
-      <c r="H185" s="122"/>
-      <c r="I185" s="122"/>
-      <c r="J185" s="122"/>
-      <c r="K185" s="122"/>
-      <c r="L185" s="122"/>
+      <c r="C185" s="112"/>
+      <c r="D185" s="112"/>
+      <c r="E185" s="112"/>
+      <c r="F185" s="113"/>
+      <c r="G185" s="113"/>
+      <c r="H185" s="113"/>
+      <c r="I185" s="113"/>
+      <c r="J185" s="113"/>
+      <c r="K185" s="113"/>
+      <c r="L185" s="113"/>
     </row>
     <row r="186" spans="1:12">
       <c r="A186" s="61"/>
       <c r="B186" s="5"/>
-      <c r="C186" s="114"/>
-      <c r="D186" s="114"/>
-      <c r="E186" s="114"/>
-      <c r="F186" s="122"/>
-      <c r="G186" s="122"/>
-      <c r="H186" s="122"/>
-      <c r="I186" s="122"/>
-      <c r="J186" s="122"/>
-      <c r="K186" s="122"/>
-      <c r="L186" s="122"/>
+      <c r="C186" s="112"/>
+      <c r="D186" s="112"/>
+      <c r="E186" s="112"/>
+      <c r="F186" s="113"/>
+      <c r="G186" s="113"/>
+      <c r="H186" s="113"/>
+      <c r="I186" s="113"/>
+      <c r="J186" s="113"/>
+      <c r="K186" s="113"/>
+      <c r="L186" s="113"/>
     </row>
     <row r="187" spans="1:12">
       <c r="A187" s="61"/>
       <c r="B187" s="5"/>
-      <c r="C187" s="114"/>
-      <c r="D187" s="114"/>
-      <c r="E187" s="114"/>
-      <c r="F187" s="122"/>
-      <c r="G187" s="122"/>
-      <c r="H187" s="122"/>
-      <c r="I187" s="122"/>
-      <c r="J187" s="122"/>
-      <c r="K187" s="122"/>
-      <c r="L187" s="122"/>
+      <c r="C187" s="112"/>
+      <c r="D187" s="112"/>
+      <c r="E187" s="112"/>
+      <c r="F187" s="113"/>
+      <c r="G187" s="113"/>
+      <c r="H187" s="113"/>
+      <c r="I187" s="113"/>
+      <c r="J187" s="113"/>
+      <c r="K187" s="113"/>
+      <c r="L187" s="113"/>
     </row>
     <row r="188" spans="1:12">
       <c r="A188" s="61"/>
       <c r="B188" s="5"/>
-      <c r="C188" s="114"/>
-      <c r="D188" s="114"/>
-      <c r="E188" s="114"/>
-      <c r="F188" s="122"/>
-      <c r="G188" s="122"/>
-      <c r="H188" s="122"/>
-      <c r="I188" s="122"/>
-      <c r="J188" s="122"/>
-      <c r="K188" s="122"/>
-      <c r="L188" s="122"/>
+      <c r="C188" s="112"/>
+      <c r="D188" s="112"/>
+      <c r="E188" s="112"/>
+      <c r="F188" s="113"/>
+      <c r="G188" s="113"/>
+      <c r="H188" s="113"/>
+      <c r="I188" s="113"/>
+      <c r="J188" s="113"/>
+      <c r="K188" s="113"/>
+      <c r="L188" s="113"/>
     </row>
     <row r="189" spans="1:12">
       <c r="A189" s="61"/>
       <c r="B189" s="5"/>
-      <c r="C189" s="114"/>
-      <c r="D189" s="114"/>
-      <c r="E189" s="114"/>
-      <c r="F189" s="122"/>
-      <c r="G189" s="122"/>
-      <c r="H189" s="122"/>
-      <c r="I189" s="122"/>
-      <c r="J189" s="122"/>
-      <c r="K189" s="122"/>
-      <c r="L189" s="122"/>
+      <c r="C189" s="112"/>
+      <c r="D189" s="112"/>
+      <c r="E189" s="112"/>
+      <c r="F189" s="113"/>
+      <c r="G189" s="113"/>
+      <c r="H189" s="113"/>
+      <c r="I189" s="113"/>
+      <c r="J189" s="113"/>
+      <c r="K189" s="113"/>
+      <c r="L189" s="113"/>
     </row>
     <row r="190" spans="1:12">
       <c r="A190" s="60"/>
       <c r="B190" s="16"/>
-      <c r="C190" s="114"/>
-      <c r="D190" s="114"/>
-      <c r="E190" s="114"/>
-      <c r="F190" s="122"/>
-      <c r="G190" s="122"/>
-      <c r="H190" s="122"/>
-      <c r="I190" s="122"/>
-      <c r="J190" s="122"/>
-      <c r="K190" s="122"/>
-      <c r="L190" s="122"/>
+      <c r="C190" s="112"/>
+      <c r="D190" s="112"/>
+      <c r="E190" s="112"/>
+      <c r="F190" s="113"/>
+      <c r="G190" s="113"/>
+      <c r="H190" s="113"/>
+      <c r="I190" s="113"/>
+      <c r="J190" s="113"/>
+      <c r="K190" s="113"/>
+      <c r="L190" s="113"/>
     </row>
     <row r="191" spans="1:12">
       <c r="A191" s="61"/>
       <c r="B191" s="5"/>
-      <c r="C191" s="114"/>
-      <c r="D191" s="114"/>
-      <c r="E191" s="114"/>
-      <c r="F191" s="122"/>
-      <c r="G191" s="122"/>
-      <c r="H191" s="122"/>
-      <c r="I191" s="122"/>
-      <c r="J191" s="122"/>
-      <c r="K191" s="122"/>
-      <c r="L191" s="122"/>
+      <c r="C191" s="112"/>
+      <c r="D191" s="112"/>
+      <c r="E191" s="112"/>
+      <c r="F191" s="113"/>
+      <c r="G191" s="113"/>
+      <c r="H191" s="113"/>
+      <c r="I191" s="113"/>
+      <c r="J191" s="113"/>
+      <c r="K191" s="113"/>
+      <c r="L191" s="113"/>
     </row>
     <row r="192" spans="1:12">
       <c r="A192" s="61"/>
       <c r="B192" s="5"/>
-      <c r="C192" s="114"/>
-      <c r="D192" s="114"/>
-      <c r="E192" s="114"/>
-      <c r="F192" s="122"/>
-      <c r="G192" s="122"/>
-      <c r="H192" s="122"/>
-      <c r="I192" s="122"/>
-      <c r="J192" s="122"/>
-      <c r="K192" s="122"/>
-      <c r="L192" s="122"/>
+      <c r="C192" s="112"/>
+      <c r="D192" s="112"/>
+      <c r="E192" s="112"/>
+      <c r="F192" s="113"/>
+      <c r="G192" s="113"/>
+      <c r="H192" s="113"/>
+      <c r="I192" s="113"/>
+      <c r="J192" s="113"/>
+      <c r="K192" s="113"/>
+      <c r="L192" s="113"/>
     </row>
     <row r="193" spans="1:12">
       <c r="A193" s="61"/>
       <c r="B193" s="5"/>
-      <c r="C193" s="114"/>
-      <c r="D193" s="114"/>
-      <c r="E193" s="114"/>
-      <c r="F193" s="122"/>
-      <c r="G193" s="122"/>
-      <c r="H193" s="122"/>
-      <c r="I193" s="122"/>
-      <c r="J193" s="122"/>
-      <c r="K193" s="122"/>
-      <c r="L193" s="122"/>
+      <c r="C193" s="112"/>
+      <c r="D193" s="112"/>
+      <c r="E193" s="112"/>
+      <c r="F193" s="113"/>
+      <c r="G193" s="113"/>
+      <c r="H193" s="113"/>
+      <c r="I193" s="113"/>
+      <c r="J193" s="113"/>
+      <c r="K193" s="113"/>
+      <c r="L193" s="113"/>
     </row>
     <row r="194" spans="1:12">
       <c r="A194" s="61"/>
       <c r="B194" s="5"/>
-      <c r="C194" s="114"/>
-      <c r="D194" s="114"/>
-      <c r="E194" s="114"/>
-      <c r="F194" s="122"/>
-      <c r="G194" s="122"/>
-      <c r="H194" s="122"/>
-      <c r="I194" s="122"/>
-      <c r="J194" s="122"/>
-      <c r="K194" s="122"/>
-      <c r="L194" s="122"/>
+      <c r="C194" s="112"/>
+      <c r="D194" s="112"/>
+      <c r="E194" s="112"/>
+      <c r="F194" s="113"/>
+      <c r="G194" s="113"/>
+      <c r="H194" s="113"/>
+      <c r="I194" s="113"/>
+      <c r="J194" s="113"/>
+      <c r="K194" s="113"/>
+      <c r="L194" s="113"/>
     </row>
     <row r="195" spans="1:12">
       <c r="A195" s="61"/>
       <c r="B195" s="5"/>
-      <c r="C195" s="114"/>
-      <c r="D195" s="114"/>
-      <c r="E195" s="114"/>
-      <c r="F195" s="122"/>
-      <c r="G195" s="122"/>
-      <c r="H195" s="122"/>
-      <c r="I195" s="122"/>
-      <c r="J195" s="122"/>
-      <c r="K195" s="122"/>
-      <c r="L195" s="122"/>
+      <c r="C195" s="112"/>
+      <c r="D195" s="112"/>
+      <c r="E195" s="112"/>
+      <c r="F195" s="113"/>
+      <c r="G195" s="113"/>
+      <c r="H195" s="113"/>
+      <c r="I195" s="113"/>
+      <c r="J195" s="113"/>
+      <c r="K195" s="113"/>
+      <c r="L195" s="113"/>
     </row>
     <row r="196" spans="1:12">
       <c r="A196" s="60"/>
       <c r="B196" s="16"/>
-      <c r="C196" s="114"/>
-      <c r="D196" s="114"/>
-      <c r="E196" s="114"/>
-      <c r="F196" s="122"/>
-      <c r="G196" s="122"/>
-      <c r="H196" s="122"/>
-      <c r="I196" s="122"/>
-      <c r="J196" s="122"/>
-      <c r="K196" s="122"/>
-      <c r="L196" s="122"/>
+      <c r="C196" s="112"/>
+      <c r="D196" s="112"/>
+      <c r="E196" s="112"/>
+      <c r="F196" s="113"/>
+      <c r="G196" s="113"/>
+      <c r="H196" s="113"/>
+      <c r="I196" s="113"/>
+      <c r="J196" s="113"/>
+      <c r="K196" s="113"/>
+      <c r="L196" s="113"/>
     </row>
     <row r="197" spans="1:12">
       <c r="A197" s="61"/>
       <c r="B197" s="5"/>
-      <c r="C197" s="114"/>
-      <c r="D197" s="114"/>
-      <c r="E197" s="114"/>
-      <c r="F197" s="122"/>
-      <c r="G197" s="122"/>
-      <c r="H197" s="122"/>
-      <c r="I197" s="122"/>
-      <c r="J197" s="122"/>
-      <c r="K197" s="122"/>
-      <c r="L197" s="122"/>
+      <c r="C197" s="112"/>
+      <c r="D197" s="112"/>
+      <c r="E197" s="112"/>
+      <c r="F197" s="113"/>
+      <c r="G197" s="113"/>
+      <c r="H197" s="113"/>
+      <c r="I197" s="113"/>
+      <c r="J197" s="113"/>
+      <c r="K197" s="113"/>
+      <c r="L197" s="113"/>
     </row>
     <row r="198" spans="1:12">
       <c r="A198" s="61"/>
       <c r="B198" s="5"/>
-      <c r="C198" s="114"/>
-      <c r="D198" s="114"/>
-      <c r="E198" s="114"/>
-      <c r="F198" s="122"/>
-      <c r="G198" s="122"/>
-      <c r="H198" s="122"/>
-      <c r="I198" s="122"/>
-      <c r="J198" s="122"/>
-      <c r="K198" s="122"/>
-      <c r="L198" s="122"/>
+      <c r="C198" s="112"/>
+      <c r="D198" s="112"/>
+      <c r="E198" s="112"/>
+      <c r="F198" s="113"/>
+      <c r="G198" s="113"/>
+      <c r="H198" s="113"/>
+      <c r="I198" s="113"/>
+      <c r="J198" s="113"/>
+      <c r="K198" s="113"/>
+      <c r="L198" s="113"/>
     </row>
     <row r="199" spans="1:12">
       <c r="A199" s="61"/>
       <c r="B199" s="5"/>
-      <c r="C199" s="114"/>
-      <c r="D199" s="114"/>
-      <c r="E199" s="114"/>
-      <c r="F199" s="122"/>
-      <c r="G199" s="122"/>
-      <c r="H199" s="122"/>
-      <c r="I199" s="122"/>
-      <c r="J199" s="122"/>
-      <c r="K199" s="122"/>
-      <c r="L199" s="122"/>
+      <c r="C199" s="112"/>
+      <c r="D199" s="112"/>
+      <c r="E199" s="112"/>
+      <c r="F199" s="113"/>
+      <c r="G199" s="113"/>
+      <c r="H199" s="113"/>
+      <c r="I199" s="113"/>
+      <c r="J199" s="113"/>
+      <c r="K199" s="113"/>
+      <c r="L199" s="113"/>
     </row>
     <row r="200" spans="1:12">
       <c r="A200" s="61"/>
       <c r="B200" s="5"/>
-      <c r="C200" s="114"/>
-      <c r="D200" s="114"/>
-      <c r="E200" s="114"/>
-      <c r="F200" s="122"/>
-      <c r="G200" s="122"/>
-      <c r="H200" s="122"/>
-      <c r="I200" s="122"/>
-      <c r="J200" s="122"/>
-      <c r="K200" s="122"/>
-      <c r="L200" s="122"/>
+      <c r="C200" s="112"/>
+      <c r="D200" s="112"/>
+      <c r="E200" s="112"/>
+      <c r="F200" s="113"/>
+      <c r="G200" s="113"/>
+      <c r="H200" s="113"/>
+      <c r="I200" s="113"/>
+      <c r="J200" s="113"/>
+      <c r="K200" s="113"/>
+      <c r="L200" s="113"/>
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="61"/>
       <c r="B201" s="5"/>
-      <c r="C201" s="114"/>
-      <c r="D201" s="114"/>
-      <c r="E201" s="114"/>
-      <c r="F201" s="122"/>
-      <c r="G201" s="122"/>
-      <c r="H201" s="122"/>
-      <c r="I201" s="122"/>
-      <c r="J201" s="122"/>
-      <c r="K201" s="122"/>
-      <c r="L201" s="122"/>
+      <c r="C201" s="112"/>
+      <c r="D201" s="112"/>
+      <c r="E201" s="112"/>
+      <c r="F201" s="113"/>
+      <c r="G201" s="113"/>
+      <c r="H201" s="113"/>
+      <c r="I201" s="113"/>
+      <c r="J201" s="113"/>
+      <c r="K201" s="113"/>
+      <c r="L201" s="113"/>
     </row>
     <row r="202" spans="1:12">
       <c r="A202" s="60"/>
       <c r="B202" s="16"/>
-      <c r="C202" s="114"/>
-      <c r="D202" s="114"/>
-      <c r="E202" s="114"/>
-      <c r="F202" s="122"/>
-      <c r="G202" s="122"/>
-      <c r="H202" s="122"/>
-      <c r="I202" s="122"/>
-      <c r="J202" s="122"/>
-      <c r="K202" s="122"/>
-      <c r="L202" s="122"/>
+      <c r="C202" s="112"/>
+      <c r="D202" s="112"/>
+      <c r="E202" s="112"/>
+      <c r="F202" s="113"/>
+      <c r="G202" s="113"/>
+      <c r="H202" s="113"/>
+      <c r="I202" s="113"/>
+      <c r="J202" s="113"/>
+      <c r="K202" s="113"/>
+      <c r="L202" s="113"/>
     </row>
     <row r="203" spans="1:12">
       <c r="A203" s="61"/>
       <c r="B203" s="5"/>
-      <c r="C203" s="114"/>
-      <c r="D203" s="114"/>
-      <c r="E203" s="114"/>
-      <c r="F203" s="122"/>
-      <c r="G203" s="122"/>
-      <c r="H203" s="122"/>
-      <c r="I203" s="122"/>
-      <c r="J203" s="122"/>
-      <c r="K203" s="122"/>
-      <c r="L203" s="122"/>
+      <c r="C203" s="112"/>
+      <c r="D203" s="112"/>
+      <c r="E203" s="112"/>
+      <c r="F203" s="113"/>
+      <c r="G203" s="113"/>
+      <c r="H203" s="113"/>
+      <c r="I203" s="113"/>
+      <c r="J203" s="113"/>
+      <c r="K203" s="113"/>
+      <c r="L203" s="113"/>
     </row>
     <row r="204" spans="1:12">
       <c r="A204" s="61"/>
       <c r="B204" s="5"/>
-      <c r="C204" s="114"/>
-      <c r="D204" s="114"/>
-      <c r="E204" s="114"/>
-      <c r="F204" s="122"/>
-      <c r="G204" s="122"/>
-      <c r="H204" s="122"/>
-      <c r="I204" s="122"/>
-      <c r="J204" s="122"/>
-      <c r="K204" s="122"/>
-      <c r="L204" s="122"/>
+      <c r="C204" s="112"/>
+      <c r="D204" s="112"/>
+      <c r="E204" s="112"/>
+      <c r="F204" s="113"/>
+      <c r="G204" s="113"/>
+      <c r="H204" s="113"/>
+      <c r="I204" s="113"/>
+      <c r="J204" s="113"/>
+      <c r="K204" s="113"/>
+      <c r="L204" s="113"/>
     </row>
     <row r="205" spans="1:12">
       <c r="A205" s="61"/>
@@ -11163,20 +11163,67 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="F198:L198"/>
-    <mergeCell ref="F199:L199"/>
-    <mergeCell ref="F200:L200"/>
-    <mergeCell ref="F201:L201"/>
-    <mergeCell ref="F202:L202"/>
-    <mergeCell ref="F203:L203"/>
-    <mergeCell ref="F204:L204"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C201:E201"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C166:E166"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B162:L162"/>
+    <mergeCell ref="F163:L163"/>
+    <mergeCell ref="A163:E163"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A157:L157"/>
+    <mergeCell ref="C164:E164"/>
+    <mergeCell ref="C177:E177"/>
+    <mergeCell ref="C178:E178"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="C180:E180"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="C172:E172"/>
+    <mergeCell ref="C173:E173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C175:E175"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C170:E170"/>
+    <mergeCell ref="F164:L164"/>
+    <mergeCell ref="F165:L165"/>
+    <mergeCell ref="F166:L166"/>
+    <mergeCell ref="F167:L167"/>
+    <mergeCell ref="F168:L168"/>
+    <mergeCell ref="F169:L169"/>
+    <mergeCell ref="F170:L170"/>
+    <mergeCell ref="F171:L171"/>
+    <mergeCell ref="C167:E167"/>
+    <mergeCell ref="C168:E168"/>
+    <mergeCell ref="F181:L181"/>
+    <mergeCell ref="F182:L182"/>
+    <mergeCell ref="C182:E182"/>
+    <mergeCell ref="F172:L172"/>
+    <mergeCell ref="F173:L173"/>
+    <mergeCell ref="F174:L174"/>
+    <mergeCell ref="F175:L175"/>
+    <mergeCell ref="F176:L176"/>
+    <mergeCell ref="F177:L177"/>
+    <mergeCell ref="F178:L178"/>
+    <mergeCell ref="F179:L179"/>
+    <mergeCell ref="F180:L180"/>
+    <mergeCell ref="C169:E169"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="F183:L183"/>
+    <mergeCell ref="F184:L184"/>
+    <mergeCell ref="F185:L185"/>
+    <mergeCell ref="F186:L186"/>
+    <mergeCell ref="F187:L187"/>
+    <mergeCell ref="F188:L188"/>
+    <mergeCell ref="F189:L189"/>
     <mergeCell ref="C195:E195"/>
     <mergeCell ref="C196:E196"/>
     <mergeCell ref="C197:E197"/>
@@ -11193,67 +11240,20 @@
     <mergeCell ref="C194:E194"/>
     <mergeCell ref="C185:E185"/>
     <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="F183:L183"/>
-    <mergeCell ref="F184:L184"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="F185:L185"/>
-    <mergeCell ref="F186:L186"/>
-    <mergeCell ref="F187:L187"/>
-    <mergeCell ref="F188:L188"/>
-    <mergeCell ref="F189:L189"/>
-    <mergeCell ref="F171:L171"/>
-    <mergeCell ref="C167:E167"/>
-    <mergeCell ref="C168:E168"/>
-    <mergeCell ref="F181:L181"/>
-    <mergeCell ref="F182:L182"/>
-    <mergeCell ref="C182:E182"/>
-    <mergeCell ref="F172:L172"/>
-    <mergeCell ref="F173:L173"/>
-    <mergeCell ref="F174:L174"/>
-    <mergeCell ref="F175:L175"/>
-    <mergeCell ref="F176:L176"/>
-    <mergeCell ref="F177:L177"/>
-    <mergeCell ref="F178:L178"/>
-    <mergeCell ref="F179:L179"/>
-    <mergeCell ref="F180:L180"/>
-    <mergeCell ref="C169:E169"/>
-    <mergeCell ref="C170:E170"/>
-    <mergeCell ref="F164:L164"/>
-    <mergeCell ref="F165:L165"/>
-    <mergeCell ref="F166:L166"/>
-    <mergeCell ref="F167:L167"/>
-    <mergeCell ref="F168:L168"/>
-    <mergeCell ref="F169:L169"/>
-    <mergeCell ref="F170:L170"/>
-    <mergeCell ref="C172:E172"/>
-    <mergeCell ref="C173:E173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C175:E175"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C177:E177"/>
-    <mergeCell ref="C178:E178"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="C180:E180"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C165:E165"/>
-    <mergeCell ref="C166:E166"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B162:L162"/>
-    <mergeCell ref="F163:L163"/>
-    <mergeCell ref="A163:E163"/>
-    <mergeCell ref="A161:L161"/>
-    <mergeCell ref="A157:L157"/>
-    <mergeCell ref="C164:E164"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="F198:L198"/>
+    <mergeCell ref="F199:L199"/>
+    <mergeCell ref="F200:L200"/>
+    <mergeCell ref="F201:L201"/>
+    <mergeCell ref="F202:L202"/>
+    <mergeCell ref="F203:L203"/>
+    <mergeCell ref="F204:L204"/>
+    <mergeCell ref="C199:E199"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C198:E198"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C261:E261 C237:E237 C243:E243 C249:E249 C255:E255 C225:E225 C231:E231 C213:E213 C219:E219 C207:E207" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -11283,14 +11283,14 @@
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
@@ -11316,11 +11316,11 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="118" t="s">
         <v>403</v>
       </c>
-      <c r="C2" s="115"/>
-      <c r="D2" s="115"/>
+      <c r="C2" s="118"/>
+      <c r="D2" s="118"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="18" t="s">
@@ -11825,14 +11825,14 @@
   <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="87.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
@@ -11852,10 +11852,10 @@
     </row>
     <row r="2" spans="1:3" ht="44.45" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="118" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="115"/>
+      <c r="C2" s="118"/>
     </row>
     <row r="3" spans="1:3" ht="17.45" customHeight="1">
       <c r="A3" s="47"/>

</xml_diff>

<commit_message>
revert [BUGFIX] columns not fit into one page
</commit_message>
<xml_diff>
--- a/resources/excel/specification_configurator_template.xlsx
+++ b/resources/excel/specification_configurator_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\repos\abas-specificationsconfigurator-api-web\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1E35AE8-D625-4171-8122-76BF453FE78F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BC99D77-FDE9-4021-B0DE-0D278973BFFB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41550" yWindow="3315" windowWidth="32100" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1. Firmenprofil" sheetId="1" r:id="rId1"/>
@@ -2323,24 +2323,14 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2356,6 +2346,16 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2796,13 +2796,13 @@
   <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="48.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -3133,14 +3133,14 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A61" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -3778,14 +3778,14 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:E88"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -4327,14 +4327,14 @@
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:E238"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView view="pageLayout" topLeftCell="A26" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5" style="9" customWidth="1"/>
-    <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="85.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="1"/>
     <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
@@ -6097,14 +6097,14 @@
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:C240"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
-    <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="56.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
     <col min="4" max="16384" width="11.5703125" style="1"/>
   </cols>
@@ -7445,14 +7445,14 @@
   <sheetPr codeName="Tabelle6"/>
   <dimension ref="A1:L269"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView view="pageLayout" topLeftCell="A151" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.7109375" style="59" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" style="59" customWidth="1"/>
+    <col min="2" max="2" width="32.42578125" style="59" customWidth="1"/>
     <col min="3" max="5" width="8.7109375" style="59" customWidth="1"/>
     <col min="6" max="11" width="5.28515625" style="59" customWidth="1"/>
     <col min="12" max="12" width="45.140625" style="59" customWidth="1"/>
@@ -7470,38 +7470,38 @@
       <c r="B1" s="75" t="s">
         <v>396</v>
       </c>
-      <c r="C1" s="117" t="s">
+      <c r="C1" s="113" t="s">
         <v>345</v>
       </c>
-      <c r="D1" s="117"/>
-      <c r="E1" s="117"/>
-      <c r="F1" s="116" t="s">
+      <c r="D1" s="113"/>
+      <c r="E1" s="113"/>
+      <c r="F1" s="112" t="s">
         <v>398</v>
       </c>
-      <c r="G1" s="116"/>
-      <c r="H1" s="116"/>
-      <c r="I1" s="116"/>
-      <c r="J1" s="116"/>
-      <c r="K1" s="116"/>
-      <c r="L1" s="116"/>
+      <c r="G1" s="112"/>
+      <c r="H1" s="112"/>
+      <c r="I1" s="112"/>
+      <c r="J1" s="112"/>
+      <c r="K1" s="112"/>
+      <c r="L1" s="112"/>
     </row>
     <row r="2" spans="1:12" ht="37.9" customHeight="1">
       <c r="A2" s="76"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="115" t="s">
         <v>512</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="116" t="s">
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="112" t="s">
         <v>503</v>
       </c>
-      <c r="G2" s="116"/>
-      <c r="H2" s="116"/>
-      <c r="I2" s="116"/>
-      <c r="J2" s="116"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="112"/>
     </row>
     <row r="3" spans="1:12" ht="24">
       <c r="A3" s="77" t="s">
@@ -9948,18 +9948,18 @@
       <c r="L156" s="87"/>
     </row>
     <row r="157" spans="1:12">
-      <c r="A157" s="122"/>
-      <c r="B157" s="122"/>
-      <c r="C157" s="122"/>
-      <c r="D157" s="122"/>
-      <c r="E157" s="122"/>
-      <c r="F157" s="122"/>
-      <c r="G157" s="122"/>
-      <c r="H157" s="122"/>
-      <c r="I157" s="122"/>
-      <c r="J157" s="122"/>
-      <c r="K157" s="122"/>
-      <c r="L157" s="122"/>
+      <c r="A157" s="119"/>
+      <c r="B157" s="119"/>
+      <c r="C157" s="119"/>
+      <c r="D157" s="119"/>
+      <c r="E157" s="119"/>
+      <c r="F157" s="119"/>
+      <c r="G157" s="119"/>
+      <c r="H157" s="119"/>
+      <c r="I157" s="119"/>
+      <c r="J157" s="119"/>
+      <c r="K157" s="119"/>
+      <c r="L157" s="119"/>
     </row>
     <row r="158" spans="1:12">
       <c r="A158" s="61"/>
@@ -10063,648 +10063,648 @@
       </c>
     </row>
     <row r="161" spans="1:12">
-      <c r="A161" s="121"/>
-      <c r="B161" s="121"/>
-      <c r="C161" s="121"/>
-      <c r="D161" s="121"/>
-      <c r="E161" s="121"/>
-      <c r="F161" s="121"/>
-      <c r="G161" s="121"/>
-      <c r="H161" s="121"/>
-      <c r="I161" s="121"/>
-      <c r="J161" s="121"/>
-      <c r="K161" s="121"/>
-      <c r="L161" s="121"/>
+      <c r="A161" s="118"/>
+      <c r="B161" s="118"/>
+      <c r="C161" s="118"/>
+      <c r="D161" s="118"/>
+      <c r="E161" s="118"/>
+      <c r="F161" s="118"/>
+      <c r="G161" s="118"/>
+      <c r="H161" s="118"/>
+      <c r="I161" s="118"/>
+      <c r="J161" s="118"/>
+      <c r="K161" s="118"/>
+      <c r="L161" s="118"/>
     </row>
     <row r="162" spans="1:12" ht="16.149999999999999" customHeight="1">
       <c r="A162" s="92" t="s">
         <v>130</v>
       </c>
-      <c r="B162" s="119" t="s">
+      <c r="B162" s="116" t="s">
         <v>168</v>
       </c>
-      <c r="C162" s="119"/>
-      <c r="D162" s="119"/>
-      <c r="E162" s="119"/>
-      <c r="F162" s="119"/>
-      <c r="G162" s="119"/>
-      <c r="H162" s="119"/>
-      <c r="I162" s="119"/>
-      <c r="J162" s="119"/>
-      <c r="K162" s="119"/>
-      <c r="L162" s="119"/>
+      <c r="C162" s="116"/>
+      <c r="D162" s="116"/>
+      <c r="E162" s="116"/>
+      <c r="F162" s="116"/>
+      <c r="G162" s="116"/>
+      <c r="H162" s="116"/>
+      <c r="I162" s="116"/>
+      <c r="J162" s="116"/>
+      <c r="K162" s="116"/>
+      <c r="L162" s="116"/>
     </row>
     <row r="163" spans="1:12" ht="33" customHeight="1">
-      <c r="A163" s="120"/>
-      <c r="B163" s="120"/>
-      <c r="C163" s="120"/>
-      <c r="D163" s="120"/>
-      <c r="E163" s="120"/>
-      <c r="F163" s="116" t="s">
+      <c r="A163" s="117"/>
+      <c r="B163" s="117"/>
+      <c r="C163" s="117"/>
+      <c r="D163" s="117"/>
+      <c r="E163" s="117"/>
+      <c r="F163" s="112" t="s">
         <v>501</v>
       </c>
-      <c r="G163" s="116"/>
-      <c r="H163" s="116"/>
-      <c r="I163" s="116"/>
-      <c r="J163" s="116"/>
-      <c r="K163" s="116"/>
-      <c r="L163" s="116"/>
+      <c r="G163" s="112"/>
+      <c r="H163" s="112"/>
+      <c r="I163" s="112"/>
+      <c r="J163" s="112"/>
+      <c r="K163" s="112"/>
+      <c r="L163" s="112"/>
     </row>
     <row r="164" spans="1:12">
       <c r="A164" s="61"/>
       <c r="B164" s="16" t="s">
         <v>399</v>
       </c>
-      <c r="C164" s="112"/>
-      <c r="D164" s="112"/>
-      <c r="E164" s="112"/>
-      <c r="F164" s="114"/>
-      <c r="G164" s="114"/>
-      <c r="H164" s="114"/>
-      <c r="I164" s="114"/>
-      <c r="J164" s="114"/>
-      <c r="K164" s="114"/>
-      <c r="L164" s="114"/>
+      <c r="C164" s="114"/>
+      <c r="D164" s="114"/>
+      <c r="E164" s="114"/>
+      <c r="F164" s="121"/>
+      <c r="G164" s="121"/>
+      <c r="H164" s="121"/>
+      <c r="I164" s="121"/>
+      <c r="J164" s="121"/>
+      <c r="K164" s="121"/>
+      <c r="L164" s="121"/>
     </row>
     <row r="165" spans="1:12" ht="25.5">
       <c r="A165" s="61"/>
       <c r="B165" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C165" s="112"/>
-      <c r="D165" s="112"/>
-      <c r="E165" s="112"/>
-      <c r="F165" s="114"/>
-      <c r="G165" s="114"/>
-      <c r="H165" s="114"/>
-      <c r="I165" s="114"/>
-      <c r="J165" s="114"/>
-      <c r="K165" s="114"/>
-      <c r="L165" s="114"/>
+      <c r="C165" s="114"/>
+      <c r="D165" s="114"/>
+      <c r="E165" s="114"/>
+      <c r="F165" s="121"/>
+      <c r="G165" s="121"/>
+      <c r="H165" s="121"/>
+      <c r="I165" s="121"/>
+      <c r="J165" s="121"/>
+      <c r="K165" s="121"/>
+      <c r="L165" s="121"/>
     </row>
     <row r="166" spans="1:12" ht="25.5">
       <c r="A166" s="60"/>
       <c r="B166" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C166" s="112"/>
-      <c r="D166" s="112"/>
-      <c r="E166" s="112"/>
-      <c r="F166" s="114"/>
-      <c r="G166" s="114"/>
-      <c r="H166" s="114"/>
-      <c r="I166" s="114"/>
-      <c r="J166" s="114"/>
-      <c r="K166" s="114"/>
-      <c r="L166" s="114"/>
+      <c r="C166" s="114"/>
+      <c r="D166" s="114"/>
+      <c r="E166" s="114"/>
+      <c r="F166" s="121"/>
+      <c r="G166" s="121"/>
+      <c r="H166" s="121"/>
+      <c r="I166" s="121"/>
+      <c r="J166" s="121"/>
+      <c r="K166" s="121"/>
+      <c r="L166" s="121"/>
     </row>
     <row r="167" spans="1:12" ht="14.45" customHeight="1">
       <c r="A167" s="61"/>
       <c r="B167" s="5" t="s">
         <v>400</v>
       </c>
-      <c r="C167" s="115" t="s">
-        <v>510</v>
-      </c>
-      <c r="D167" s="115"/>
-      <c r="E167" s="115"/>
-      <c r="F167" s="114"/>
-      <c r="G167" s="114"/>
-      <c r="H167" s="114"/>
-      <c r="I167" s="114"/>
-      <c r="J167" s="114"/>
-      <c r="K167" s="114"/>
-      <c r="L167" s="114"/>
+      <c r="C167" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D167" s="120"/>
+      <c r="E167" s="120"/>
+      <c r="F167" s="121"/>
+      <c r="G167" s="121"/>
+      <c r="H167" s="121"/>
+      <c r="I167" s="121"/>
+      <c r="J167" s="121"/>
+      <c r="K167" s="121"/>
+      <c r="L167" s="121"/>
     </row>
     <row r="168" spans="1:12">
       <c r="A168" s="61"/>
       <c r="B168" s="16" t="s">
         <v>322</v>
       </c>
-      <c r="C168" s="112"/>
-      <c r="D168" s="112"/>
-      <c r="E168" s="112"/>
-      <c r="F168" s="114"/>
-      <c r="G168" s="114"/>
-      <c r="H168" s="114"/>
-      <c r="I168" s="114"/>
-      <c r="J168" s="114"/>
-      <c r="K168" s="114"/>
-      <c r="L168" s="114"/>
+      <c r="C168" s="114"/>
+      <c r="D168" s="114"/>
+      <c r="E168" s="114"/>
+      <c r="F168" s="121"/>
+      <c r="G168" s="121"/>
+      <c r="H168" s="121"/>
+      <c r="I168" s="121"/>
+      <c r="J168" s="121"/>
+      <c r="K168" s="121"/>
+      <c r="L168" s="121"/>
     </row>
     <row r="169" spans="1:12" ht="25.5">
       <c r="A169" s="61"/>
       <c r="B169" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C169" s="115" t="s">
-        <v>510</v>
-      </c>
-      <c r="D169" s="115"/>
-      <c r="E169" s="115"/>
-      <c r="F169" s="114"/>
-      <c r="G169" s="114"/>
-      <c r="H169" s="114"/>
-      <c r="I169" s="114"/>
-      <c r="J169" s="114"/>
-      <c r="K169" s="114"/>
-      <c r="L169" s="114"/>
+      <c r="C169" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D169" s="120"/>
+      <c r="E169" s="120"/>
+      <c r="F169" s="121"/>
+      <c r="G169" s="121"/>
+      <c r="H169" s="121"/>
+      <c r="I169" s="121"/>
+      <c r="J169" s="121"/>
+      <c r="K169" s="121"/>
+      <c r="L169" s="121"/>
     </row>
     <row r="170" spans="1:12" ht="25.5">
       <c r="A170" s="61"/>
       <c r="B170" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C170" s="115" t="s">
-        <v>510</v>
-      </c>
-      <c r="D170" s="115"/>
-      <c r="E170" s="115"/>
-      <c r="F170" s="114"/>
-      <c r="G170" s="114"/>
-      <c r="H170" s="114"/>
-      <c r="I170" s="114"/>
-      <c r="J170" s="114"/>
-      <c r="K170" s="114"/>
-      <c r="L170" s="114"/>
+      <c r="C170" s="120" t="s">
+        <v>510</v>
+      </c>
+      <c r="D170" s="120"/>
+      <c r="E170" s="120"/>
+      <c r="F170" s="121"/>
+      <c r="G170" s="121"/>
+      <c r="H170" s="121"/>
+      <c r="I170" s="121"/>
+      <c r="J170" s="121"/>
+      <c r="K170" s="121"/>
+      <c r="L170" s="121"/>
     </row>
     <row r="171" spans="1:12" ht="25.5">
       <c r="A171" s="61"/>
       <c r="B171" s="5" t="s">
         <v>401</v>
       </c>
-      <c r="C171" s="112"/>
-      <c r="D171" s="112"/>
-      <c r="E171" s="112"/>
-      <c r="F171" s="114"/>
-      <c r="G171" s="114"/>
-      <c r="H171" s="114"/>
-      <c r="I171" s="114"/>
-      <c r="J171" s="114"/>
-      <c r="K171" s="114"/>
-      <c r="L171" s="114"/>
+      <c r="C171" s="114"/>
+      <c r="D171" s="114"/>
+      <c r="E171" s="114"/>
+      <c r="F171" s="121"/>
+      <c r="G171" s="121"/>
+      <c r="H171" s="121"/>
+      <c r="I171" s="121"/>
+      <c r="J171" s="121"/>
+      <c r="K171" s="121"/>
+      <c r="L171" s="121"/>
     </row>
     <row r="172" spans="1:12">
       <c r="A172" s="60"/>
       <c r="B172" s="16"/>
-      <c r="C172" s="112"/>
-      <c r="D172" s="112"/>
-      <c r="E172" s="112"/>
-      <c r="F172" s="113"/>
-      <c r="G172" s="113"/>
-      <c r="H172" s="113"/>
-      <c r="I172" s="113"/>
-      <c r="J172" s="113"/>
-      <c r="K172" s="113"/>
-      <c r="L172" s="113"/>
+      <c r="C172" s="114"/>
+      <c r="D172" s="114"/>
+      <c r="E172" s="114"/>
+      <c r="F172" s="122"/>
+      <c r="G172" s="122"/>
+      <c r="H172" s="122"/>
+      <c r="I172" s="122"/>
+      <c r="J172" s="122"/>
+      <c r="K172" s="122"/>
+      <c r="L172" s="122"/>
     </row>
     <row r="173" spans="1:12">
       <c r="A173" s="61"/>
       <c r="B173" s="5"/>
-      <c r="C173" s="112"/>
-      <c r="D173" s="112"/>
-      <c r="E173" s="112"/>
-      <c r="F173" s="113"/>
-      <c r="G173" s="113"/>
-      <c r="H173" s="113"/>
-      <c r="I173" s="113"/>
-      <c r="J173" s="113"/>
-      <c r="K173" s="113"/>
-      <c r="L173" s="113"/>
+      <c r="C173" s="114"/>
+      <c r="D173" s="114"/>
+      <c r="E173" s="114"/>
+      <c r="F173" s="122"/>
+      <c r="G173" s="122"/>
+      <c r="H173" s="122"/>
+      <c r="I173" s="122"/>
+      <c r="J173" s="122"/>
+      <c r="K173" s="122"/>
+      <c r="L173" s="122"/>
     </row>
     <row r="174" spans="1:12">
       <c r="A174" s="61"/>
       <c r="B174" s="5"/>
-      <c r="C174" s="112"/>
-      <c r="D174" s="112"/>
-      <c r="E174" s="112"/>
-      <c r="F174" s="113"/>
-      <c r="G174" s="113"/>
-      <c r="H174" s="113"/>
-      <c r="I174" s="113"/>
-      <c r="J174" s="113"/>
-      <c r="K174" s="113"/>
-      <c r="L174" s="113"/>
+      <c r="C174" s="114"/>
+      <c r="D174" s="114"/>
+      <c r="E174" s="114"/>
+      <c r="F174" s="122"/>
+      <c r="G174" s="122"/>
+      <c r="H174" s="122"/>
+      <c r="I174" s="122"/>
+      <c r="J174" s="122"/>
+      <c r="K174" s="122"/>
+      <c r="L174" s="122"/>
     </row>
     <row r="175" spans="1:12">
       <c r="A175" s="61"/>
       <c r="B175" s="5"/>
-      <c r="C175" s="112"/>
-      <c r="D175" s="112"/>
-      <c r="E175" s="112"/>
-      <c r="F175" s="113"/>
-      <c r="G175" s="113"/>
-      <c r="H175" s="113"/>
-      <c r="I175" s="113"/>
-      <c r="J175" s="113"/>
-      <c r="K175" s="113"/>
-      <c r="L175" s="113"/>
+      <c r="C175" s="114"/>
+      <c r="D175" s="114"/>
+      <c r="E175" s="114"/>
+      <c r="F175" s="122"/>
+      <c r="G175" s="122"/>
+      <c r="H175" s="122"/>
+      <c r="I175" s="122"/>
+      <c r="J175" s="122"/>
+      <c r="K175" s="122"/>
+      <c r="L175" s="122"/>
     </row>
     <row r="176" spans="1:12">
       <c r="A176" s="61"/>
       <c r="B176" s="5"/>
-      <c r="C176" s="112"/>
-      <c r="D176" s="112"/>
-      <c r="E176" s="112"/>
-      <c r="F176" s="113"/>
-      <c r="G176" s="113"/>
-      <c r="H176" s="113"/>
-      <c r="I176" s="113"/>
-      <c r="J176" s="113"/>
-      <c r="K176" s="113"/>
-      <c r="L176" s="113"/>
+      <c r="C176" s="114"/>
+      <c r="D176" s="114"/>
+      <c r="E176" s="114"/>
+      <c r="F176" s="122"/>
+      <c r="G176" s="122"/>
+      <c r="H176" s="122"/>
+      <c r="I176" s="122"/>
+      <c r="J176" s="122"/>
+      <c r="K176" s="122"/>
+      <c r="L176" s="122"/>
     </row>
     <row r="177" spans="1:12">
       <c r="A177" s="61"/>
       <c r="B177" s="5"/>
-      <c r="C177" s="112"/>
-      <c r="D177" s="112"/>
-      <c r="E177" s="112"/>
-      <c r="F177" s="113"/>
-      <c r="G177" s="113"/>
-      <c r="H177" s="113"/>
-      <c r="I177" s="113"/>
-      <c r="J177" s="113"/>
-      <c r="K177" s="113"/>
-      <c r="L177" s="113"/>
+      <c r="C177" s="114"/>
+      <c r="D177" s="114"/>
+      <c r="E177" s="114"/>
+      <c r="F177" s="122"/>
+      <c r="G177" s="122"/>
+      <c r="H177" s="122"/>
+      <c r="I177" s="122"/>
+      <c r="J177" s="122"/>
+      <c r="K177" s="122"/>
+      <c r="L177" s="122"/>
     </row>
     <row r="178" spans="1:12">
       <c r="A178" s="60"/>
       <c r="B178" s="16"/>
-      <c r="C178" s="112"/>
-      <c r="D178" s="112"/>
-      <c r="E178" s="112"/>
-      <c r="F178" s="113"/>
-      <c r="G178" s="113"/>
-      <c r="H178" s="113"/>
-      <c r="I178" s="113"/>
-      <c r="J178" s="113"/>
-      <c r="K178" s="113"/>
-      <c r="L178" s="113"/>
+      <c r="C178" s="114"/>
+      <c r="D178" s="114"/>
+      <c r="E178" s="114"/>
+      <c r="F178" s="122"/>
+      <c r="G178" s="122"/>
+      <c r="H178" s="122"/>
+      <c r="I178" s="122"/>
+      <c r="J178" s="122"/>
+      <c r="K178" s="122"/>
+      <c r="L178" s="122"/>
     </row>
     <row r="179" spans="1:12">
       <c r="A179" s="61"/>
       <c r="B179" s="5"/>
-      <c r="C179" s="112"/>
-      <c r="D179" s="112"/>
-      <c r="E179" s="112"/>
-      <c r="F179" s="113"/>
-      <c r="G179" s="113"/>
-      <c r="H179" s="113"/>
-      <c r="I179" s="113"/>
-      <c r="J179" s="113"/>
-      <c r="K179" s="113"/>
-      <c r="L179" s="113"/>
+      <c r="C179" s="114"/>
+      <c r="D179" s="114"/>
+      <c r="E179" s="114"/>
+      <c r="F179" s="122"/>
+      <c r="G179" s="122"/>
+      <c r="H179" s="122"/>
+      <c r="I179" s="122"/>
+      <c r="J179" s="122"/>
+      <c r="K179" s="122"/>
+      <c r="L179" s="122"/>
     </row>
     <row r="180" spans="1:12">
       <c r="A180" s="61"/>
       <c r="B180" s="5"/>
-      <c r="C180" s="112"/>
-      <c r="D180" s="112"/>
-      <c r="E180" s="112"/>
-      <c r="F180" s="113"/>
-      <c r="G180" s="113"/>
-      <c r="H180" s="113"/>
-      <c r="I180" s="113"/>
-      <c r="J180" s="113"/>
-      <c r="K180" s="113"/>
-      <c r="L180" s="113"/>
+      <c r="C180" s="114"/>
+      <c r="D180" s="114"/>
+      <c r="E180" s="114"/>
+      <c r="F180" s="122"/>
+      <c r="G180" s="122"/>
+      <c r="H180" s="122"/>
+      <c r="I180" s="122"/>
+      <c r="J180" s="122"/>
+      <c r="K180" s="122"/>
+      <c r="L180" s="122"/>
     </row>
     <row r="181" spans="1:12">
       <c r="A181" s="61"/>
       <c r="B181" s="5"/>
-      <c r="C181" s="112"/>
-      <c r="D181" s="112"/>
-      <c r="E181" s="112"/>
-      <c r="F181" s="113"/>
-      <c r="G181" s="113"/>
-      <c r="H181" s="113"/>
-      <c r="I181" s="113"/>
-      <c r="J181" s="113"/>
-      <c r="K181" s="113"/>
-      <c r="L181" s="113"/>
+      <c r="C181" s="114"/>
+      <c r="D181" s="114"/>
+      <c r="E181" s="114"/>
+      <c r="F181" s="122"/>
+      <c r="G181" s="122"/>
+      <c r="H181" s="122"/>
+      <c r="I181" s="122"/>
+      <c r="J181" s="122"/>
+      <c r="K181" s="122"/>
+      <c r="L181" s="122"/>
     </row>
     <row r="182" spans="1:12">
       <c r="A182" s="61"/>
       <c r="B182" s="5"/>
-      <c r="C182" s="112"/>
-      <c r="D182" s="112"/>
-      <c r="E182" s="112"/>
-      <c r="F182" s="113"/>
-      <c r="G182" s="113"/>
-      <c r="H182" s="113"/>
-      <c r="I182" s="113"/>
-      <c r="J182" s="113"/>
-      <c r="K182" s="113"/>
-      <c r="L182" s="113"/>
+      <c r="C182" s="114"/>
+      <c r="D182" s="114"/>
+      <c r="E182" s="114"/>
+      <c r="F182" s="122"/>
+      <c r="G182" s="122"/>
+      <c r="H182" s="122"/>
+      <c r="I182" s="122"/>
+      <c r="J182" s="122"/>
+      <c r="K182" s="122"/>
+      <c r="L182" s="122"/>
     </row>
     <row r="183" spans="1:12">
       <c r="A183" s="61"/>
       <c r="B183" s="5"/>
-      <c r="C183" s="112"/>
-      <c r="D183" s="112"/>
-      <c r="E183" s="112"/>
-      <c r="F183" s="113"/>
-      <c r="G183" s="113"/>
-      <c r="H183" s="113"/>
-      <c r="I183" s="113"/>
-      <c r="J183" s="113"/>
-      <c r="K183" s="113"/>
-      <c r="L183" s="113"/>
+      <c r="C183" s="114"/>
+      <c r="D183" s="114"/>
+      <c r="E183" s="114"/>
+      <c r="F183" s="122"/>
+      <c r="G183" s="122"/>
+      <c r="H183" s="122"/>
+      <c r="I183" s="122"/>
+      <c r="J183" s="122"/>
+      <c r="K183" s="122"/>
+      <c r="L183" s="122"/>
     </row>
     <row r="184" spans="1:12">
       <c r="A184" s="60"/>
       <c r="B184" s="16"/>
-      <c r="C184" s="112"/>
-      <c r="D184" s="112"/>
-      <c r="E184" s="112"/>
-      <c r="F184" s="113"/>
-      <c r="G184" s="113"/>
-      <c r="H184" s="113"/>
-      <c r="I184" s="113"/>
-      <c r="J184" s="113"/>
-      <c r="K184" s="113"/>
-      <c r="L184" s="113"/>
+      <c r="C184" s="114"/>
+      <c r="D184" s="114"/>
+      <c r="E184" s="114"/>
+      <c r="F184" s="122"/>
+      <c r="G184" s="122"/>
+      <c r="H184" s="122"/>
+      <c r="I184" s="122"/>
+      <c r="J184" s="122"/>
+      <c r="K184" s="122"/>
+      <c r="L184" s="122"/>
     </row>
     <row r="185" spans="1:12">
       <c r="A185" s="61"/>
       <c r="B185" s="5"/>
-      <c r="C185" s="112"/>
-      <c r="D185" s="112"/>
-      <c r="E185" s="112"/>
-      <c r="F185" s="113"/>
-      <c r="G185" s="113"/>
-      <c r="H185" s="113"/>
-      <c r="I185" s="113"/>
-      <c r="J185" s="113"/>
-      <c r="K185" s="113"/>
-      <c r="L185" s="113"/>
+      <c r="C185" s="114"/>
+      <c r="D185" s="114"/>
+      <c r="E185" s="114"/>
+      <c r="F185" s="122"/>
+      <c r="G185" s="122"/>
+      <c r="H185" s="122"/>
+      <c r="I185" s="122"/>
+      <c r="J185" s="122"/>
+      <c r="K185" s="122"/>
+      <c r="L185" s="122"/>
     </row>
     <row r="186" spans="1:12">
       <c r="A186" s="61"/>
       <c r="B186" s="5"/>
-      <c r="C186" s="112"/>
-      <c r="D186" s="112"/>
-      <c r="E186" s="112"/>
-      <c r="F186" s="113"/>
-      <c r="G186" s="113"/>
-      <c r="H186" s="113"/>
-      <c r="I186" s="113"/>
-      <c r="J186" s="113"/>
-      <c r="K186" s="113"/>
-      <c r="L186" s="113"/>
+      <c r="C186" s="114"/>
+      <c r="D186" s="114"/>
+      <c r="E186" s="114"/>
+      <c r="F186" s="122"/>
+      <c r="G186" s="122"/>
+      <c r="H186" s="122"/>
+      <c r="I186" s="122"/>
+      <c r="J186" s="122"/>
+      <c r="K186" s="122"/>
+      <c r="L186" s="122"/>
     </row>
     <row r="187" spans="1:12">
       <c r="A187" s="61"/>
       <c r="B187" s="5"/>
-      <c r="C187" s="112"/>
-      <c r="D187" s="112"/>
-      <c r="E187" s="112"/>
-      <c r="F187" s="113"/>
-      <c r="G187" s="113"/>
-      <c r="H187" s="113"/>
-      <c r="I187" s="113"/>
-      <c r="J187" s="113"/>
-      <c r="K187" s="113"/>
-      <c r="L187" s="113"/>
+      <c r="C187" s="114"/>
+      <c r="D187" s="114"/>
+      <c r="E187" s="114"/>
+      <c r="F187" s="122"/>
+      <c r="G187" s="122"/>
+      <c r="H187" s="122"/>
+      <c r="I187" s="122"/>
+      <c r="J187" s="122"/>
+      <c r="K187" s="122"/>
+      <c r="L187" s="122"/>
     </row>
     <row r="188" spans="1:12">
       <c r="A188" s="61"/>
       <c r="B188" s="5"/>
-      <c r="C188" s="112"/>
-      <c r="D188" s="112"/>
-      <c r="E188" s="112"/>
-      <c r="F188" s="113"/>
-      <c r="G188" s="113"/>
-      <c r="H188" s="113"/>
-      <c r="I188" s="113"/>
-      <c r="J188" s="113"/>
-      <c r="K188" s="113"/>
-      <c r="L188" s="113"/>
+      <c r="C188" s="114"/>
+      <c r="D188" s="114"/>
+      <c r="E188" s="114"/>
+      <c r="F188" s="122"/>
+      <c r="G188" s="122"/>
+      <c r="H188" s="122"/>
+      <c r="I188" s="122"/>
+      <c r="J188" s="122"/>
+      <c r="K188" s="122"/>
+      <c r="L188" s="122"/>
     </row>
     <row r="189" spans="1:12">
       <c r="A189" s="61"/>
       <c r="B189" s="5"/>
-      <c r="C189" s="112"/>
-      <c r="D189" s="112"/>
-      <c r="E189" s="112"/>
-      <c r="F189" s="113"/>
-      <c r="G189" s="113"/>
-      <c r="H189" s="113"/>
-      <c r="I189" s="113"/>
-      <c r="J189" s="113"/>
-      <c r="K189" s="113"/>
-      <c r="L189" s="113"/>
+      <c r="C189" s="114"/>
+      <c r="D189" s="114"/>
+      <c r="E189" s="114"/>
+      <c r="F189" s="122"/>
+      <c r="G189" s="122"/>
+      <c r="H189" s="122"/>
+      <c r="I189" s="122"/>
+      <c r="J189" s="122"/>
+      <c r="K189" s="122"/>
+      <c r="L189" s="122"/>
     </row>
     <row r="190" spans="1:12">
       <c r="A190" s="60"/>
       <c r="B190" s="16"/>
-      <c r="C190" s="112"/>
-      <c r="D190" s="112"/>
-      <c r="E190" s="112"/>
-      <c r="F190" s="113"/>
-      <c r="G190" s="113"/>
-      <c r="H190" s="113"/>
-      <c r="I190" s="113"/>
-      <c r="J190" s="113"/>
-      <c r="K190" s="113"/>
-      <c r="L190" s="113"/>
+      <c r="C190" s="114"/>
+      <c r="D190" s="114"/>
+      <c r="E190" s="114"/>
+      <c r="F190" s="122"/>
+      <c r="G190" s="122"/>
+      <c r="H190" s="122"/>
+      <c r="I190" s="122"/>
+      <c r="J190" s="122"/>
+      <c r="K190" s="122"/>
+      <c r="L190" s="122"/>
     </row>
     <row r="191" spans="1:12">
       <c r="A191" s="61"/>
       <c r="B191" s="5"/>
-      <c r="C191" s="112"/>
-      <c r="D191" s="112"/>
-      <c r="E191" s="112"/>
-      <c r="F191" s="113"/>
-      <c r="G191" s="113"/>
-      <c r="H191" s="113"/>
-      <c r="I191" s="113"/>
-      <c r="J191" s="113"/>
-      <c r="K191" s="113"/>
-      <c r="L191" s="113"/>
+      <c r="C191" s="114"/>
+      <c r="D191" s="114"/>
+      <c r="E191" s="114"/>
+      <c r="F191" s="122"/>
+      <c r="G191" s="122"/>
+      <c r="H191" s="122"/>
+      <c r="I191" s="122"/>
+      <c r="J191" s="122"/>
+      <c r="K191" s="122"/>
+      <c r="L191" s="122"/>
     </row>
     <row r="192" spans="1:12">
       <c r="A192" s="61"/>
       <c r="B192" s="5"/>
-      <c r="C192" s="112"/>
-      <c r="D192" s="112"/>
-      <c r="E192" s="112"/>
-      <c r="F192" s="113"/>
-      <c r="G192" s="113"/>
-      <c r="H192" s="113"/>
-      <c r="I192" s="113"/>
-      <c r="J192" s="113"/>
-      <c r="K192" s="113"/>
-      <c r="L192" s="113"/>
+      <c r="C192" s="114"/>
+      <c r="D192" s="114"/>
+      <c r="E192" s="114"/>
+      <c r="F192" s="122"/>
+      <c r="G192" s="122"/>
+      <c r="H192" s="122"/>
+      <c r="I192" s="122"/>
+      <c r="J192" s="122"/>
+      <c r="K192" s="122"/>
+      <c r="L192" s="122"/>
     </row>
     <row r="193" spans="1:12">
       <c r="A193" s="61"/>
       <c r="B193" s="5"/>
-      <c r="C193" s="112"/>
-      <c r="D193" s="112"/>
-      <c r="E193" s="112"/>
-      <c r="F193" s="113"/>
-      <c r="G193" s="113"/>
-      <c r="H193" s="113"/>
-      <c r="I193" s="113"/>
-      <c r="J193" s="113"/>
-      <c r="K193" s="113"/>
-      <c r="L193" s="113"/>
+      <c r="C193" s="114"/>
+      <c r="D193" s="114"/>
+      <c r="E193" s="114"/>
+      <c r="F193" s="122"/>
+      <c r="G193" s="122"/>
+      <c r="H193" s="122"/>
+      <c r="I193" s="122"/>
+      <c r="J193" s="122"/>
+      <c r="K193" s="122"/>
+      <c r="L193" s="122"/>
     </row>
     <row r="194" spans="1:12">
       <c r="A194" s="61"/>
       <c r="B194" s="5"/>
-      <c r="C194" s="112"/>
-      <c r="D194" s="112"/>
-      <c r="E194" s="112"/>
-      <c r="F194" s="113"/>
-      <c r="G194" s="113"/>
-      <c r="H194" s="113"/>
-      <c r="I194" s="113"/>
-      <c r="J194" s="113"/>
-      <c r="K194" s="113"/>
-      <c r="L194" s="113"/>
+      <c r="C194" s="114"/>
+      <c r="D194" s="114"/>
+      <c r="E194" s="114"/>
+      <c r="F194" s="122"/>
+      <c r="G194" s="122"/>
+      <c r="H194" s="122"/>
+      <c r="I194" s="122"/>
+      <c r="J194" s="122"/>
+      <c r="K194" s="122"/>
+      <c r="L194" s="122"/>
     </row>
     <row r="195" spans="1:12">
       <c r="A195" s="61"/>
       <c r="B195" s="5"/>
-      <c r="C195" s="112"/>
-      <c r="D195" s="112"/>
-      <c r="E195" s="112"/>
-      <c r="F195" s="113"/>
-      <c r="G195" s="113"/>
-      <c r="H195" s="113"/>
-      <c r="I195" s="113"/>
-      <c r="J195" s="113"/>
-      <c r="K195" s="113"/>
-      <c r="L195" s="113"/>
+      <c r="C195" s="114"/>
+      <c r="D195" s="114"/>
+      <c r="E195" s="114"/>
+      <c r="F195" s="122"/>
+      <c r="G195" s="122"/>
+      <c r="H195" s="122"/>
+      <c r="I195" s="122"/>
+      <c r="J195" s="122"/>
+      <c r="K195" s="122"/>
+      <c r="L195" s="122"/>
     </row>
     <row r="196" spans="1:12">
       <c r="A196" s="60"/>
       <c r="B196" s="16"/>
-      <c r="C196" s="112"/>
-      <c r="D196" s="112"/>
-      <c r="E196" s="112"/>
-      <c r="F196" s="113"/>
-      <c r="G196" s="113"/>
-      <c r="H196" s="113"/>
-      <c r="I196" s="113"/>
-      <c r="J196" s="113"/>
-      <c r="K196" s="113"/>
-      <c r="L196" s="113"/>
+      <c r="C196" s="114"/>
+      <c r="D196" s="114"/>
+      <c r="E196" s="114"/>
+      <c r="F196" s="122"/>
+      <c r="G196" s="122"/>
+      <c r="H196" s="122"/>
+      <c r="I196" s="122"/>
+      <c r="J196" s="122"/>
+      <c r="K196" s="122"/>
+      <c r="L196" s="122"/>
     </row>
     <row r="197" spans="1:12">
       <c r="A197" s="61"/>
       <c r="B197" s="5"/>
-      <c r="C197" s="112"/>
-      <c r="D197" s="112"/>
-      <c r="E197" s="112"/>
-      <c r="F197" s="113"/>
-      <c r="G197" s="113"/>
-      <c r="H197" s="113"/>
-      <c r="I197" s="113"/>
-      <c r="J197" s="113"/>
-      <c r="K197" s="113"/>
-      <c r="L197" s="113"/>
+      <c r="C197" s="114"/>
+      <c r="D197" s="114"/>
+      <c r="E197" s="114"/>
+      <c r="F197" s="122"/>
+      <c r="G197" s="122"/>
+      <c r="H197" s="122"/>
+      <c r="I197" s="122"/>
+      <c r="J197" s="122"/>
+      <c r="K197" s="122"/>
+      <c r="L197" s="122"/>
     </row>
     <row r="198" spans="1:12">
       <c r="A198" s="61"/>
       <c r="B198" s="5"/>
-      <c r="C198" s="112"/>
-      <c r="D198" s="112"/>
-      <c r="E198" s="112"/>
-      <c r="F198" s="113"/>
-      <c r="G198" s="113"/>
-      <c r="H198" s="113"/>
-      <c r="I198" s="113"/>
-      <c r="J198" s="113"/>
-      <c r="K198" s="113"/>
-      <c r="L198" s="113"/>
+      <c r="C198" s="114"/>
+      <c r="D198" s="114"/>
+      <c r="E198" s="114"/>
+      <c r="F198" s="122"/>
+      <c r="G198" s="122"/>
+      <c r="H198" s="122"/>
+      <c r="I198" s="122"/>
+      <c r="J198" s="122"/>
+      <c r="K198" s="122"/>
+      <c r="L198" s="122"/>
     </row>
     <row r="199" spans="1:12">
       <c r="A199" s="61"/>
       <c r="B199" s="5"/>
-      <c r="C199" s="112"/>
-      <c r="D199" s="112"/>
-      <c r="E199" s="112"/>
-      <c r="F199" s="113"/>
-      <c r="G199" s="113"/>
-      <c r="H199" s="113"/>
-      <c r="I199" s="113"/>
-      <c r="J199" s="113"/>
-      <c r="K199" s="113"/>
-      <c r="L199" s="113"/>
+      <c r="C199" s="114"/>
+      <c r="D199" s="114"/>
+      <c r="E199" s="114"/>
+      <c r="F199" s="122"/>
+      <c r="G199" s="122"/>
+      <c r="H199" s="122"/>
+      <c r="I199" s="122"/>
+      <c r="J199" s="122"/>
+      <c r="K199" s="122"/>
+      <c r="L199" s="122"/>
     </row>
     <row r="200" spans="1:12">
       <c r="A200" s="61"/>
       <c r="B200" s="5"/>
-      <c r="C200" s="112"/>
-      <c r="D200" s="112"/>
-      <c r="E200" s="112"/>
-      <c r="F200" s="113"/>
-      <c r="G200" s="113"/>
-      <c r="H200" s="113"/>
-      <c r="I200" s="113"/>
-      <c r="J200" s="113"/>
-      <c r="K200" s="113"/>
-      <c r="L200" s="113"/>
+      <c r="C200" s="114"/>
+      <c r="D200" s="114"/>
+      <c r="E200" s="114"/>
+      <c r="F200" s="122"/>
+      <c r="G200" s="122"/>
+      <c r="H200" s="122"/>
+      <c r="I200" s="122"/>
+      <c r="J200" s="122"/>
+      <c r="K200" s="122"/>
+      <c r="L200" s="122"/>
     </row>
     <row r="201" spans="1:12">
       <c r="A201" s="61"/>
       <c r="B201" s="5"/>
-      <c r="C201" s="112"/>
-      <c r="D201" s="112"/>
-      <c r="E201" s="112"/>
-      <c r="F201" s="113"/>
-      <c r="G201" s="113"/>
-      <c r="H201" s="113"/>
-      <c r="I201" s="113"/>
-      <c r="J201" s="113"/>
-      <c r="K201" s="113"/>
-      <c r="L201" s="113"/>
+      <c r="C201" s="114"/>
+      <c r="D201" s="114"/>
+      <c r="E201" s="114"/>
+      <c r="F201" s="122"/>
+      <c r="G201" s="122"/>
+      <c r="H201" s="122"/>
+      <c r="I201" s="122"/>
+      <c r="J201" s="122"/>
+      <c r="K201" s="122"/>
+      <c r="L201" s="122"/>
     </row>
     <row r="202" spans="1:12">
       <c r="A202" s="60"/>
       <c r="B202" s="16"/>
-      <c r="C202" s="112"/>
-      <c r="D202" s="112"/>
-      <c r="E202" s="112"/>
-      <c r="F202" s="113"/>
-      <c r="G202" s="113"/>
-      <c r="H202" s="113"/>
-      <c r="I202" s="113"/>
-      <c r="J202" s="113"/>
-      <c r="K202" s="113"/>
-      <c r="L202" s="113"/>
+      <c r="C202" s="114"/>
+      <c r="D202" s="114"/>
+      <c r="E202" s="114"/>
+      <c r="F202" s="122"/>
+      <c r="G202" s="122"/>
+      <c r="H202" s="122"/>
+      <c r="I202" s="122"/>
+      <c r="J202" s="122"/>
+      <c r="K202" s="122"/>
+      <c r="L202" s="122"/>
     </row>
     <row r="203" spans="1:12">
       <c r="A203" s="61"/>
       <c r="B203" s="5"/>
-      <c r="C203" s="112"/>
-      <c r="D203" s="112"/>
-      <c r="E203" s="112"/>
-      <c r="F203" s="113"/>
-      <c r="G203" s="113"/>
-      <c r="H203" s="113"/>
-      <c r="I203" s="113"/>
-      <c r="J203" s="113"/>
-      <c r="K203" s="113"/>
-      <c r="L203" s="113"/>
+      <c r="C203" s="114"/>
+      <c r="D203" s="114"/>
+      <c r="E203" s="114"/>
+      <c r="F203" s="122"/>
+      <c r="G203" s="122"/>
+      <c r="H203" s="122"/>
+      <c r="I203" s="122"/>
+      <c r="J203" s="122"/>
+      <c r="K203" s="122"/>
+      <c r="L203" s="122"/>
     </row>
     <row r="204" spans="1:12">
       <c r="A204" s="61"/>
       <c r="B204" s="5"/>
-      <c r="C204" s="112"/>
-      <c r="D204" s="112"/>
-      <c r="E204" s="112"/>
-      <c r="F204" s="113"/>
-      <c r="G204" s="113"/>
-      <c r="H204" s="113"/>
-      <c r="I204" s="113"/>
-      <c r="J204" s="113"/>
-      <c r="K204" s="113"/>
-      <c r="L204" s="113"/>
+      <c r="C204" s="114"/>
+      <c r="D204" s="114"/>
+      <c r="E204" s="114"/>
+      <c r="F204" s="122"/>
+      <c r="G204" s="122"/>
+      <c r="H204" s="122"/>
+      <c r="I204" s="122"/>
+      <c r="J204" s="122"/>
+      <c r="K204" s="122"/>
+      <c r="L204" s="122"/>
     </row>
     <row r="205" spans="1:12">
       <c r="A205" s="61"/>
@@ -11163,36 +11163,51 @@
     </row>
   </sheetData>
   <mergeCells count="91">
-    <mergeCell ref="F1:L1"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="C165:E165"/>
-    <mergeCell ref="C166:E166"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B162:L162"/>
-    <mergeCell ref="F163:L163"/>
-    <mergeCell ref="A163:E163"/>
-    <mergeCell ref="A161:L161"/>
-    <mergeCell ref="A157:L157"/>
-    <mergeCell ref="C164:E164"/>
-    <mergeCell ref="C177:E177"/>
-    <mergeCell ref="C178:E178"/>
-    <mergeCell ref="C179:E179"/>
-    <mergeCell ref="C180:E180"/>
-    <mergeCell ref="C181:E181"/>
-    <mergeCell ref="C172:E172"/>
-    <mergeCell ref="C173:E173"/>
-    <mergeCell ref="C174:E174"/>
-    <mergeCell ref="C175:E175"/>
-    <mergeCell ref="C176:E176"/>
-    <mergeCell ref="C170:E170"/>
-    <mergeCell ref="F164:L164"/>
-    <mergeCell ref="F165:L165"/>
-    <mergeCell ref="F166:L166"/>
-    <mergeCell ref="F167:L167"/>
-    <mergeCell ref="F168:L168"/>
-    <mergeCell ref="F169:L169"/>
-    <mergeCell ref="F170:L170"/>
+    <mergeCell ref="C204:E204"/>
+    <mergeCell ref="F198:L198"/>
+    <mergeCell ref="F199:L199"/>
+    <mergeCell ref="F200:L200"/>
+    <mergeCell ref="F201:L201"/>
+    <mergeCell ref="F202:L202"/>
+    <mergeCell ref="F203:L203"/>
+    <mergeCell ref="F204:L204"/>
+    <mergeCell ref="C199:E199"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C201:E201"/>
+    <mergeCell ref="C202:E202"/>
+    <mergeCell ref="C203:E203"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C195:E195"/>
+    <mergeCell ref="C196:E196"/>
+    <mergeCell ref="C197:E197"/>
+    <mergeCell ref="C171:E171"/>
+    <mergeCell ref="F195:L195"/>
+    <mergeCell ref="F196:L196"/>
+    <mergeCell ref="F197:L197"/>
+    <mergeCell ref="F190:L190"/>
+    <mergeCell ref="F191:L191"/>
+    <mergeCell ref="F192:L192"/>
+    <mergeCell ref="F193:L193"/>
+    <mergeCell ref="F194:L194"/>
+    <mergeCell ref="C193:E193"/>
+    <mergeCell ref="C194:E194"/>
+    <mergeCell ref="C185:E185"/>
+    <mergeCell ref="C186:E186"/>
+    <mergeCell ref="C187:E187"/>
+    <mergeCell ref="C188:E188"/>
+    <mergeCell ref="C189:E189"/>
+    <mergeCell ref="F183:L183"/>
+    <mergeCell ref="F184:L184"/>
+    <mergeCell ref="C190:E190"/>
+    <mergeCell ref="C191:E191"/>
+    <mergeCell ref="C192:E192"/>
+    <mergeCell ref="C183:E183"/>
+    <mergeCell ref="C184:E184"/>
+    <mergeCell ref="F185:L185"/>
+    <mergeCell ref="F186:L186"/>
+    <mergeCell ref="F187:L187"/>
+    <mergeCell ref="F188:L188"/>
+    <mergeCell ref="F189:L189"/>
     <mergeCell ref="F171:L171"/>
     <mergeCell ref="C167:E167"/>
     <mergeCell ref="C168:E168"/>
@@ -11209,51 +11224,36 @@
     <mergeCell ref="F179:L179"/>
     <mergeCell ref="F180:L180"/>
     <mergeCell ref="C169:E169"/>
-    <mergeCell ref="C190:E190"/>
-    <mergeCell ref="C191:E191"/>
-    <mergeCell ref="C192:E192"/>
-    <mergeCell ref="C183:E183"/>
-    <mergeCell ref="C184:E184"/>
-    <mergeCell ref="C187:E187"/>
-    <mergeCell ref="C188:E188"/>
-    <mergeCell ref="C189:E189"/>
-    <mergeCell ref="F183:L183"/>
-    <mergeCell ref="F184:L184"/>
-    <mergeCell ref="F185:L185"/>
-    <mergeCell ref="F186:L186"/>
-    <mergeCell ref="F187:L187"/>
-    <mergeCell ref="F188:L188"/>
-    <mergeCell ref="F189:L189"/>
-    <mergeCell ref="C195:E195"/>
-    <mergeCell ref="C196:E196"/>
-    <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C171:E171"/>
-    <mergeCell ref="F195:L195"/>
-    <mergeCell ref="F196:L196"/>
-    <mergeCell ref="F197:L197"/>
-    <mergeCell ref="F190:L190"/>
-    <mergeCell ref="F191:L191"/>
-    <mergeCell ref="F192:L192"/>
-    <mergeCell ref="F193:L193"/>
-    <mergeCell ref="F194:L194"/>
-    <mergeCell ref="C193:E193"/>
-    <mergeCell ref="C194:E194"/>
-    <mergeCell ref="C185:E185"/>
-    <mergeCell ref="C186:E186"/>
-    <mergeCell ref="C204:E204"/>
-    <mergeCell ref="F198:L198"/>
-    <mergeCell ref="F199:L199"/>
-    <mergeCell ref="F200:L200"/>
-    <mergeCell ref="F201:L201"/>
-    <mergeCell ref="F202:L202"/>
-    <mergeCell ref="F203:L203"/>
-    <mergeCell ref="F204:L204"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C201:E201"/>
-    <mergeCell ref="C202:E202"/>
-    <mergeCell ref="C203:E203"/>
-    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C170:E170"/>
+    <mergeCell ref="F164:L164"/>
+    <mergeCell ref="F165:L165"/>
+    <mergeCell ref="F166:L166"/>
+    <mergeCell ref="F167:L167"/>
+    <mergeCell ref="F168:L168"/>
+    <mergeCell ref="F169:L169"/>
+    <mergeCell ref="F170:L170"/>
+    <mergeCell ref="C172:E172"/>
+    <mergeCell ref="C173:E173"/>
+    <mergeCell ref="C174:E174"/>
+    <mergeCell ref="C175:E175"/>
+    <mergeCell ref="C176:E176"/>
+    <mergeCell ref="C177:E177"/>
+    <mergeCell ref="C178:E178"/>
+    <mergeCell ref="C179:E179"/>
+    <mergeCell ref="C180:E180"/>
+    <mergeCell ref="C181:E181"/>
+    <mergeCell ref="F1:L1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C165:E165"/>
+    <mergeCell ref="C166:E166"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B162:L162"/>
+    <mergeCell ref="F163:L163"/>
+    <mergeCell ref="A163:E163"/>
+    <mergeCell ref="A161:L161"/>
+    <mergeCell ref="A157:L157"/>
+    <mergeCell ref="C164:E164"/>
   </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C261:E261 C237:E237 C243:E243 C249:E249 C255:E255 C225:E225 C231:E231 C213:E213 C219:E219 C207:E207" xr:uid="{00000000-0002-0000-0500-000000000000}">
@@ -11283,14 +11283,14 @@
   <sheetPr codeName="Tabelle7"/>
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
@@ -11316,11 +11316,11 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="115" t="s">
         <v>403</v>
       </c>
-      <c r="C2" s="118"/>
-      <c r="D2" s="118"/>
+      <c r="C2" s="115"/>
+      <c r="D2" s="115"/>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="18" t="s">
@@ -11825,14 +11825,14 @@
   <sheetPr codeName="Tabelle8"/>
   <dimension ref="A1:C83"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="87.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1"/>
@@ -11852,10 +11852,10 @@
     </row>
     <row r="2" spans="1:3" ht="44.45" customHeight="1">
       <c r="A2" s="10"/>
-      <c r="B2" s="118" t="s">
+      <c r="B2" s="115" t="s">
         <v>451</v>
       </c>
-      <c r="C2" s="118"/>
+      <c r="C2" s="115"/>
     </row>
     <row r="3" spans="1:3" ht="17.45" customHeight="1">
       <c r="A3" s="47"/>

</xml_diff>

<commit_message>
[BUGFIX] remove empty pages from excel template
</commit_message>
<xml_diff>
--- a/resources/excel/specification_configurator_template.xlsx
+++ b/resources/excel/specification_configurator_template.xlsx
@@ -2804,13 +2804,6 @@
     <col min="1" max="1" width="12.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="44.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="81.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1"/>
-    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1"/>
-    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -2928,7 +2921,6 @@
         <v>377</v>
       </c>
       <c r="C16" s="7"/>
-      <c r="E16" s="3"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="8"/>
@@ -2936,7 +2928,6 @@
         <v>378</v>
       </c>
       <c r="C17" s="7"/>
-      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="8"/>
@@ -2944,7 +2935,6 @@
         <v>379</v>
       </c>
       <c r="C18" s="7"/>
-      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="8"/>
@@ -2952,7 +2942,6 @@
         <v>0</v>
       </c>
       <c r="C19" s="7"/>
-      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="8"/>
@@ -2960,7 +2949,6 @@
         <v>1</v>
       </c>
       <c r="C20" s="7"/>
-      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="8"/>
@@ -2970,7 +2958,6 @@
       <c r="C21" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="8"/>
@@ -2978,7 +2965,6 @@
         <v>375</v>
       </c>
       <c r="C22" s="7"/>
-      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="8"/>
@@ -2986,7 +2972,6 @@
         <v>380</v>
       </c>
       <c r="C23" s="7"/>
-      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="8"/>
@@ -2994,7 +2979,6 @@
         <v>3</v>
       </c>
       <c r="C24" s="7"/>
-      <c r="E24" s="3"/>
     </row>
     <row r="25" spans="1:5" ht="49.9" customHeight="1">
       <c r="A25" s="8"/>
@@ -3002,7 +2986,6 @@
         <v>511</v>
       </c>
       <c r="C25" s="7"/>
-      <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="18" t="s">
@@ -3036,13 +3019,11 @@
       <c r="B30" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5">
       <c r="B31" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="18" t="s">
@@ -3057,52 +3038,16 @@
       <c r="B33" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E33" s="3"/>
     </row>
     <row r="34" spans="2:5">
       <c r="B34" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="2:5">
       <c r="B35" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="E35" s="3"/>
-    </row>
-    <row r="57" spans="2:2">
-      <c r="B57" s="67"/>
-    </row>
-    <row r="58" spans="2:2">
-      <c r="B58" s="67"/>
-    </row>
-    <row r="59" spans="2:2">
-      <c r="B59" s="67"/>
-    </row>
-    <row r="60" spans="2:2">
-      <c r="B60" s="67"/>
-    </row>
-    <row r="61" spans="2:2">
-      <c r="B61" s="67"/>
-    </row>
-    <row r="62" spans="2:2">
-      <c r="B62" s="67"/>
-    </row>
-    <row r="63" spans="2:2">
-      <c r="B63" s="67"/>
-    </row>
-    <row r="64" spans="2:2">
-      <c r="B64" s="67"/>
-    </row>
-    <row r="65" spans="2:2">
-      <c r="B65" s="67"/>
-    </row>
-    <row r="66" spans="2:2">
-      <c r="B66" s="67"/>
-    </row>
-    <row r="67" spans="2:2">
-      <c r="B67" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3142,13 +3087,6 @@
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1"/>
-    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1"/>
-    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3186,7 +3124,6 @@
       <c r="C4" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8"/>
@@ -3196,7 +3133,6 @@
       <c r="C5" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8"/>
@@ -3206,7 +3142,6 @@
       <c r="C6" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="8"/>
@@ -3216,7 +3151,6 @@
       <c r="C7" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="8"/>
@@ -3226,7 +3160,6 @@
       <c r="C8" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="8"/>
@@ -3236,7 +3169,6 @@
       <c r="C9" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8"/>
@@ -3246,7 +3178,6 @@
       <c r="C10" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8"/>
@@ -3256,7 +3187,6 @@
       <c r="C11" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="8"/>
@@ -3266,7 +3196,6 @@
       <c r="C12" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8"/>
@@ -3276,7 +3205,6 @@
       <c r="C13" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="18" t="s">
@@ -3313,7 +3241,6 @@
       <c r="C17" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="23"/>
@@ -3323,7 +3250,6 @@
       <c r="C18" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="15"/>
@@ -3342,7 +3268,6 @@
       <c r="C20" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="23"/>
@@ -3352,7 +3277,6 @@
       <c r="C21" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E21" s="3"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="23"/>
@@ -3362,7 +3286,6 @@
       <c r="C22" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E22" s="3"/>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="23"/>
@@ -3787,13 +3710,6 @@
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="48.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="80.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1"/>
-    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1"/>
-    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -3829,7 +3745,6 @@
         <v>151</v>
       </c>
       <c r="C4" s="7"/>
-      <c r="E4" s="3"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="8"/>
@@ -3837,7 +3752,6 @@
         <v>152</v>
       </c>
       <c r="C5" s="7"/>
-      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="8"/>
@@ -3845,7 +3759,6 @@
         <v>153</v>
       </c>
       <c r="C6" s="7"/>
-      <c r="E6" s="3"/>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="18" t="s">
@@ -3855,7 +3768,6 @@
         <v>148</v>
       </c>
       <c r="C7" s="20"/>
-      <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="8"/>
@@ -3863,7 +3775,6 @@
         <v>157</v>
       </c>
       <c r="C8" s="7"/>
-      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:5" ht="25.5">
       <c r="A9" s="8"/>
@@ -3871,7 +3782,6 @@
         <v>158</v>
       </c>
       <c r="C9" s="7"/>
-      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="8"/>
@@ -3879,7 +3789,6 @@
         <v>159</v>
       </c>
       <c r="C10" s="7"/>
-      <c r="E10" s="3"/>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="8"/>
@@ -3887,7 +3796,6 @@
         <v>160</v>
       </c>
       <c r="C11" s="7"/>
-      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="18" t="s">
@@ -3897,7 +3805,6 @@
         <v>149</v>
       </c>
       <c r="C12" s="20"/>
-      <c r="E12" s="3"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="8"/>
@@ -3905,7 +3812,6 @@
         <v>161</v>
       </c>
       <c r="C13" s="7"/>
-      <c r="E13" s="3"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="1"/>
@@ -3937,7 +3843,6 @@
       <c r="C17" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E17" s="3"/>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="23"/>
@@ -3945,7 +3850,6 @@
         <v>395</v>
       </c>
       <c r="C18" s="24"/>
-      <c r="E18" s="3"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="23"/>
@@ -3955,7 +3859,6 @@
       <c r="C19" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E19" s="3"/>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="23"/>
@@ -3963,7 +3866,6 @@
         <v>395</v>
       </c>
       <c r="C20" s="24"/>
-      <c r="E20" s="3"/>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="15"/>
@@ -3989,7 +3891,6 @@
       <c r="C23" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E23" s="3"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="23"/>
@@ -3997,312 +3898,6 @@
         <v>395</v>
       </c>
       <c r="C24" s="24"/>
-      <c r="E24" s="3"/>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="23"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="24"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="23"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="24"/>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="B27" s="5"/>
-    </row>
-    <row r="28" spans="1:5">
-      <c r="B28" s="5"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="B29" s="5"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="B30" s="5"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="B31" s="5"/>
-    </row>
-    <row r="32" spans="1:5">
-      <c r="B32" s="5"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="B33" s="5"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="B34" s="5"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="24"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="17"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="24"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="24"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="23"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="24"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="24"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="24"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="25"/>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="25"/>
-      <c r="C45" s="24"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="15"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="26"/>
-      <c r="C47" s="24"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="26"/>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="26"/>
-      <c r="C49" s="24"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="26"/>
-      <c r="C50" s="24"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="26"/>
-      <c r="C51" s="24"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="15"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="17"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="23"/>
-      <c r="B54" s="26"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="26"/>
-      <c r="C55" s="24"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="23"/>
-      <c r="B56" s="26"/>
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="23"/>
-      <c r="B57" s="26"/>
-      <c r="C57" s="24"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="26"/>
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="26"/>
-      <c r="C59" s="24"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="15"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="17"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="26"/>
-      <c r="C61" s="24"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="26"/>
-      <c r="C62" s="24"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="26"/>
-      <c r="C63" s="24"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="23"/>
-      <c r="B64" s="26"/>
-      <c r="C64" s="24"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="24"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="23"/>
-      <c r="B66" s="26"/>
-      <c r="C66" s="24"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="23"/>
-      <c r="B67" s="26"/>
-      <c r="C67" s="24"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="15"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="17"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="23"/>
-      <c r="B69" s="26"/>
-      <c r="C69" s="24"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="23"/>
-      <c r="B71" s="26"/>
-      <c r="C71" s="24"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="23"/>
-      <c r="B72" s="26"/>
-      <c r="C72" s="24"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="23"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="24"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="15"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="17"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="23"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="24"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="23"/>
-      <c r="B76" s="26"/>
-      <c r="C76" s="24"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="23"/>
-      <c r="B77" s="26"/>
-      <c r="C77" s="24"/>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="23"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="23"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="23"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="23"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="23"/>
-      <c r="B82" s="24"/>
-      <c r="C82" s="24"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="23"/>
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="23"/>
-      <c r="B84" s="24"/>
-      <c r="C84" s="24"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="23"/>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="23"/>
-      <c r="B86" s="24"/>
-      <c r="C86" s="24"/>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="23"/>
-      <c r="B87" s="24"/>
-      <c r="C87" s="24"/>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="23"/>
-      <c r="B88" s="24"/>
-      <c r="C88" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4336,16 +3931,9 @@
     <col min="1" max="1" width="5" style="9" customWidth="1"/>
     <col min="2" max="2" width="48.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="85.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" style="1"/>
-    <col min="5" max="5" width="68.85546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5703125" style="1"/>
-    <col min="8" max="8" width="47.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="34.42578125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:3">
       <c r="A1" s="11">
         <v>4</v>
       </c>
@@ -4356,14 +3944,14 @@
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:3">
       <c r="A2" s="10"/>
       <c r="B2" s="22" t="s">
         <v>363</v>
       </c>
       <c r="C2" s="34"/>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:3">
       <c r="A3" s="18" t="s">
         <v>169</v>
       </c>
@@ -4372,14 +3960,13 @@
       </c>
       <c r="C3" s="20"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:3">
       <c r="A4" s="39"/>
       <c r="B4" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="E4" s="3"/>
-    </row>
-    <row r="5" spans="1:5">
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="39"/>
       <c r="B5" s="2" t="s">
         <v>364</v>
@@ -4387,25 +3974,22 @@
       <c r="C5" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E5" s="3"/>
-    </row>
-    <row r="6" spans="1:5">
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="39"/>
       <c r="B6" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C6" s="17"/>
-      <c r="E6" s="3"/>
-    </row>
-    <row r="7" spans="1:5">
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="15"/>
       <c r="B7" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C7" s="17"/>
-      <c r="E7" s="3"/>
-    </row>
-    <row r="8" spans="1:5">
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="39"/>
       <c r="B8" s="2" t="s">
         <v>174</v>
@@ -4413,9 +3997,8 @@
       <c r="C8" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E8" s="3"/>
-    </row>
-    <row r="9" spans="1:5">
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="18" t="s">
         <v>175</v>
       </c>
@@ -4423,17 +4006,15 @@
         <v>176</v>
       </c>
       <c r="C9" s="20"/>
-      <c r="E9" s="3"/>
-    </row>
-    <row r="10" spans="1:5">
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="39"/>
       <c r="B10" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C10" s="17"/>
-      <c r="E10" s="3"/>
-    </row>
-    <row r="11" spans="1:5">
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" s="39"/>
       <c r="B11" s="2" t="s">
         <v>364</v>
@@ -4441,25 +4022,22 @@
       <c r="C11" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E11" s="3"/>
-    </row>
-    <row r="12" spans="1:5">
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" s="15"/>
       <c r="B12" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C12" s="17"/>
-      <c r="E12" s="3"/>
-    </row>
-    <row r="13" spans="1:5">
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" s="39"/>
       <c r="B13" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C13" s="17"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" s="24"/>
       <c r="B14" s="2" t="s">
         <v>174</v>
@@ -4468,7 +4046,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:3">
       <c r="A15" s="18" t="s">
         <v>177</v>
       </c>
@@ -4477,14 +4055,14 @@
       </c>
       <c r="C15" s="20"/>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:3">
       <c r="A16" s="15"/>
       <c r="B16" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C16" s="17"/>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:3">
       <c r="A17" s="23"/>
       <c r="B17" s="2" t="s">
         <v>364</v>
@@ -4492,24 +4070,22 @@
       <c r="C17" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5">
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" s="23"/>
       <c r="B18" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C18" s="24"/>
-      <c r="E18" s="3"/>
-    </row>
-    <row r="19" spans="1:5">
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" s="15"/>
       <c r="B19" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C19" s="17"/>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:3">
       <c r="A20" s="23"/>
       <c r="B20" s="2" t="s">
         <v>174</v>
@@ -4517,9 +4093,8 @@
       <c r="C20" s="66" t="s">
         <v>510</v>
       </c>
-      <c r="E20" s="3"/>
-    </row>
-    <row r="21" spans="1:5">
+    </row>
+    <row r="21" spans="1:3">
       <c r="A21" s="18" t="s">
         <v>178</v>
       </c>
@@ -4527,17 +4102,15 @@
         <v>179</v>
       </c>
       <c r="C21" s="20"/>
-      <c r="E21" s="3"/>
-    </row>
-    <row r="22" spans="1:5">
+    </row>
+    <row r="22" spans="1:3">
       <c r="A22" s="23"/>
       <c r="B22" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C22" s="24"/>
-      <c r="E22" s="3"/>
-    </row>
-    <row r="23" spans="1:5">
+    </row>
+    <row r="23" spans="1:3">
       <c r="A23" s="23"/>
       <c r="B23" s="2" t="s">
         <v>364</v>
@@ -4546,21 +4119,21 @@
         <v>510</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:3">
       <c r="A24" s="23"/>
       <c r="B24" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C24" s="24"/>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:3">
       <c r="A25" s="23"/>
       <c r="B25" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C25" s="24"/>
     </row>
-    <row r="26" spans="1:5">
+    <row r="26" spans="1:3">
       <c r="A26" s="23"/>
       <c r="B26" s="2" t="s">
         <v>174</v>
@@ -4569,7 +4142,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="27" spans="1:5">
+    <row r="27" spans="1:3">
       <c r="A27" s="18" t="s">
         <v>180</v>
       </c>
@@ -4578,14 +4151,14 @@
       </c>
       <c r="C27" s="20"/>
     </row>
-    <row r="28" spans="1:5">
+    <row r="28" spans="1:3">
       <c r="A28" s="23"/>
       <c r="B28" s="2" t="s">
         <v>171</v>
       </c>
       <c r="C28" s="24"/>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:3">
       <c r="A29" s="23"/>
       <c r="B29" s="2" t="s">
         <v>364</v>
@@ -4594,21 +4167,21 @@
         <v>510</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:3">
       <c r="A30" s="23"/>
       <c r="B30" s="2" t="s">
         <v>172</v>
       </c>
       <c r="C30" s="24"/>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:3">
       <c r="A31" s="23"/>
       <c r="B31" s="2" t="s">
         <v>173</v>
       </c>
       <c r="C31" s="24"/>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:3">
       <c r="A32" s="23"/>
       <c r="B32" s="2" t="s">
         <v>174</v>
@@ -6106,7 +5679,6 @@
     <col min="1" max="1" width="7.85546875" style="9" customWidth="1"/>
     <col min="2" max="2" width="55.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="75.7109375" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -6348,1072 +5920,6 @@
       <c r="B27" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="C27" s="17"/>
-    </row>
-    <row r="28" spans="1:3">
-      <c r="A28" s="23"/>
-      <c r="B28" s="5"/>
-      <c r="C28" s="24"/>
-    </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="23"/>
-      <c r="B29" s="5"/>
-      <c r="C29" s="24"/>
-    </row>
-    <row r="30" spans="1:3">
-      <c r="A30" s="23"/>
-      <c r="B30" s="5"/>
-      <c r="C30" s="24"/>
-    </row>
-    <row r="31" spans="1:3">
-      <c r="A31" s="23"/>
-      <c r="B31" s="5"/>
-      <c r="C31" s="24"/>
-    </row>
-    <row r="32" spans="1:3">
-      <c r="A32" s="23"/>
-      <c r="B32" s="5"/>
-      <c r="C32" s="24"/>
-    </row>
-    <row r="33" spans="1:3">
-      <c r="A33" s="15"/>
-      <c r="B33" s="16"/>
-      <c r="C33" s="17"/>
-    </row>
-    <row r="34" spans="1:3">
-      <c r="A34" s="23"/>
-      <c r="B34" s="5"/>
-      <c r="C34" s="24"/>
-    </row>
-    <row r="35" spans="1:3">
-      <c r="A35" s="23"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="24"/>
-    </row>
-    <row r="36" spans="1:3">
-      <c r="A36" s="23"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="24"/>
-    </row>
-    <row r="37" spans="1:3">
-      <c r="A37" s="23"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="24"/>
-    </row>
-    <row r="38" spans="1:3">
-      <c r="A38" s="23"/>
-      <c r="B38" s="5"/>
-      <c r="C38" s="24"/>
-    </row>
-    <row r="39" spans="1:3">
-      <c r="A39" s="15"/>
-      <c r="B39" s="16"/>
-      <c r="C39" s="17"/>
-    </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="23"/>
-      <c r="B40" s="5"/>
-      <c r="C40" s="24"/>
-    </row>
-    <row r="41" spans="1:3">
-      <c r="A41" s="23"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="24"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="23"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="17"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="15"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="24"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="24"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="23"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="24"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="15"/>
-      <c r="B50" s="5"/>
-      <c r="C50" s="17"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="17"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="23"/>
-      <c r="B52" s="5"/>
-      <c r="C52" s="24"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="23"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="23"/>
-      <c r="B54" s="5"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="24"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="23"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="15"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="17"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="24"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="23"/>
-      <c r="B60" s="5"/>
-      <c r="C60" s="24"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="5"/>
-      <c r="C61" s="24"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="24"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="15"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="17"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="23"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="24"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="15"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="17"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="23"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="24"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="23"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="24"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="23"/>
-      <c r="B68" s="5"/>
-      <c r="C68" s="24"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="15"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="17"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="15"/>
-      <c r="B71" s="5"/>
-      <c r="C71" s="17"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="23"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="24"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="23"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="24"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="23"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="24"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="15"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="17"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="23"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="24"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="23"/>
-      <c r="B77" s="5"/>
-      <c r="C77" s="24"/>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="23"/>
-      <c r="B78" s="5"/>
-      <c r="C78" s="24"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="23"/>
-      <c r="B79" s="5"/>
-      <c r="C79" s="24"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="23"/>
-      <c r="B80" s="5"/>
-      <c r="C80" s="24"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="15"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="17"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="23"/>
-      <c r="B82" s="5"/>
-      <c r="C82" s="24"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="23"/>
-      <c r="B83" s="5"/>
-      <c r="C83" s="24"/>
-    </row>
-    <row r="84" spans="1:3">
-      <c r="A84" s="23"/>
-      <c r="B84" s="5"/>
-      <c r="C84" s="24"/>
-    </row>
-    <row r="85" spans="1:3">
-      <c r="A85" s="23"/>
-      <c r="B85" s="5"/>
-      <c r="C85" s="24"/>
-    </row>
-    <row r="86" spans="1:3">
-      <c r="A86" s="23"/>
-      <c r="B86" s="5"/>
-      <c r="C86" s="24"/>
-    </row>
-    <row r="87" spans="1:3">
-      <c r="A87" s="15"/>
-      <c r="B87" s="16"/>
-      <c r="C87" s="17"/>
-    </row>
-    <row r="88" spans="1:3">
-      <c r="A88" s="23"/>
-      <c r="B88" s="5"/>
-      <c r="C88" s="24"/>
-    </row>
-    <row r="89" spans="1:3">
-      <c r="A89" s="23"/>
-      <c r="B89" s="5"/>
-      <c r="C89" s="24"/>
-    </row>
-    <row r="90" spans="1:3">
-      <c r="A90" s="23"/>
-      <c r="B90" s="5"/>
-      <c r="C90" s="24"/>
-    </row>
-    <row r="91" spans="1:3">
-      <c r="A91" s="23"/>
-      <c r="B91" s="5"/>
-      <c r="C91" s="24"/>
-    </row>
-    <row r="92" spans="1:3">
-      <c r="A92" s="23"/>
-      <c r="B92" s="5"/>
-      <c r="C92" s="24"/>
-    </row>
-    <row r="93" spans="1:3">
-      <c r="A93" s="15"/>
-      <c r="B93" s="16"/>
-      <c r="C93" s="17"/>
-    </row>
-    <row r="94" spans="1:3">
-      <c r="A94" s="23"/>
-      <c r="B94" s="5"/>
-      <c r="C94" s="24"/>
-    </row>
-    <row r="95" spans="1:3">
-      <c r="A95" s="23"/>
-      <c r="B95" s="5"/>
-      <c r="C95" s="24"/>
-    </row>
-    <row r="96" spans="1:3">
-      <c r="A96" s="23"/>
-      <c r="B96" s="5"/>
-      <c r="C96" s="24"/>
-    </row>
-    <row r="97" spans="1:3">
-      <c r="A97" s="23"/>
-      <c r="B97" s="5"/>
-      <c r="C97" s="24"/>
-    </row>
-    <row r="98" spans="1:3">
-      <c r="A98" s="23"/>
-      <c r="B98" s="5"/>
-      <c r="C98" s="24"/>
-    </row>
-    <row r="99" spans="1:3">
-      <c r="A99" s="15"/>
-      <c r="B99" s="16"/>
-      <c r="C99" s="17"/>
-    </row>
-    <row r="100" spans="1:3">
-      <c r="A100" s="23"/>
-      <c r="B100" s="5"/>
-      <c r="C100" s="24"/>
-    </row>
-    <row r="101" spans="1:3">
-      <c r="A101" s="23"/>
-      <c r="B101" s="5"/>
-      <c r="C101" s="24"/>
-    </row>
-    <row r="102" spans="1:3">
-      <c r="A102" s="23"/>
-      <c r="B102" s="5"/>
-      <c r="C102" s="24"/>
-    </row>
-    <row r="103" spans="1:3">
-      <c r="A103" s="23"/>
-      <c r="B103" s="5"/>
-      <c r="C103" s="24"/>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="A104" s="23"/>
-      <c r="B104" s="5"/>
-      <c r="C104" s="24"/>
-    </row>
-    <row r="105" spans="1:3">
-      <c r="A105" s="15"/>
-      <c r="B105" s="16"/>
-      <c r="C105" s="17"/>
-    </row>
-    <row r="106" spans="1:3">
-      <c r="A106" s="23"/>
-      <c r="B106" s="5"/>
-      <c r="C106" s="24"/>
-    </row>
-    <row r="107" spans="1:3">
-      <c r="A107" s="23"/>
-      <c r="B107" s="5"/>
-      <c r="C107" s="24"/>
-    </row>
-    <row r="108" spans="1:3">
-      <c r="A108" s="23"/>
-      <c r="B108" s="5"/>
-      <c r="C108" s="24"/>
-    </row>
-    <row r="109" spans="1:3">
-      <c r="A109" s="23"/>
-      <c r="B109" s="5"/>
-      <c r="C109" s="24"/>
-    </row>
-    <row r="110" spans="1:3">
-      <c r="A110" s="23"/>
-      <c r="B110" s="5"/>
-      <c r="C110" s="24"/>
-    </row>
-    <row r="111" spans="1:3">
-      <c r="A111" s="15"/>
-      <c r="B111" s="16"/>
-      <c r="C111" s="17"/>
-    </row>
-    <row r="112" spans="1:3">
-      <c r="A112" s="23"/>
-      <c r="B112" s="5"/>
-      <c r="C112" s="24"/>
-    </row>
-    <row r="113" spans="1:3">
-      <c r="A113" s="23"/>
-      <c r="B113" s="5"/>
-      <c r="C113" s="24"/>
-    </row>
-    <row r="114" spans="1:3">
-      <c r="A114" s="23"/>
-      <c r="B114" s="5"/>
-      <c r="C114" s="24"/>
-    </row>
-    <row r="115" spans="1:3">
-      <c r="A115" s="23"/>
-      <c r="B115" s="5"/>
-      <c r="C115" s="24"/>
-    </row>
-    <row r="116" spans="1:3">
-      <c r="A116" s="23"/>
-      <c r="B116" s="5"/>
-      <c r="C116" s="24"/>
-    </row>
-    <row r="117" spans="1:3">
-      <c r="A117" s="15"/>
-      <c r="B117" s="16"/>
-      <c r="C117" s="17"/>
-    </row>
-    <row r="118" spans="1:3">
-      <c r="A118" s="23"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="24"/>
-    </row>
-    <row r="119" spans="1:3">
-      <c r="A119" s="23"/>
-      <c r="B119" s="5"/>
-      <c r="C119" s="24"/>
-    </row>
-    <row r="120" spans="1:3">
-      <c r="A120" s="23"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="24"/>
-    </row>
-    <row r="121" spans="1:3">
-      <c r="A121" s="23"/>
-      <c r="B121" s="5"/>
-      <c r="C121" s="24"/>
-    </row>
-    <row r="122" spans="1:3">
-      <c r="A122" s="23"/>
-      <c r="B122" s="5"/>
-      <c r="C122" s="24"/>
-    </row>
-    <row r="123" spans="1:3">
-      <c r="A123" s="15"/>
-      <c r="B123" s="16"/>
-      <c r="C123" s="17"/>
-    </row>
-    <row r="124" spans="1:3">
-      <c r="A124" s="23"/>
-      <c r="B124" s="5"/>
-      <c r="C124" s="24"/>
-    </row>
-    <row r="125" spans="1:3">
-      <c r="A125" s="23"/>
-      <c r="B125" s="5"/>
-      <c r="C125" s="24"/>
-    </row>
-    <row r="126" spans="1:3">
-      <c r="A126" s="23"/>
-      <c r="B126" s="5"/>
-      <c r="C126" s="24"/>
-    </row>
-    <row r="127" spans="1:3">
-      <c r="A127" s="23"/>
-      <c r="B127" s="5"/>
-      <c r="C127" s="24"/>
-    </row>
-    <row r="128" spans="1:3">
-      <c r="A128" s="23"/>
-      <c r="B128" s="5"/>
-      <c r="C128" s="24"/>
-    </row>
-    <row r="129" spans="1:3">
-      <c r="A129" s="15"/>
-      <c r="B129" s="16"/>
-      <c r="C129" s="17"/>
-    </row>
-    <row r="130" spans="1:3">
-      <c r="A130" s="23"/>
-      <c r="B130" s="5"/>
-      <c r="C130" s="24"/>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="A131" s="23"/>
-      <c r="B131" s="5"/>
-      <c r="C131" s="24"/>
-    </row>
-    <row r="132" spans="1:3">
-      <c r="A132" s="23"/>
-      <c r="B132" s="5"/>
-      <c r="C132" s="24"/>
-    </row>
-    <row r="133" spans="1:3">
-      <c r="A133" s="23"/>
-      <c r="B133" s="5"/>
-      <c r="C133" s="24"/>
-    </row>
-    <row r="134" spans="1:3">
-      <c r="A134" s="23"/>
-      <c r="B134" s="5"/>
-      <c r="C134" s="24"/>
-    </row>
-    <row r="135" spans="1:3">
-      <c r="A135" s="15"/>
-      <c r="B135" s="16"/>
-      <c r="C135" s="17"/>
-    </row>
-    <row r="136" spans="1:3">
-      <c r="A136" s="23"/>
-      <c r="B136" s="5"/>
-      <c r="C136" s="24"/>
-    </row>
-    <row r="137" spans="1:3">
-      <c r="A137" s="23"/>
-      <c r="B137" s="5"/>
-      <c r="C137" s="24"/>
-    </row>
-    <row r="138" spans="1:3">
-      <c r="A138" s="23"/>
-      <c r="B138" s="5"/>
-      <c r="C138" s="24"/>
-    </row>
-    <row r="139" spans="1:3">
-      <c r="A139" s="23"/>
-      <c r="B139" s="5"/>
-      <c r="C139" s="24"/>
-    </row>
-    <row r="140" spans="1:3">
-      <c r="A140" s="23"/>
-      <c r="B140" s="5"/>
-      <c r="C140" s="24"/>
-    </row>
-    <row r="141" spans="1:3">
-      <c r="A141" s="15"/>
-      <c r="B141" s="16"/>
-      <c r="C141" s="17"/>
-    </row>
-    <row r="142" spans="1:3">
-      <c r="A142" s="23"/>
-      <c r="B142" s="5"/>
-      <c r="C142" s="24"/>
-    </row>
-    <row r="143" spans="1:3">
-      <c r="A143" s="23"/>
-      <c r="B143" s="5"/>
-      <c r="C143" s="24"/>
-    </row>
-    <row r="144" spans="1:3">
-      <c r="A144" s="23"/>
-      <c r="B144" s="5"/>
-      <c r="C144" s="24"/>
-    </row>
-    <row r="145" spans="1:3">
-      <c r="A145" s="23"/>
-      <c r="B145" s="5"/>
-      <c r="C145" s="24"/>
-    </row>
-    <row r="146" spans="1:3">
-      <c r="A146" s="23"/>
-      <c r="B146" s="5"/>
-      <c r="C146" s="24"/>
-    </row>
-    <row r="147" spans="1:3">
-      <c r="A147" s="15"/>
-      <c r="B147" s="16"/>
-      <c r="C147" s="17"/>
-    </row>
-    <row r="148" spans="1:3">
-      <c r="A148" s="23"/>
-      <c r="B148" s="5"/>
-      <c r="C148" s="24"/>
-    </row>
-    <row r="149" spans="1:3">
-      <c r="A149" s="23"/>
-      <c r="B149" s="5"/>
-      <c r="C149" s="24"/>
-    </row>
-    <row r="150" spans="1:3">
-      <c r="A150" s="23"/>
-      <c r="B150" s="5"/>
-      <c r="C150" s="24"/>
-    </row>
-    <row r="151" spans="1:3">
-      <c r="A151" s="23"/>
-      <c r="B151" s="5"/>
-      <c r="C151" s="24"/>
-    </row>
-    <row r="152" spans="1:3">
-      <c r="A152" s="23"/>
-      <c r="B152" s="5"/>
-      <c r="C152" s="24"/>
-    </row>
-    <row r="153" spans="1:3">
-      <c r="A153" s="15"/>
-      <c r="B153" s="16"/>
-      <c r="C153" s="17"/>
-    </row>
-    <row r="154" spans="1:3">
-      <c r="A154" s="23"/>
-      <c r="B154" s="5"/>
-      <c r="C154" s="24"/>
-    </row>
-    <row r="155" spans="1:3">
-      <c r="A155" s="23"/>
-      <c r="B155" s="5"/>
-      <c r="C155" s="24"/>
-    </row>
-    <row r="156" spans="1:3">
-      <c r="A156" s="23"/>
-      <c r="B156" s="5"/>
-      <c r="C156" s="24"/>
-    </row>
-    <row r="157" spans="1:3">
-      <c r="A157" s="23"/>
-      <c r="B157" s="5"/>
-      <c r="C157" s="24"/>
-    </row>
-    <row r="158" spans="1:3">
-      <c r="A158" s="23"/>
-      <c r="B158" s="5"/>
-      <c r="C158" s="24"/>
-    </row>
-    <row r="159" spans="1:3">
-      <c r="A159" s="15"/>
-      <c r="B159" s="16"/>
-      <c r="C159" s="17"/>
-    </row>
-    <row r="160" spans="1:3">
-      <c r="A160" s="23"/>
-      <c r="B160" s="5"/>
-      <c r="C160" s="24"/>
-    </row>
-    <row r="161" spans="1:3">
-      <c r="A161" s="23"/>
-      <c r="B161" s="5"/>
-      <c r="C161" s="24"/>
-    </row>
-    <row r="162" spans="1:3">
-      <c r="A162" s="23"/>
-      <c r="B162" s="5"/>
-      <c r="C162" s="24"/>
-    </row>
-    <row r="163" spans="1:3">
-      <c r="A163" s="23"/>
-      <c r="B163" s="5"/>
-      <c r="C163" s="24"/>
-    </row>
-    <row r="164" spans="1:3">
-      <c r="A164" s="23"/>
-      <c r="B164" s="5"/>
-      <c r="C164" s="24"/>
-    </row>
-    <row r="165" spans="1:3">
-      <c r="A165" s="15"/>
-      <c r="B165" s="16"/>
-      <c r="C165" s="17"/>
-    </row>
-    <row r="166" spans="1:3">
-      <c r="A166" s="23"/>
-      <c r="B166" s="5"/>
-      <c r="C166" s="24"/>
-    </row>
-    <row r="167" spans="1:3">
-      <c r="A167" s="23"/>
-      <c r="B167" s="5"/>
-      <c r="C167" s="24"/>
-    </row>
-    <row r="168" spans="1:3">
-      <c r="A168" s="23"/>
-      <c r="B168" s="5"/>
-      <c r="C168" s="24"/>
-    </row>
-    <row r="169" spans="1:3">
-      <c r="A169" s="23"/>
-      <c r="B169" s="5"/>
-      <c r="C169" s="24"/>
-    </row>
-    <row r="170" spans="1:3">
-      <c r="A170" s="23"/>
-      <c r="B170" s="5"/>
-      <c r="C170" s="24"/>
-    </row>
-    <row r="171" spans="1:3">
-      <c r="A171" s="15"/>
-      <c r="B171" s="16"/>
-      <c r="C171" s="17"/>
-    </row>
-    <row r="172" spans="1:3">
-      <c r="A172" s="23"/>
-      <c r="B172" s="5"/>
-      <c r="C172" s="24"/>
-    </row>
-    <row r="173" spans="1:3">
-      <c r="A173" s="23"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="24"/>
-    </row>
-    <row r="174" spans="1:3">
-      <c r="A174" s="23"/>
-      <c r="B174" s="5"/>
-      <c r="C174" s="24"/>
-    </row>
-    <row r="175" spans="1:3">
-      <c r="A175" s="23"/>
-      <c r="B175" s="5"/>
-      <c r="C175" s="24"/>
-    </row>
-    <row r="176" spans="1:3">
-      <c r="A176" s="23"/>
-      <c r="B176" s="5"/>
-      <c r="C176" s="24"/>
-    </row>
-    <row r="177" spans="1:3">
-      <c r="A177" s="15"/>
-      <c r="B177" s="16"/>
-      <c r="C177" s="17"/>
-    </row>
-    <row r="178" spans="1:3">
-      <c r="A178" s="23"/>
-      <c r="B178" s="5"/>
-      <c r="C178" s="24"/>
-    </row>
-    <row r="179" spans="1:3">
-      <c r="A179" s="23"/>
-      <c r="B179" s="5"/>
-      <c r="C179" s="24"/>
-    </row>
-    <row r="180" spans="1:3">
-      <c r="A180" s="23"/>
-      <c r="B180" s="5"/>
-      <c r="C180" s="24"/>
-    </row>
-    <row r="181" spans="1:3">
-      <c r="A181" s="23"/>
-      <c r="B181" s="5"/>
-      <c r="C181" s="24"/>
-    </row>
-    <row r="182" spans="1:3">
-      <c r="A182" s="23"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="24"/>
-    </row>
-    <row r="183" spans="1:3">
-      <c r="A183" s="15"/>
-      <c r="B183" s="16"/>
-      <c r="C183" s="17"/>
-    </row>
-    <row r="184" spans="1:3">
-      <c r="A184" s="23"/>
-      <c r="B184" s="5"/>
-      <c r="C184" s="24"/>
-    </row>
-    <row r="185" spans="1:3">
-      <c r="A185" s="23"/>
-      <c r="B185" s="5"/>
-      <c r="C185" s="24"/>
-    </row>
-    <row r="186" spans="1:3">
-      <c r="A186" s="23"/>
-      <c r="B186" s="5"/>
-      <c r="C186" s="24"/>
-    </row>
-    <row r="187" spans="1:3">
-      <c r="A187" s="23"/>
-      <c r="B187" s="5"/>
-      <c r="C187" s="24"/>
-    </row>
-    <row r="188" spans="1:3">
-      <c r="A188" s="23"/>
-      <c r="B188" s="5"/>
-      <c r="C188" s="24"/>
-    </row>
-    <row r="189" spans="1:3">
-      <c r="A189" s="15"/>
-      <c r="B189" s="16"/>
-      <c r="C189" s="17"/>
-    </row>
-    <row r="190" spans="1:3">
-      <c r="A190" s="23"/>
-      <c r="B190" s="5"/>
-      <c r="C190" s="24"/>
-    </row>
-    <row r="191" spans="1:3">
-      <c r="A191" s="23"/>
-      <c r="B191" s="5"/>
-      <c r="C191" s="24"/>
-    </row>
-    <row r="192" spans="1:3">
-      <c r="A192" s="23"/>
-      <c r="B192" s="5"/>
-      <c r="C192" s="24"/>
-    </row>
-    <row r="193" spans="1:3">
-      <c r="A193" s="23"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="24"/>
-    </row>
-    <row r="194" spans="1:3">
-      <c r="A194" s="23"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="24"/>
-    </row>
-    <row r="195" spans="1:3">
-      <c r="A195" s="15"/>
-      <c r="B195" s="16"/>
-      <c r="C195" s="17"/>
-    </row>
-    <row r="196" spans="1:3">
-      <c r="A196" s="23"/>
-      <c r="B196" s="5"/>
-      <c r="C196" s="24"/>
-    </row>
-    <row r="197" spans="1:3">
-      <c r="A197" s="23"/>
-      <c r="B197" s="5"/>
-      <c r="C197" s="24"/>
-    </row>
-    <row r="198" spans="1:3">
-      <c r="A198" s="23"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="24"/>
-    </row>
-    <row r="199" spans="1:3">
-      <c r="A199" s="23"/>
-      <c r="B199" s="5"/>
-      <c r="C199" s="24"/>
-    </row>
-    <row r="200" spans="1:3">
-      <c r="A200" s="23"/>
-      <c r="B200" s="5"/>
-      <c r="C200" s="24"/>
-    </row>
-    <row r="201" spans="1:3">
-      <c r="A201" s="15"/>
-      <c r="B201" s="16"/>
-      <c r="C201" s="17"/>
-    </row>
-    <row r="202" spans="1:3">
-      <c r="A202" s="23"/>
-      <c r="B202" s="5"/>
-      <c r="C202" s="24"/>
-    </row>
-    <row r="203" spans="1:3">
-      <c r="A203" s="23"/>
-      <c r="B203" s="5"/>
-      <c r="C203" s="24"/>
-    </row>
-    <row r="204" spans="1:3">
-      <c r="A204" s="23"/>
-      <c r="B204" s="5"/>
-      <c r="C204" s="24"/>
-    </row>
-    <row r="205" spans="1:3">
-      <c r="A205" s="23"/>
-      <c r="B205" s="5"/>
-      <c r="C205" s="24"/>
-    </row>
-    <row r="206" spans="1:3">
-      <c r="A206" s="23"/>
-      <c r="B206" s="5"/>
-      <c r="C206" s="24"/>
-    </row>
-    <row r="207" spans="1:3">
-      <c r="A207" s="15"/>
-      <c r="B207" s="16"/>
-      <c r="C207" s="17"/>
-    </row>
-    <row r="208" spans="1:3">
-      <c r="A208" s="23"/>
-      <c r="B208" s="5"/>
-      <c r="C208" s="24"/>
-    </row>
-    <row r="209" spans="1:3">
-      <c r="A209" s="23"/>
-      <c r="B209" s="5"/>
-      <c r="C209" s="24"/>
-    </row>
-    <row r="210" spans="1:3">
-      <c r="A210" s="23"/>
-      <c r="B210" s="5"/>
-      <c r="C210" s="24"/>
-    </row>
-    <row r="211" spans="1:3">
-      <c r="A211" s="23"/>
-      <c r="B211" s="5"/>
-      <c r="C211" s="24"/>
-    </row>
-    <row r="212" spans="1:3">
-      <c r="A212" s="23"/>
-      <c r="B212" s="5"/>
-      <c r="C212" s="24"/>
-    </row>
-    <row r="213" spans="1:3">
-      <c r="A213" s="15"/>
-      <c r="B213" s="16"/>
-      <c r="C213" s="17"/>
-    </row>
-    <row r="214" spans="1:3">
-      <c r="A214" s="23"/>
-      <c r="B214" s="5"/>
-      <c r="C214" s="24"/>
-    </row>
-    <row r="215" spans="1:3">
-      <c r="A215" s="23"/>
-      <c r="B215" s="5"/>
-      <c r="C215" s="24"/>
-    </row>
-    <row r="216" spans="1:3">
-      <c r="A216" s="23"/>
-      <c r="B216" s="5"/>
-      <c r="C216" s="24"/>
-    </row>
-    <row r="217" spans="1:3">
-      <c r="A217" s="23"/>
-      <c r="B217" s="5"/>
-      <c r="C217" s="24"/>
-    </row>
-    <row r="218" spans="1:3">
-      <c r="A218" s="23"/>
-      <c r="B218" s="5"/>
-      <c r="C218" s="24"/>
-    </row>
-    <row r="219" spans="1:3">
-      <c r="A219" s="15"/>
-      <c r="B219" s="16"/>
-      <c r="C219" s="17"/>
-    </row>
-    <row r="220" spans="1:3">
-      <c r="A220" s="23"/>
-      <c r="B220" s="5"/>
-      <c r="C220" s="24"/>
-    </row>
-    <row r="221" spans="1:3">
-      <c r="A221" s="23"/>
-      <c r="B221" s="5"/>
-      <c r="C221" s="24"/>
-    </row>
-    <row r="222" spans="1:3">
-      <c r="A222" s="23"/>
-      <c r="B222" s="5"/>
-      <c r="C222" s="24"/>
-    </row>
-    <row r="223" spans="1:3">
-      <c r="A223" s="23"/>
-      <c r="B223" s="5"/>
-      <c r="C223" s="24"/>
-    </row>
-    <row r="224" spans="1:3">
-      <c r="A224" s="23"/>
-      <c r="B224" s="5"/>
-      <c r="C224" s="24"/>
-    </row>
-    <row r="225" spans="1:3">
-      <c r="A225" s="15"/>
-      <c r="B225" s="16"/>
-      <c r="C225" s="17"/>
-    </row>
-    <row r="226" spans="1:3">
-      <c r="A226" s="23"/>
-      <c r="B226" s="5"/>
-      <c r="C226" s="24"/>
-    </row>
-    <row r="227" spans="1:3">
-      <c r="A227" s="23"/>
-      <c r="B227" s="5"/>
-      <c r="C227" s="24"/>
-    </row>
-    <row r="228" spans="1:3">
-      <c r="A228" s="23"/>
-      <c r="B228" s="5"/>
-      <c r="C228" s="24"/>
-    </row>
-    <row r="229" spans="1:3">
-      <c r="A229" s="23"/>
-      <c r="B229" s="5"/>
-      <c r="C229" s="24"/>
-    </row>
-    <row r="230" spans="1:3">
-      <c r="A230" s="23"/>
-      <c r="B230" s="5"/>
-      <c r="C230" s="24"/>
-    </row>
-    <row r="231" spans="1:3">
-      <c r="A231" s="15"/>
-      <c r="B231" s="16"/>
-      <c r="C231" s="17"/>
-    </row>
-    <row r="232" spans="1:3">
-      <c r="A232" s="23"/>
-      <c r="B232" s="5"/>
-      <c r="C232" s="24"/>
-    </row>
-    <row r="233" spans="1:3">
-      <c r="A233" s="23"/>
-      <c r="B233" s="5"/>
-      <c r="C233" s="24"/>
-    </row>
-    <row r="234" spans="1:3">
-      <c r="A234" s="23"/>
-      <c r="B234" s="5"/>
-      <c r="C234" s="24"/>
-    </row>
-    <row r="235" spans="1:3">
-      <c r="A235" s="23"/>
-      <c r="B235" s="5"/>
-      <c r="C235" s="24"/>
-    </row>
-    <row r="236" spans="1:3">
-      <c r="A236" s="23"/>
-      <c r="B236" s="5"/>
-      <c r="C236" s="24"/>
-    </row>
-    <row r="237" spans="1:3">
-      <c r="A237" s="15"/>
-      <c r="B237" s="16"/>
-      <c r="C237" s="17"/>
-    </row>
-    <row r="238" spans="1:3">
-      <c r="A238" s="23"/>
-      <c r="B238" s="25"/>
-      <c r="C238" s="24"/>
-    </row>
-    <row r="239" spans="1:3">
-      <c r="A239" s="23"/>
-      <c r="B239" s="24"/>
-      <c r="C239" s="24"/>
-    </row>
-    <row r="240" spans="1:3">
-      <c r="A240" s="23"/>
-      <c r="B240" s="24"/>
-      <c r="C240" s="24"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -7456,11 +5962,6 @@
     <col min="3" max="5" width="8.7109375" style="59" customWidth="1"/>
     <col min="6" max="11" width="5.28515625" style="59" customWidth="1"/>
     <col min="12" max="12" width="45.140625" style="59" customWidth="1"/>
-    <col min="13" max="13" width="28.28515625" style="59" customWidth="1"/>
-    <col min="14" max="14" width="11.5703125" style="59"/>
-    <col min="15" max="15" width="47.5703125" style="59" customWidth="1"/>
-    <col min="16" max="16" width="34.42578125" style="59" customWidth="1"/>
-    <col min="17" max="16384" width="11.5703125" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -10243,923 +8744,6 @@
       <c r="J171" s="114"/>
       <c r="K171" s="114"/>
       <c r="L171" s="114"/>
-    </row>
-    <row r="172" spans="1:12">
-      <c r="A172" s="60"/>
-      <c r="B172" s="16"/>
-      <c r="C172" s="112"/>
-      <c r="D172" s="112"/>
-      <c r="E172" s="112"/>
-      <c r="F172" s="113"/>
-      <c r="G172" s="113"/>
-      <c r="H172" s="113"/>
-      <c r="I172" s="113"/>
-      <c r="J172" s="113"/>
-      <c r="K172" s="113"/>
-      <c r="L172" s="113"/>
-    </row>
-    <row r="173" spans="1:12">
-      <c r="A173" s="61"/>
-      <c r="B173" s="5"/>
-      <c r="C173" s="112"/>
-      <c r="D173" s="112"/>
-      <c r="E173" s="112"/>
-      <c r="F173" s="113"/>
-      <c r="G173" s="113"/>
-      <c r="H173" s="113"/>
-      <c r="I173" s="113"/>
-      <c r="J173" s="113"/>
-      <c r="K173" s="113"/>
-      <c r="L173" s="113"/>
-    </row>
-    <row r="174" spans="1:12">
-      <c r="A174" s="61"/>
-      <c r="B174" s="5"/>
-      <c r="C174" s="112"/>
-      <c r="D174" s="112"/>
-      <c r="E174" s="112"/>
-      <c r="F174" s="113"/>
-      <c r="G174" s="113"/>
-      <c r="H174" s="113"/>
-      <c r="I174" s="113"/>
-      <c r="J174" s="113"/>
-      <c r="K174" s="113"/>
-      <c r="L174" s="113"/>
-    </row>
-    <row r="175" spans="1:12">
-      <c r="A175" s="61"/>
-      <c r="B175" s="5"/>
-      <c r="C175" s="112"/>
-      <c r="D175" s="112"/>
-      <c r="E175" s="112"/>
-      <c r="F175" s="113"/>
-      <c r="G175" s="113"/>
-      <c r="H175" s="113"/>
-      <c r="I175" s="113"/>
-      <c r="J175" s="113"/>
-      <c r="K175" s="113"/>
-      <c r="L175" s="113"/>
-    </row>
-    <row r="176" spans="1:12">
-      <c r="A176" s="61"/>
-      <c r="B176" s="5"/>
-      <c r="C176" s="112"/>
-      <c r="D176" s="112"/>
-      <c r="E176" s="112"/>
-      <c r="F176" s="113"/>
-      <c r="G176" s="113"/>
-      <c r="H176" s="113"/>
-      <c r="I176" s="113"/>
-      <c r="J176" s="113"/>
-      <c r="K176" s="113"/>
-      <c r="L176" s="113"/>
-    </row>
-    <row r="177" spans="1:12">
-      <c r="A177" s="61"/>
-      <c r="B177" s="5"/>
-      <c r="C177" s="112"/>
-      <c r="D177" s="112"/>
-      <c r="E177" s="112"/>
-      <c r="F177" s="113"/>
-      <c r="G177" s="113"/>
-      <c r="H177" s="113"/>
-      <c r="I177" s="113"/>
-      <c r="J177" s="113"/>
-      <c r="K177" s="113"/>
-      <c r="L177" s="113"/>
-    </row>
-    <row r="178" spans="1:12">
-      <c r="A178" s="60"/>
-      <c r="B178" s="16"/>
-      <c r="C178" s="112"/>
-      <c r="D178" s="112"/>
-      <c r="E178" s="112"/>
-      <c r="F178" s="113"/>
-      <c r="G178" s="113"/>
-      <c r="H178" s="113"/>
-      <c r="I178" s="113"/>
-      <c r="J178" s="113"/>
-      <c r="K178" s="113"/>
-      <c r="L178" s="113"/>
-    </row>
-    <row r="179" spans="1:12">
-      <c r="A179" s="61"/>
-      <c r="B179" s="5"/>
-      <c r="C179" s="112"/>
-      <c r="D179" s="112"/>
-      <c r="E179" s="112"/>
-      <c r="F179" s="113"/>
-      <c r="G179" s="113"/>
-      <c r="H179" s="113"/>
-      <c r="I179" s="113"/>
-      <c r="J179" s="113"/>
-      <c r="K179" s="113"/>
-      <c r="L179" s="113"/>
-    </row>
-    <row r="180" spans="1:12">
-      <c r="A180" s="61"/>
-      <c r="B180" s="5"/>
-      <c r="C180" s="112"/>
-      <c r="D180" s="112"/>
-      <c r="E180" s="112"/>
-      <c r="F180" s="113"/>
-      <c r="G180" s="113"/>
-      <c r="H180" s="113"/>
-      <c r="I180" s="113"/>
-      <c r="J180" s="113"/>
-      <c r="K180" s="113"/>
-      <c r="L180" s="113"/>
-    </row>
-    <row r="181" spans="1:12">
-      <c r="A181" s="61"/>
-      <c r="B181" s="5"/>
-      <c r="C181" s="112"/>
-      <c r="D181" s="112"/>
-      <c r="E181" s="112"/>
-      <c r="F181" s="113"/>
-      <c r="G181" s="113"/>
-      <c r="H181" s="113"/>
-      <c r="I181" s="113"/>
-      <c r="J181" s="113"/>
-      <c r="K181" s="113"/>
-      <c r="L181" s="113"/>
-    </row>
-    <row r="182" spans="1:12">
-      <c r="A182" s="61"/>
-      <c r="B182" s="5"/>
-      <c r="C182" s="112"/>
-      <c r="D182" s="112"/>
-      <c r="E182" s="112"/>
-      <c r="F182" s="113"/>
-      <c r="G182" s="113"/>
-      <c r="H182" s="113"/>
-      <c r="I182" s="113"/>
-      <c r="J182" s="113"/>
-      <c r="K182" s="113"/>
-      <c r="L182" s="113"/>
-    </row>
-    <row r="183" spans="1:12">
-      <c r="A183" s="61"/>
-      <c r="B183" s="5"/>
-      <c r="C183" s="112"/>
-      <c r="D183" s="112"/>
-      <c r="E183" s="112"/>
-      <c r="F183" s="113"/>
-      <c r="G183" s="113"/>
-      <c r="H183" s="113"/>
-      <c r="I183" s="113"/>
-      <c r="J183" s="113"/>
-      <c r="K183" s="113"/>
-      <c r="L183" s="113"/>
-    </row>
-    <row r="184" spans="1:12">
-      <c r="A184" s="60"/>
-      <c r="B184" s="16"/>
-      <c r="C184" s="112"/>
-      <c r="D184" s="112"/>
-      <c r="E184" s="112"/>
-      <c r="F184" s="113"/>
-      <c r="G184" s="113"/>
-      <c r="H184" s="113"/>
-      <c r="I184" s="113"/>
-      <c r="J184" s="113"/>
-      <c r="K184" s="113"/>
-      <c r="L184" s="113"/>
-    </row>
-    <row r="185" spans="1:12">
-      <c r="A185" s="61"/>
-      <c r="B185" s="5"/>
-      <c r="C185" s="112"/>
-      <c r="D185" s="112"/>
-      <c r="E185" s="112"/>
-      <c r="F185" s="113"/>
-      <c r="G185" s="113"/>
-      <c r="H185" s="113"/>
-      <c r="I185" s="113"/>
-      <c r="J185" s="113"/>
-      <c r="K185" s="113"/>
-      <c r="L185" s="113"/>
-    </row>
-    <row r="186" spans="1:12">
-      <c r="A186" s="61"/>
-      <c r="B186" s="5"/>
-      <c r="C186" s="112"/>
-      <c r="D186" s="112"/>
-      <c r="E186" s="112"/>
-      <c r="F186" s="113"/>
-      <c r="G186" s="113"/>
-      <c r="H186" s="113"/>
-      <c r="I186" s="113"/>
-      <c r="J186" s="113"/>
-      <c r="K186" s="113"/>
-      <c r="L186" s="113"/>
-    </row>
-    <row r="187" spans="1:12">
-      <c r="A187" s="61"/>
-      <c r="B187" s="5"/>
-      <c r="C187" s="112"/>
-      <c r="D187" s="112"/>
-      <c r="E187" s="112"/>
-      <c r="F187" s="113"/>
-      <c r="G187" s="113"/>
-      <c r="H187" s="113"/>
-      <c r="I187" s="113"/>
-      <c r="J187" s="113"/>
-      <c r="K187" s="113"/>
-      <c r="L187" s="113"/>
-    </row>
-    <row r="188" spans="1:12">
-      <c r="A188" s="61"/>
-      <c r="B188" s="5"/>
-      <c r="C188" s="112"/>
-      <c r="D188" s="112"/>
-      <c r="E188" s="112"/>
-      <c r="F188" s="113"/>
-      <c r="G188" s="113"/>
-      <c r="H188" s="113"/>
-      <c r="I188" s="113"/>
-      <c r="J188" s="113"/>
-      <c r="K188" s="113"/>
-      <c r="L188" s="113"/>
-    </row>
-    <row r="189" spans="1:12">
-      <c r="A189" s="61"/>
-      <c r="B189" s="5"/>
-      <c r="C189" s="112"/>
-      <c r="D189" s="112"/>
-      <c r="E189" s="112"/>
-      <c r="F189" s="113"/>
-      <c r="G189" s="113"/>
-      <c r="H189" s="113"/>
-      <c r="I189" s="113"/>
-      <c r="J189" s="113"/>
-      <c r="K189" s="113"/>
-      <c r="L189" s="113"/>
-    </row>
-    <row r="190" spans="1:12">
-      <c r="A190" s="60"/>
-      <c r="B190" s="16"/>
-      <c r="C190" s="112"/>
-      <c r="D190" s="112"/>
-      <c r="E190" s="112"/>
-      <c r="F190" s="113"/>
-      <c r="G190" s="113"/>
-      <c r="H190" s="113"/>
-      <c r="I190" s="113"/>
-      <c r="J190" s="113"/>
-      <c r="K190" s="113"/>
-      <c r="L190" s="113"/>
-    </row>
-    <row r="191" spans="1:12">
-      <c r="A191" s="61"/>
-      <c r="B191" s="5"/>
-      <c r="C191" s="112"/>
-      <c r="D191" s="112"/>
-      <c r="E191" s="112"/>
-      <c r="F191" s="113"/>
-      <c r="G191" s="113"/>
-      <c r="H191" s="113"/>
-      <c r="I191" s="113"/>
-      <c r="J191" s="113"/>
-      <c r="K191" s="113"/>
-      <c r="L191" s="113"/>
-    </row>
-    <row r="192" spans="1:12">
-      <c r="A192" s="61"/>
-      <c r="B192" s="5"/>
-      <c r="C192" s="112"/>
-      <c r="D192" s="112"/>
-      <c r="E192" s="112"/>
-      <c r="F192" s="113"/>
-      <c r="G192" s="113"/>
-      <c r="H192" s="113"/>
-      <c r="I192" s="113"/>
-      <c r="J192" s="113"/>
-      <c r="K192" s="113"/>
-      <c r="L192" s="113"/>
-    </row>
-    <row r="193" spans="1:12">
-      <c r="A193" s="61"/>
-      <c r="B193" s="5"/>
-      <c r="C193" s="112"/>
-      <c r="D193" s="112"/>
-      <c r="E193" s="112"/>
-      <c r="F193" s="113"/>
-      <c r="G193" s="113"/>
-      <c r="H193" s="113"/>
-      <c r="I193" s="113"/>
-      <c r="J193" s="113"/>
-      <c r="K193" s="113"/>
-      <c r="L193" s="113"/>
-    </row>
-    <row r="194" spans="1:12">
-      <c r="A194" s="61"/>
-      <c r="B194" s="5"/>
-      <c r="C194" s="112"/>
-      <c r="D194" s="112"/>
-      <c r="E194" s="112"/>
-      <c r="F194" s="113"/>
-      <c r="G194" s="113"/>
-      <c r="H194" s="113"/>
-      <c r="I194" s="113"/>
-      <c r="J194" s="113"/>
-      <c r="K194" s="113"/>
-      <c r="L194" s="113"/>
-    </row>
-    <row r="195" spans="1:12">
-      <c r="A195" s="61"/>
-      <c r="B195" s="5"/>
-      <c r="C195" s="112"/>
-      <c r="D195" s="112"/>
-      <c r="E195" s="112"/>
-      <c r="F195" s="113"/>
-      <c r="G195" s="113"/>
-      <c r="H195" s="113"/>
-      <c r="I195" s="113"/>
-      <c r="J195" s="113"/>
-      <c r="K195" s="113"/>
-      <c r="L195" s="113"/>
-    </row>
-    <row r="196" spans="1:12">
-      <c r="A196" s="60"/>
-      <c r="B196" s="16"/>
-      <c r="C196" s="112"/>
-      <c r="D196" s="112"/>
-      <c r="E196" s="112"/>
-      <c r="F196" s="113"/>
-      <c r="G196" s="113"/>
-      <c r="H196" s="113"/>
-      <c r="I196" s="113"/>
-      <c r="J196" s="113"/>
-      <c r="K196" s="113"/>
-      <c r="L196" s="113"/>
-    </row>
-    <row r="197" spans="1:12">
-      <c r="A197" s="61"/>
-      <c r="B197" s="5"/>
-      <c r="C197" s="112"/>
-      <c r="D197" s="112"/>
-      <c r="E197" s="112"/>
-      <c r="F197" s="113"/>
-      <c r="G197" s="113"/>
-      <c r="H197" s="113"/>
-      <c r="I197" s="113"/>
-      <c r="J197" s="113"/>
-      <c r="K197" s="113"/>
-      <c r="L197" s="113"/>
-    </row>
-    <row r="198" spans="1:12">
-      <c r="A198" s="61"/>
-      <c r="B198" s="5"/>
-      <c r="C198" s="112"/>
-      <c r="D198" s="112"/>
-      <c r="E198" s="112"/>
-      <c r="F198" s="113"/>
-      <c r="G198" s="113"/>
-      <c r="H198" s="113"/>
-      <c r="I198" s="113"/>
-      <c r="J198" s="113"/>
-      <c r="K198" s="113"/>
-      <c r="L198" s="113"/>
-    </row>
-    <row r="199" spans="1:12">
-      <c r="A199" s="61"/>
-      <c r="B199" s="5"/>
-      <c r="C199" s="112"/>
-      <c r="D199" s="112"/>
-      <c r="E199" s="112"/>
-      <c r="F199" s="113"/>
-      <c r="G199" s="113"/>
-      <c r="H199" s="113"/>
-      <c r="I199" s="113"/>
-      <c r="J199" s="113"/>
-      <c r="K199" s="113"/>
-      <c r="L199" s="113"/>
-    </row>
-    <row r="200" spans="1:12">
-      <c r="A200" s="61"/>
-      <c r="B200" s="5"/>
-      <c r="C200" s="112"/>
-      <c r="D200" s="112"/>
-      <c r="E200" s="112"/>
-      <c r="F200" s="113"/>
-      <c r="G200" s="113"/>
-      <c r="H200" s="113"/>
-      <c r="I200" s="113"/>
-      <c r="J200" s="113"/>
-      <c r="K200" s="113"/>
-      <c r="L200" s="113"/>
-    </row>
-    <row r="201" spans="1:12">
-      <c r="A201" s="61"/>
-      <c r="B201" s="5"/>
-      <c r="C201" s="112"/>
-      <c r="D201" s="112"/>
-      <c r="E201" s="112"/>
-      <c r="F201" s="113"/>
-      <c r="G201" s="113"/>
-      <c r="H201" s="113"/>
-      <c r="I201" s="113"/>
-      <c r="J201" s="113"/>
-      <c r="K201" s="113"/>
-      <c r="L201" s="113"/>
-    </row>
-    <row r="202" spans="1:12">
-      <c r="A202" s="60"/>
-      <c r="B202" s="16"/>
-      <c r="C202" s="112"/>
-      <c r="D202" s="112"/>
-      <c r="E202" s="112"/>
-      <c r="F202" s="113"/>
-      <c r="G202" s="113"/>
-      <c r="H202" s="113"/>
-      <c r="I202" s="113"/>
-      <c r="J202" s="113"/>
-      <c r="K202" s="113"/>
-      <c r="L202" s="113"/>
-    </row>
-    <row r="203" spans="1:12">
-      <c r="A203" s="61"/>
-      <c r="B203" s="5"/>
-      <c r="C203" s="112"/>
-      <c r="D203" s="112"/>
-      <c r="E203" s="112"/>
-      <c r="F203" s="113"/>
-      <c r="G203" s="113"/>
-      <c r="H203" s="113"/>
-      <c r="I203" s="113"/>
-      <c r="J203" s="113"/>
-      <c r="K203" s="113"/>
-      <c r="L203" s="113"/>
-    </row>
-    <row r="204" spans="1:12">
-      <c r="A204" s="61"/>
-      <c r="B204" s="5"/>
-      <c r="C204" s="112"/>
-      <c r="D204" s="112"/>
-      <c r="E204" s="112"/>
-      <c r="F204" s="113"/>
-      <c r="G204" s="113"/>
-      <c r="H204" s="113"/>
-      <c r="I204" s="113"/>
-      <c r="J204" s="113"/>
-      <c r="K204" s="113"/>
-      <c r="L204" s="113"/>
-    </row>
-    <row r="205" spans="1:12">
-      <c r="A205" s="61"/>
-      <c r="B205" s="5"/>
-      <c r="C205" s="61"/>
-      <c r="D205" s="61"/>
-      <c r="E205" s="61"/>
-    </row>
-    <row r="206" spans="1:12">
-      <c r="A206" s="61"/>
-      <c r="B206" s="5"/>
-      <c r="C206" s="61"/>
-      <c r="D206" s="61"/>
-      <c r="E206" s="61"/>
-    </row>
-    <row r="207" spans="1:12">
-      <c r="A207" s="61"/>
-      <c r="B207" s="5"/>
-      <c r="C207" s="17"/>
-      <c r="D207" s="17"/>
-      <c r="E207" s="17"/>
-    </row>
-    <row r="208" spans="1:12">
-      <c r="A208" s="60"/>
-      <c r="B208" s="16"/>
-      <c r="C208" s="17"/>
-      <c r="D208" s="17"/>
-      <c r="E208" s="17"/>
-    </row>
-    <row r="209" spans="1:5">
-      <c r="A209" s="61"/>
-      <c r="B209" s="5"/>
-      <c r="C209" s="61"/>
-      <c r="D209" s="61"/>
-      <c r="E209" s="61"/>
-    </row>
-    <row r="210" spans="1:5">
-      <c r="A210" s="61"/>
-      <c r="B210" s="5"/>
-      <c r="C210" s="17"/>
-      <c r="D210" s="17"/>
-      <c r="E210" s="17"/>
-    </row>
-    <row r="211" spans="1:5">
-      <c r="A211" s="61"/>
-      <c r="B211" s="5"/>
-      <c r="C211" s="61"/>
-      <c r="D211" s="61"/>
-      <c r="E211" s="61"/>
-    </row>
-    <row r="212" spans="1:5">
-      <c r="A212" s="61"/>
-      <c r="B212" s="5"/>
-      <c r="C212" s="61"/>
-      <c r="D212" s="61"/>
-      <c r="E212" s="61"/>
-    </row>
-    <row r="213" spans="1:5">
-      <c r="A213" s="61"/>
-      <c r="B213" s="5"/>
-      <c r="C213" s="17"/>
-      <c r="D213" s="17"/>
-      <c r="E213" s="17"/>
-    </row>
-    <row r="214" spans="1:5">
-      <c r="A214" s="60"/>
-      <c r="B214" s="16"/>
-      <c r="C214" s="17"/>
-      <c r="D214" s="17"/>
-      <c r="E214" s="17"/>
-    </row>
-    <row r="215" spans="1:5">
-      <c r="A215" s="61"/>
-      <c r="B215" s="5"/>
-      <c r="C215" s="61"/>
-      <c r="D215" s="61"/>
-      <c r="E215" s="61"/>
-    </row>
-    <row r="216" spans="1:5">
-      <c r="A216" s="61"/>
-      <c r="B216" s="5"/>
-      <c r="C216" s="17"/>
-      <c r="D216" s="17"/>
-      <c r="E216" s="17"/>
-    </row>
-    <row r="217" spans="1:5">
-      <c r="A217" s="61"/>
-      <c r="B217" s="5"/>
-      <c r="C217" s="61"/>
-      <c r="D217" s="61"/>
-      <c r="E217" s="61"/>
-    </row>
-    <row r="218" spans="1:5">
-      <c r="A218" s="61"/>
-      <c r="B218" s="5"/>
-      <c r="C218" s="61"/>
-      <c r="D218" s="61"/>
-      <c r="E218" s="61"/>
-    </row>
-    <row r="219" spans="1:5">
-      <c r="A219" s="61"/>
-      <c r="B219" s="5"/>
-      <c r="C219" s="17"/>
-      <c r="D219" s="17"/>
-      <c r="E219" s="17"/>
-    </row>
-    <row r="220" spans="1:5">
-      <c r="A220" s="60"/>
-      <c r="B220" s="16"/>
-      <c r="C220" s="17"/>
-      <c r="D220" s="17"/>
-      <c r="E220" s="17"/>
-    </row>
-    <row r="221" spans="1:5">
-      <c r="A221" s="61"/>
-      <c r="B221" s="5"/>
-      <c r="C221" s="61"/>
-      <c r="D221" s="61"/>
-      <c r="E221" s="61"/>
-    </row>
-    <row r="222" spans="1:5">
-      <c r="A222" s="61"/>
-      <c r="B222" s="5"/>
-      <c r="C222" s="17"/>
-      <c r="D222" s="17"/>
-      <c r="E222" s="17"/>
-    </row>
-    <row r="223" spans="1:5">
-      <c r="A223" s="61"/>
-      <c r="B223" s="5"/>
-      <c r="C223" s="61"/>
-      <c r="D223" s="61"/>
-      <c r="E223" s="61"/>
-    </row>
-    <row r="224" spans="1:5">
-      <c r="A224" s="61"/>
-      <c r="B224" s="5"/>
-      <c r="C224" s="61"/>
-      <c r="D224" s="61"/>
-      <c r="E224" s="61"/>
-    </row>
-    <row r="225" spans="1:5">
-      <c r="A225" s="61"/>
-      <c r="B225" s="5"/>
-      <c r="C225" s="17"/>
-      <c r="D225" s="17"/>
-      <c r="E225" s="17"/>
-    </row>
-    <row r="226" spans="1:5">
-      <c r="A226" s="60"/>
-      <c r="B226" s="16"/>
-      <c r="C226" s="17"/>
-      <c r="D226" s="17"/>
-      <c r="E226" s="17"/>
-    </row>
-    <row r="227" spans="1:5">
-      <c r="A227" s="61"/>
-      <c r="B227" s="5"/>
-      <c r="C227" s="61"/>
-      <c r="D227" s="61"/>
-      <c r="E227" s="61"/>
-    </row>
-    <row r="228" spans="1:5">
-      <c r="A228" s="61"/>
-      <c r="B228" s="5"/>
-      <c r="C228" s="17"/>
-      <c r="D228" s="17"/>
-      <c r="E228" s="17"/>
-    </row>
-    <row r="229" spans="1:5">
-      <c r="A229" s="61"/>
-      <c r="B229" s="5"/>
-      <c r="C229" s="61"/>
-      <c r="D229" s="61"/>
-      <c r="E229" s="61"/>
-    </row>
-    <row r="230" spans="1:5">
-      <c r="A230" s="61"/>
-      <c r="B230" s="5"/>
-      <c r="C230" s="61"/>
-      <c r="D230" s="61"/>
-      <c r="E230" s="61"/>
-    </row>
-    <row r="231" spans="1:5">
-      <c r="A231" s="61"/>
-      <c r="B231" s="5"/>
-      <c r="C231" s="17"/>
-      <c r="D231" s="17"/>
-      <c r="E231" s="17"/>
-    </row>
-    <row r="232" spans="1:5">
-      <c r="A232" s="60"/>
-      <c r="B232" s="16"/>
-      <c r="C232" s="17"/>
-      <c r="D232" s="17"/>
-      <c r="E232" s="17"/>
-    </row>
-    <row r="233" spans="1:5">
-      <c r="A233" s="61"/>
-      <c r="B233" s="5"/>
-      <c r="C233" s="61"/>
-      <c r="D233" s="61"/>
-      <c r="E233" s="61"/>
-    </row>
-    <row r="234" spans="1:5">
-      <c r="A234" s="61"/>
-      <c r="B234" s="5"/>
-      <c r="C234" s="17"/>
-      <c r="D234" s="17"/>
-      <c r="E234" s="17"/>
-    </row>
-    <row r="235" spans="1:5">
-      <c r="A235" s="61"/>
-      <c r="B235" s="5"/>
-      <c r="C235" s="61"/>
-      <c r="D235" s="61"/>
-      <c r="E235" s="61"/>
-    </row>
-    <row r="236" spans="1:5">
-      <c r="A236" s="61"/>
-      <c r="B236" s="5"/>
-      <c r="C236" s="61"/>
-      <c r="D236" s="61"/>
-      <c r="E236" s="61"/>
-    </row>
-    <row r="237" spans="1:5">
-      <c r="A237" s="61"/>
-      <c r="B237" s="5"/>
-      <c r="C237" s="17"/>
-      <c r="D237" s="17"/>
-      <c r="E237" s="17"/>
-    </row>
-    <row r="238" spans="1:5">
-      <c r="A238" s="60"/>
-      <c r="B238" s="16"/>
-      <c r="C238" s="17"/>
-      <c r="D238" s="17"/>
-      <c r="E238" s="17"/>
-    </row>
-    <row r="239" spans="1:5">
-      <c r="A239" s="61"/>
-      <c r="B239" s="5"/>
-      <c r="C239" s="61"/>
-      <c r="D239" s="61"/>
-      <c r="E239" s="61"/>
-    </row>
-    <row r="240" spans="1:5">
-      <c r="A240" s="61"/>
-      <c r="B240" s="5"/>
-      <c r="C240" s="17"/>
-      <c r="D240" s="17"/>
-      <c r="E240" s="17"/>
-    </row>
-    <row r="241" spans="1:5">
-      <c r="A241" s="61"/>
-      <c r="B241" s="5"/>
-      <c r="C241" s="61"/>
-      <c r="D241" s="61"/>
-      <c r="E241" s="61"/>
-    </row>
-    <row r="242" spans="1:5">
-      <c r="A242" s="61"/>
-      <c r="B242" s="5"/>
-      <c r="C242" s="61"/>
-      <c r="D242" s="61"/>
-      <c r="E242" s="61"/>
-    </row>
-    <row r="243" spans="1:5">
-      <c r="A243" s="61"/>
-      <c r="B243" s="5"/>
-      <c r="C243" s="17"/>
-      <c r="D243" s="17"/>
-      <c r="E243" s="17"/>
-    </row>
-    <row r="244" spans="1:5">
-      <c r="A244" s="60"/>
-      <c r="B244" s="16"/>
-      <c r="C244" s="17"/>
-      <c r="D244" s="17"/>
-      <c r="E244" s="17"/>
-    </row>
-    <row r="245" spans="1:5">
-      <c r="A245" s="61"/>
-      <c r="B245" s="5"/>
-      <c r="C245" s="61"/>
-      <c r="D245" s="61"/>
-      <c r="E245" s="61"/>
-    </row>
-    <row r="246" spans="1:5">
-      <c r="A246" s="61"/>
-      <c r="B246" s="5"/>
-      <c r="C246" s="17"/>
-      <c r="D246" s="17"/>
-      <c r="E246" s="17"/>
-    </row>
-    <row r="247" spans="1:5">
-      <c r="A247" s="61"/>
-      <c r="B247" s="5"/>
-      <c r="C247" s="61"/>
-      <c r="D247" s="61"/>
-      <c r="E247" s="61"/>
-    </row>
-    <row r="248" spans="1:5">
-      <c r="A248" s="61"/>
-      <c r="B248" s="5"/>
-      <c r="C248" s="61"/>
-      <c r="D248" s="61"/>
-      <c r="E248" s="61"/>
-    </row>
-    <row r="249" spans="1:5">
-      <c r="A249" s="61"/>
-      <c r="B249" s="5"/>
-      <c r="C249" s="17"/>
-      <c r="D249" s="17"/>
-      <c r="E249" s="17"/>
-    </row>
-    <row r="250" spans="1:5">
-      <c r="A250" s="60"/>
-      <c r="B250" s="16"/>
-      <c r="C250" s="17"/>
-      <c r="D250" s="17"/>
-      <c r="E250" s="17"/>
-    </row>
-    <row r="251" spans="1:5">
-      <c r="A251" s="61"/>
-      <c r="B251" s="5"/>
-      <c r="C251" s="61"/>
-      <c r="D251" s="61"/>
-      <c r="E251" s="61"/>
-    </row>
-    <row r="252" spans="1:5">
-      <c r="A252" s="61"/>
-      <c r="B252" s="5"/>
-      <c r="C252" s="17"/>
-      <c r="D252" s="17"/>
-      <c r="E252" s="17"/>
-    </row>
-    <row r="253" spans="1:5">
-      <c r="A253" s="61"/>
-      <c r="B253" s="5"/>
-      <c r="C253" s="61"/>
-      <c r="D253" s="61"/>
-      <c r="E253" s="61"/>
-    </row>
-    <row r="254" spans="1:5">
-      <c r="A254" s="61"/>
-      <c r="B254" s="5"/>
-      <c r="C254" s="61"/>
-      <c r="D254" s="61"/>
-      <c r="E254" s="61"/>
-    </row>
-    <row r="255" spans="1:5">
-      <c r="A255" s="61"/>
-      <c r="B255" s="5"/>
-      <c r="C255" s="17"/>
-      <c r="D255" s="17"/>
-      <c r="E255" s="17"/>
-    </row>
-    <row r="256" spans="1:5">
-      <c r="A256" s="60"/>
-      <c r="B256" s="16"/>
-      <c r="C256" s="17"/>
-      <c r="D256" s="17"/>
-      <c r="E256" s="17"/>
-    </row>
-    <row r="257" spans="1:5">
-      <c r="A257" s="61"/>
-      <c r="B257" s="5"/>
-      <c r="C257" s="61"/>
-      <c r="D257" s="61"/>
-      <c r="E257" s="61"/>
-    </row>
-    <row r="258" spans="1:5">
-      <c r="A258" s="61"/>
-      <c r="B258" s="5"/>
-      <c r="C258" s="17"/>
-      <c r="D258" s="17"/>
-      <c r="E258" s="17"/>
-    </row>
-    <row r="259" spans="1:5">
-      <c r="A259" s="61"/>
-      <c r="B259" s="5"/>
-      <c r="C259" s="61"/>
-      <c r="D259" s="61"/>
-      <c r="E259" s="61"/>
-    </row>
-    <row r="260" spans="1:5">
-      <c r="A260" s="61"/>
-      <c r="B260" s="5"/>
-      <c r="C260" s="61"/>
-      <c r="D260" s="61"/>
-      <c r="E260" s="61"/>
-    </row>
-    <row r="261" spans="1:5">
-      <c r="A261" s="61"/>
-      <c r="B261" s="5"/>
-      <c r="C261" s="17"/>
-      <c r="D261" s="17"/>
-      <c r="E261" s="17"/>
-    </row>
-    <row r="262" spans="1:5">
-      <c r="A262" s="60"/>
-      <c r="B262" s="16"/>
-      <c r="C262" s="17"/>
-      <c r="D262" s="17"/>
-      <c r="E262" s="17"/>
-    </row>
-    <row r="263" spans="1:5">
-      <c r="A263" s="61"/>
-      <c r="B263" s="26"/>
-      <c r="C263" s="61"/>
-      <c r="D263" s="61"/>
-      <c r="E263" s="61"/>
-    </row>
-    <row r="264" spans="1:5">
-      <c r="A264" s="61"/>
-      <c r="B264" s="61"/>
-      <c r="C264" s="61"/>
-      <c r="D264" s="61"/>
-      <c r="E264" s="61"/>
-    </row>
-    <row r="265" spans="1:5">
-      <c r="A265" s="61"/>
-      <c r="B265" s="61"/>
-      <c r="C265" s="61"/>
-      <c r="D265" s="61"/>
-      <c r="E265" s="61"/>
-    </row>
-    <row r="266" spans="1:5">
-      <c r="A266" s="61"/>
-      <c r="B266" s="61"/>
-      <c r="C266" s="61"/>
-      <c r="D266" s="61"/>
-      <c r="E266" s="61"/>
-    </row>
-    <row r="267" spans="1:5">
-      <c r="A267" s="61"/>
-      <c r="B267" s="61"/>
-      <c r="C267" s="61"/>
-      <c r="D267" s="61"/>
-      <c r="E267" s="61"/>
-    </row>
-    <row r="268" spans="1:5">
-      <c r="A268" s="61"/>
-      <c r="B268" s="61"/>
-      <c r="C268" s="61"/>
-      <c r="D268" s="61"/>
-      <c r="E268" s="61"/>
-    </row>
-    <row r="269" spans="1:5">
-      <c r="A269" s="61"/>
-      <c r="B269" s="61"/>
-      <c r="C269" s="61"/>
-      <c r="D269" s="61"/>
-      <c r="E269" s="61"/>
     </row>
   </sheetData>
   <mergeCells count="91">
@@ -11293,11 +8877,6 @@
     <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="45.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" style="1"/>
-    <col min="7" max="7" width="47.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="34.42578125" style="1" customWidth="1"/>
-    <col min="9" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -11834,11 +9413,6 @@
     <col min="1" max="1" width="9.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="42.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="87.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="28.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" style="1"/>
-    <col min="6" max="6" width="47.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="34.42578125" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -12145,216 +9719,6 @@
         <v>471</v>
       </c>
       <c r="C41" s="45"/>
-    </row>
-    <row r="42" spans="1:3">
-      <c r="A42" s="15"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="24"/>
-    </row>
-    <row r="43" spans="1:3">
-      <c r="A43" s="23"/>
-      <c r="B43" s="5"/>
-      <c r="C43" s="24"/>
-    </row>
-    <row r="44" spans="1:3">
-      <c r="A44" s="23"/>
-      <c r="B44" s="5"/>
-      <c r="C44" s="24"/>
-    </row>
-    <row r="45" spans="1:3">
-      <c r="A45" s="23"/>
-      <c r="B45" s="5"/>
-      <c r="C45" s="24"/>
-    </row>
-    <row r="46" spans="1:3">
-      <c r="A46" s="23"/>
-      <c r="B46" s="5"/>
-      <c r="C46" s="24"/>
-    </row>
-    <row r="47" spans="1:3">
-      <c r="A47" s="23"/>
-      <c r="B47" s="5"/>
-      <c r="C47" s="24"/>
-    </row>
-    <row r="48" spans="1:3">
-      <c r="A48" s="15"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="24"/>
-    </row>
-    <row r="49" spans="1:3">
-      <c r="A49" s="23"/>
-      <c r="B49" s="5"/>
-      <c r="C49" s="24"/>
-    </row>
-    <row r="50" spans="1:3">
-      <c r="A50" s="23"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="24"/>
-    </row>
-    <row r="51" spans="1:3">
-      <c r="A51" s="23"/>
-      <c r="B51" s="5"/>
-      <c r="C51" s="24"/>
-    </row>
-    <row r="52" spans="1:3">
-      <c r="A52" s="15"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="56"/>
-    </row>
-    <row r="53" spans="1:3">
-      <c r="A53" s="23"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="24"/>
-    </row>
-    <row r="54" spans="1:3">
-      <c r="A54" s="15"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="24"/>
-    </row>
-    <row r="55" spans="1:3">
-      <c r="A55" s="23"/>
-      <c r="B55" s="5"/>
-      <c r="C55" s="24"/>
-    </row>
-    <row r="56" spans="1:3">
-      <c r="A56" s="23"/>
-      <c r="B56" s="5"/>
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:3">
-      <c r="A57" s="23"/>
-      <c r="B57" s="5"/>
-      <c r="C57" s="24"/>
-    </row>
-    <row r="58" spans="1:3">
-      <c r="A58" s="23"/>
-      <c r="B58" s="5"/>
-      <c r="C58" s="24"/>
-    </row>
-    <row r="59" spans="1:3">
-      <c r="A59" s="23"/>
-      <c r="B59" s="5"/>
-      <c r="C59" s="24"/>
-    </row>
-    <row r="60" spans="1:3">
-      <c r="A60" s="15"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="57"/>
-    </row>
-    <row r="61" spans="1:3">
-      <c r="A61" s="23"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="24"/>
-    </row>
-    <row r="62" spans="1:3">
-      <c r="A62" s="23"/>
-      <c r="B62" s="5"/>
-      <c r="C62" s="24"/>
-    </row>
-    <row r="63" spans="1:3">
-      <c r="A63" s="23"/>
-      <c r="B63" s="5"/>
-      <c r="C63" s="24"/>
-    </row>
-    <row r="64" spans="1:3">
-      <c r="A64" s="15"/>
-      <c r="B64" s="5"/>
-      <c r="C64" s="24"/>
-    </row>
-    <row r="65" spans="1:3">
-      <c r="A65" s="23"/>
-      <c r="B65" s="5"/>
-      <c r="C65" s="24"/>
-    </row>
-    <row r="66" spans="1:3">
-      <c r="A66" s="15"/>
-      <c r="B66" s="5"/>
-      <c r="C66" s="24"/>
-    </row>
-    <row r="67" spans="1:3">
-      <c r="A67" s="23"/>
-      <c r="B67" s="5"/>
-      <c r="C67" s="24"/>
-    </row>
-    <row r="68" spans="1:3">
-      <c r="A68" s="23"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="24"/>
-    </row>
-    <row r="69" spans="1:3">
-      <c r="A69" s="23"/>
-      <c r="B69" s="58"/>
-      <c r="C69" s="24"/>
-    </row>
-    <row r="70" spans="1:3">
-      <c r="A70" s="23"/>
-      <c r="B70" s="5"/>
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="1:3">
-      <c r="A71" s="15"/>
-      <c r="B71" s="58"/>
-      <c r="C71" s="24"/>
-    </row>
-    <row r="72" spans="1:3">
-      <c r="A72" s="15"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="24"/>
-    </row>
-    <row r="73" spans="1:3">
-      <c r="A73" s="23"/>
-      <c r="B73" s="5"/>
-      <c r="C73" s="24"/>
-    </row>
-    <row r="74" spans="1:3">
-      <c r="A74" s="23"/>
-      <c r="B74" s="5"/>
-      <c r="C74" s="24"/>
-    </row>
-    <row r="75" spans="1:3">
-      <c r="A75" s="23"/>
-      <c r="B75" s="5"/>
-      <c r="C75" s="24"/>
-    </row>
-    <row r="76" spans="1:3">
-      <c r="A76" s="23"/>
-      <c r="B76" s="5"/>
-      <c r="C76" s="24"/>
-    </row>
-    <row r="77" spans="1:3">
-      <c r="A77" s="23"/>
-      <c r="B77" s="2"/>
-      <c r="C77" s="24"/>
-    </row>
-    <row r="78" spans="1:3">
-      <c r="A78" s="15"/>
-      <c r="B78" s="2"/>
-      <c r="C78" s="24"/>
-    </row>
-    <row r="79" spans="1:3">
-      <c r="A79" s="23"/>
-      <c r="B79" s="2"/>
-      <c r="C79" s="24"/>
-    </row>
-    <row r="80" spans="1:3">
-      <c r="A80" s="23"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="24"/>
-    </row>
-    <row r="81" spans="1:3">
-      <c r="A81" s="23"/>
-      <c r="B81" s="2"/>
-      <c r="C81" s="24"/>
-    </row>
-    <row r="82" spans="1:3">
-      <c r="A82" s="23"/>
-      <c r="B82" s="2"/>
-      <c r="C82" s="24"/>
-    </row>
-    <row r="83" spans="1:3">
-      <c r="A83" s="23"/>
-      <c r="B83" s="2"/>
-      <c r="C83" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
:bug: excel export could not be open without error
</commit_message>
<xml_diff>
--- a/resources/excel/specification_configurator_template.xlsx
+++ b/resources/excel/specification_configurator_template.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -22,13 +22,6 @@
     <sheet name="7. Projekt" sheetId="25" r:id="rId7"/>
     <sheet name="8. Angaben Softwareanbieter" sheetId="26" r:id="rId8"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId9"/>
-  </externalReferences>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'6. Anforderungen'!$A$1:$M$15</definedName>
-    <definedName name="Bewertung">[1]Listen!$B$4:$B$9</definedName>
-  </definedNames>
   <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -2463,25 +2456,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Übersicht"/>
-      <sheetName val="Lastenheft"/>
-      <sheetName val="Legende"/>
-      <sheetName val="Listen"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>

</xml_diff>